<commit_message>
KIBON-1432 Rundungsfehler in Tagesschule Anmeldungen Statistik. Nur gültige Anmeldungen zeigen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD6049F-FAEC-4C73-BED7-F2588AAB2305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F125E957-16FF-4CCE-968D-EAC52BDBB1DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,10 +463,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0\ &quot;h&quot;"/>
     <numFmt numFmtId="166" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.0\ &quot;h&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -728,18 +729,12 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -748,9 +743,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -767,37 +759,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -810,7 +774,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1225,7 +1226,9 @@
   </sheetPr>
   <dimension ref="A1:DP39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1733,158 +1736,158 @@
       <c r="DN6" s="13"/>
     </row>
     <row r="7" spans="1:120" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="52" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="16"/>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="45"/>
-      <c r="AC7" s="46"/>
-      <c r="AD7" s="44" t="s">
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+      <c r="X7" s="47"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
+      <c r="AA7" s="47"/>
+      <c r="AB7" s="47"/>
+      <c r="AC7" s="48"/>
+      <c r="AD7" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="AE7" s="45"/>
-      <c r="AF7" s="45"/>
-      <c r="AG7" s="45"/>
-      <c r="AH7" s="45"/>
-      <c r="AI7" s="45"/>
-      <c r="AJ7" s="45"/>
-      <c r="AK7" s="45"/>
-      <c r="AL7" s="45"/>
-      <c r="AM7" s="45"/>
-      <c r="AN7" s="45"/>
-      <c r="AO7" s="45"/>
-      <c r="AP7" s="45"/>
-      <c r="AQ7" s="45"/>
-      <c r="AR7" s="45"/>
-      <c r="AS7" s="45"/>
-      <c r="AT7" s="45"/>
-      <c r="AU7" s="45"/>
-      <c r="AV7" s="45"/>
-      <c r="AW7" s="45"/>
-      <c r="AX7" s="45"/>
-      <c r="AY7" s="46"/>
-      <c r="AZ7" s="44" t="s">
+      <c r="AE7" s="47"/>
+      <c r="AF7" s="47"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="47"/>
+      <c r="AI7" s="47"/>
+      <c r="AJ7" s="47"/>
+      <c r="AK7" s="47"/>
+      <c r="AL7" s="47"/>
+      <c r="AM7" s="47"/>
+      <c r="AN7" s="47"/>
+      <c r="AO7" s="47"/>
+      <c r="AP7" s="47"/>
+      <c r="AQ7" s="47"/>
+      <c r="AR7" s="47"/>
+      <c r="AS7" s="47"/>
+      <c r="AT7" s="47"/>
+      <c r="AU7" s="47"/>
+      <c r="AV7" s="47"/>
+      <c r="AW7" s="47"/>
+      <c r="AX7" s="47"/>
+      <c r="AY7" s="48"/>
+      <c r="AZ7" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="BA7" s="45"/>
-      <c r="BB7" s="45"/>
-      <c r="BC7" s="45"/>
-      <c r="BD7" s="45"/>
-      <c r="BE7" s="45"/>
-      <c r="BF7" s="45"/>
-      <c r="BG7" s="45"/>
-      <c r="BH7" s="45"/>
-      <c r="BI7" s="45"/>
-      <c r="BJ7" s="45"/>
-      <c r="BK7" s="45"/>
-      <c r="BL7" s="45"/>
-      <c r="BM7" s="45"/>
-      <c r="BN7" s="45"/>
-      <c r="BO7" s="45"/>
-      <c r="BP7" s="45"/>
-      <c r="BQ7" s="45"/>
-      <c r="BR7" s="45"/>
-      <c r="BS7" s="45"/>
-      <c r="BT7" s="45"/>
-      <c r="BU7" s="46"/>
-      <c r="BV7" s="44" t="s">
+      <c r="BA7" s="47"/>
+      <c r="BB7" s="47"/>
+      <c r="BC7" s="47"/>
+      <c r="BD7" s="47"/>
+      <c r="BE7" s="47"/>
+      <c r="BF7" s="47"/>
+      <c r="BG7" s="47"/>
+      <c r="BH7" s="47"/>
+      <c r="BI7" s="47"/>
+      <c r="BJ7" s="47"/>
+      <c r="BK7" s="47"/>
+      <c r="BL7" s="47"/>
+      <c r="BM7" s="47"/>
+      <c r="BN7" s="47"/>
+      <c r="BO7" s="47"/>
+      <c r="BP7" s="47"/>
+      <c r="BQ7" s="47"/>
+      <c r="BR7" s="47"/>
+      <c r="BS7" s="47"/>
+      <c r="BT7" s="47"/>
+      <c r="BU7" s="48"/>
+      <c r="BV7" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="BW7" s="45"/>
-      <c r="BX7" s="45"/>
-      <c r="BY7" s="45"/>
-      <c r="BZ7" s="45"/>
-      <c r="CA7" s="45"/>
-      <c r="CB7" s="45"/>
-      <c r="CC7" s="45"/>
-      <c r="CD7" s="45"/>
-      <c r="CE7" s="45"/>
-      <c r="CF7" s="45"/>
-      <c r="CG7" s="45"/>
-      <c r="CH7" s="45"/>
-      <c r="CI7" s="45"/>
-      <c r="CJ7" s="45"/>
-      <c r="CK7" s="45"/>
-      <c r="CL7" s="45"/>
-      <c r="CM7" s="45"/>
-      <c r="CN7" s="45"/>
-      <c r="CO7" s="45"/>
-      <c r="CP7" s="45"/>
-      <c r="CQ7" s="46"/>
-      <c r="CR7" s="44" t="s">
+      <c r="BW7" s="47"/>
+      <c r="BX7" s="47"/>
+      <c r="BY7" s="47"/>
+      <c r="BZ7" s="47"/>
+      <c r="CA7" s="47"/>
+      <c r="CB7" s="47"/>
+      <c r="CC7" s="47"/>
+      <c r="CD7" s="47"/>
+      <c r="CE7" s="47"/>
+      <c r="CF7" s="47"/>
+      <c r="CG7" s="47"/>
+      <c r="CH7" s="47"/>
+      <c r="CI7" s="47"/>
+      <c r="CJ7" s="47"/>
+      <c r="CK7" s="47"/>
+      <c r="CL7" s="47"/>
+      <c r="CM7" s="47"/>
+      <c r="CN7" s="47"/>
+      <c r="CO7" s="47"/>
+      <c r="CP7" s="47"/>
+      <c r="CQ7" s="48"/>
+      <c r="CR7" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="CS7" s="45"/>
-      <c r="CT7" s="45"/>
-      <c r="CU7" s="45"/>
-      <c r="CV7" s="45"/>
-      <c r="CW7" s="45"/>
-      <c r="CX7" s="45"/>
-      <c r="CY7" s="45"/>
-      <c r="CZ7" s="45"/>
-      <c r="DA7" s="45"/>
-      <c r="DB7" s="45"/>
-      <c r="DC7" s="45"/>
-      <c r="DD7" s="45"/>
-      <c r="DE7" s="45"/>
-      <c r="DF7" s="45"/>
-      <c r="DG7" s="45"/>
-      <c r="DH7" s="45"/>
-      <c r="DI7" s="45"/>
-      <c r="DJ7" s="45"/>
-      <c r="DK7" s="45"/>
-      <c r="DL7" s="45"/>
-      <c r="DM7" s="46"/>
-      <c r="DN7" s="54" t="s">
+      <c r="CS7" s="47"/>
+      <c r="CT7" s="47"/>
+      <c r="CU7" s="47"/>
+      <c r="CV7" s="47"/>
+      <c r="CW7" s="47"/>
+      <c r="CX7" s="47"/>
+      <c r="CY7" s="47"/>
+      <c r="CZ7" s="47"/>
+      <c r="DA7" s="47"/>
+      <c r="DB7" s="47"/>
+      <c r="DC7" s="47"/>
+      <c r="DD7" s="47"/>
+      <c r="DE7" s="47"/>
+      <c r="DF7" s="47"/>
+      <c r="DG7" s="47"/>
+      <c r="DH7" s="47"/>
+      <c r="DI7" s="47"/>
+      <c r="DJ7" s="47"/>
+      <c r="DK7" s="47"/>
+      <c r="DL7" s="47"/>
+      <c r="DM7" s="48"/>
+      <c r="DN7" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="DO7" s="54"/>
+      <c r="DO7" s="39"/>
       <c r="DP7" s="11"/>
     </row>
     <row r="8" spans="1:120" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
       <c r="G8" s="17"/>
       <c r="H8" s="4" t="s">
         <v>6</v>
@@ -1946,10 +1949,10 @@
       <c r="AA8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AB8" s="48" t="s">
+      <c r="AB8" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="AC8" s="48" t="s">
+      <c r="AC8" s="43" t="s">
         <v>51</v>
       </c>
       <c r="AD8" s="4" t="s">
@@ -2012,10 +2015,10 @@
       <c r="AW8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AX8" s="48" t="s">
+      <c r="AX8" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="AY8" s="48" t="s">
+      <c r="AY8" s="43" t="s">
         <v>51</v>
       </c>
       <c r="AZ8" s="4" t="s">
@@ -2078,10 +2081,10 @@
       <c r="BS8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BT8" s="48" t="s">
+      <c r="BT8" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="BU8" s="48" t="s">
+      <c r="BU8" s="43" t="s">
         <v>51</v>
       </c>
       <c r="BV8" s="4" t="s">
@@ -2144,10 +2147,10 @@
       <c r="CO8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CP8" s="48" t="s">
+      <c r="CP8" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="CQ8" s="48" t="s">
+      <c r="CQ8" s="43" t="s">
         <v>51</v>
       </c>
       <c r="CR8" s="4" t="s">
@@ -2210,16 +2213,16 @@
       <c r="DK8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DL8" s="48" t="s">
+      <c r="DL8" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="DM8" s="48" t="s">
+      <c r="DM8" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="DN8" s="55" t="s">
+      <c r="DN8" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="DO8" s="55" t="s">
+      <c r="DO8" s="40" t="s">
         <v>58</v>
       </c>
       <c r="DP8" s="11"/>
@@ -2292,8 +2295,8 @@
       <c r="AA9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AB9" s="49"/>
-      <c r="AC9" s="49"/>
+      <c r="AB9" s="44"/>
+      <c r="AC9" s="44"/>
       <c r="AD9" s="20" t="s">
         <v>52</v>
       </c>
@@ -2354,8 +2357,8 @@
       <c r="AW9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AX9" s="49"/>
-      <c r="AY9" s="49"/>
+      <c r="AX9" s="44"/>
+      <c r="AY9" s="44"/>
       <c r="AZ9" s="20" t="s">
         <v>52</v>
       </c>
@@ -2416,8 +2419,8 @@
       <c r="BS9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="BT9" s="49"/>
-      <c r="BU9" s="49"/>
+      <c r="BT9" s="44"/>
+      <c r="BU9" s="44"/>
       <c r="BV9" s="20" t="s">
         <v>52</v>
       </c>
@@ -2478,8 +2481,8 @@
       <c r="CO9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="CP9" s="49"/>
-      <c r="CQ9" s="49"/>
+      <c r="CP9" s="44"/>
+      <c r="CQ9" s="44"/>
       <c r="CR9" s="20" t="s">
         <v>52</v>
       </c>
@@ -2540,10 +2543,10 @@
       <c r="DK9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="DL9" s="49"/>
-      <c r="DM9" s="49"/>
-      <c r="DN9" s="56"/>
-      <c r="DO9" s="56"/>
+      <c r="DL9" s="44"/>
+      <c r="DM9" s="44"/>
+      <c r="DN9" s="41"/>
+      <c r="DO9" s="41"/>
       <c r="DP9" s="11"/>
     </row>
     <row r="10" spans="1:120" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2614,8 +2617,8 @@
       <c r="AA10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AB10" s="50"/>
-      <c r="AC10" s="50"/>
+      <c r="AB10" s="45"/>
+      <c r="AC10" s="45"/>
       <c r="AD10" s="21" t="s">
         <v>55</v>
       </c>
@@ -2676,8 +2679,8 @@
       <c r="AW10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AX10" s="50"/>
-      <c r="AY10" s="50"/>
+      <c r="AX10" s="45"/>
+      <c r="AY10" s="45"/>
       <c r="AZ10" s="21" t="s">
         <v>55</v>
       </c>
@@ -2738,8 +2741,8 @@
       <c r="BS10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="BT10" s="50"/>
-      <c r="BU10" s="50"/>
+      <c r="BT10" s="45"/>
+      <c r="BU10" s="45"/>
       <c r="BV10" s="21" t="s">
         <v>55</v>
       </c>
@@ -2800,8 +2803,8 @@
       <c r="CO10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="CP10" s="50"/>
-      <c r="CQ10" s="50"/>
+      <c r="CP10" s="45"/>
+      <c r="CQ10" s="45"/>
       <c r="CR10" s="21" t="s">
         <v>55</v>
       </c>
@@ -2862,10 +2865,10 @@
       <c r="DK10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="DL10" s="50"/>
-      <c r="DM10" s="50"/>
-      <c r="DN10" s="57"/>
-      <c r="DO10" s="57"/>
+      <c r="DL10" s="45"/>
+      <c r="DM10" s="45"/>
+      <c r="DN10" s="42"/>
+      <c r="DO10" s="42"/>
       <c r="DP10" s="11"/>
     </row>
     <row r="11" spans="1:120" x14ac:dyDescent="0.25">
@@ -2891,366 +2894,366 @@
         <f>VLOOKUP(F11,$A$18:$B$29,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="R11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="S11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="T11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="U11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="V11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="W11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="X11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB11" s="28">
+      <c r="H11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="X11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB11" s="56">
         <f>SUMIF(H11:AA11,1,H$9:AA$9)
 +SUMIF(H11:AA11,2,H$9:AA$9)*0.5
 +SUMIF(H11:AA11,3,H$9:AA$9)</f>
         <v>0</v>
       </c>
-      <c r="AC11" s="29">
+      <c r="AC11" s="27">
         <f>SUMIF(H11:AA11,1,H$10:AA$10)
 +SUMIF(H11:AA11,2,H$10:AA$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="AD11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AH11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AK11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AM11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AN11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AO11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AP11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AQ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AR11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AS11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AT11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AU11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AV11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AW11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX11" s="28">
+      <c r="AD11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AS11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AV11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX11" s="56">
         <f>SUMIF(AD11:AW11,1,AD$9:AW$9)
 +SUMIF(AD11:AW11,2,AD$9:AW$9)*0.5
 +SUMIF(AD11:AW11,3,AD$9:AW$9)</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="29">
+      <c r="AY11" s="27">
         <f>SUMIF(AD11:AW11,1,AD$10:AW$10)
 +SUMIF(AD11:AW11,2,AD$10:AW$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="AZ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BA11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BB11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BC11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BD11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BE11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BF11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BG11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BH11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BI11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BJ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BK11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BL11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BM11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BN11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BO11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BP11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BQ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BR11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BS11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BT11" s="28">
+      <c r="AZ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BD11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BE11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BG11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BI11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BJ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BL11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BM11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BN11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BO11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BP11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BQ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BR11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BS11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BT11" s="56">
         <f>SUMIF(AZ11:BS11,1,AZ$9:BS$9)
 +SUMIF(AZ11:BS11,2,AZ$9:BS$9)*0.5
 +SUMIF(AZ11:BS11,3,AZ$9:BS$9)</f>
         <v>0</v>
       </c>
-      <c r="BU11" s="29">
+      <c r="BU11" s="27">
         <f>SUMIF(AZ11:BS11,1,AZ$10:BS$10)
 +SUMIF(AZ11:BS11,2,AZ$10:BS$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="BV11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BW11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BX11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BY11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="BZ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CA11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CB11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CC11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CD11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CE11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CF11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CG11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CH11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CI11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CJ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CK11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CL11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CM11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CN11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CO11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CP11" s="28">
+      <c r="BV11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BW11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BX11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="BZ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CA11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CB11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CC11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CD11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CE11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CF11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CG11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CH11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CI11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CJ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CK11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CL11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CM11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CN11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CO11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP11" s="56">
         <f>SUMIF(BV11:CO11,1,BV$9:CO$9)
 +SUMIF(BV11:CO11,2,BV$9:CO$9)*0.5
 +SUMIF(BV11:CO11,3,BV$9:CO$9)</f>
         <v>0</v>
       </c>
-      <c r="CQ11" s="29">
+      <c r="CQ11" s="27">
         <f>SUMIF(BV11:CO11,1,BV$10:CO$10)
 +SUMIF(BV11:CO11,2,BV$10:CO$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="CR11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CS11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CT11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CU11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CV11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CW11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CX11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CY11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="CZ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DA11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DB11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DC11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DD11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DE11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DF11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DG11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DH11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DI11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DJ11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DK11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="DL11" s="28">
+      <c r="CR11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CS11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CT11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CU11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CV11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CW11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CX11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CY11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="CZ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DA11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DB11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DC11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DD11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DF11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DG11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DH11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DI11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DJ11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DK11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="DL11" s="56">
         <f>SUMIF(CR11:DK11,1,CR$9:DK$9)
 +SUMIF(CR11:DK11,2,CR$9:DK$9)*0.5
 +SUMIF(CR11:DK11,3,CR$9:DK$9)</f>
         <v>0</v>
       </c>
-      <c r="DM11" s="29">
+      <c r="DM11" s="27">
         <f>SUMIF(CR11:DK11,1,CR$10:DK$10)
 +SUMIF(CR11:DK11,2,CR$10:DK$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="DN11" s="28">
+      <c r="DN11" s="56">
         <f>SUM(DL11,AB11,AX11,BT11,CP11)</f>
         <v>0</v>
       </c>
-      <c r="DO11" s="30">
+      <c r="DO11" s="28">
         <f>SUM(DM11,AC11,AY11,BU11,CQ11)</f>
         <v>0</v>
       </c>
@@ -3259,13 +3262,13 @@
       </c>
     </row>
     <row r="12" spans="1:120" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="15">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -3351,11 +3354,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AB12" s="24">
+      <c r="AB12" s="57">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AC12" s="26">
+      <c r="AC12" s="25">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3439,11 +3442,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AX12" s="24">
+      <c r="AX12" s="57">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AY12" s="26">
+      <c r="AY12" s="25">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3527,11 +3530,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="BT12" s="24">
+      <c r="BT12" s="57">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="BU12" s="26">
+      <c r="BU12" s="25">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3615,11 +3618,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CP12" s="24">
+      <c r="CP12" s="57">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CQ12" s="26">
+      <c r="CQ12" s="25">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3703,31 +3706,31 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DL12" s="24">
+      <c r="DL12" s="57">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DM12" s="26">
+      <c r="DM12" s="25">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DN12" s="24">
+      <c r="DN12" s="57">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DO12" s="25">
+      <c r="DO12" s="24">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:120" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
       <c r="F13" s="15">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -3813,11 +3816,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AB13" s="24">
+      <c r="AB13" s="57">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AC13" s="26">
+      <c r="AC13" s="25">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -3901,11 +3904,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AX13" s="24">
+      <c r="AX13" s="57">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AY13" s="26">
+      <c r="AY13" s="25">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -3989,11 +3992,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="BT13" s="24">
+      <c r="BT13" s="57">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="BU13" s="26">
+      <c r="BU13" s="25">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4077,11 +4080,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CP13" s="24">
+      <c r="CP13" s="57">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CQ13" s="26">
+      <c r="CQ13" s="25">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4165,31 +4168,31 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DL13" s="24">
+      <c r="DL13" s="57">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DM13" s="26">
+      <c r="DM13" s="25">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DN13" s="24">
+      <c r="DN13" s="57">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DO13" s="26">
+      <c r="DO13" s="25">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:120" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="15">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -4275,11 +4278,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AB14" s="32">
+      <c r="AB14" s="58">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AC14" s="33">
+      <c r="AC14" s="30">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4363,11 +4366,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AX14" s="32">
+      <c r="AX14" s="58">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="33">
+      <c r="AY14" s="30">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4451,11 +4454,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="BT14" s="32">
+      <c r="BT14" s="58">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="BU14" s="33">
+      <c r="BU14" s="30">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4539,11 +4542,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CP14" s="32">
+      <c r="CP14" s="58">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CQ14" s="33">
+      <c r="CQ14" s="30">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4627,19 +4630,19 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DL14" s="32">
+      <c r="DL14" s="58">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DM14" s="33">
+      <c r="DM14" s="30">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DN14" s="32">
+      <c r="DN14" s="58">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DO14" s="33">
+      <c r="DO14" s="30">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4716,12 +4719,12 @@
       <c r="Z15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AA15" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB15" s="36"/>
-      <c r="AC15" s="37"/>
-      <c r="AD15" s="34" t="s">
+      <c r="AA15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB15" s="33"/>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="AE15" s="9" t="s">
@@ -4778,12 +4781,12 @@
       <c r="AV15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AW15" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX15" s="36"/>
-      <c r="AY15" s="37"/>
-      <c r="AZ15" s="34" t="s">
+      <c r="AW15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX15" s="33"/>
+      <c r="AY15" s="34"/>
+      <c r="AZ15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="BA15" s="9" t="s">
@@ -4840,12 +4843,12 @@
       <c r="BR15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BS15" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="BT15" s="36"/>
-      <c r="BU15" s="37"/>
-      <c r="BV15" s="34" t="s">
+      <c r="BS15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="BT15" s="33"/>
+      <c r="BU15" s="34"/>
+      <c r="BV15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="BW15" s="9" t="s">
@@ -4902,12 +4905,12 @@
       <c r="CN15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="CO15" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="CP15" s="36"/>
-      <c r="CQ15" s="37"/>
-      <c r="CR15" s="34" t="s">
+      <c r="CO15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP15" s="33"/>
+      <c r="CQ15" s="34"/>
+      <c r="CR15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="CS15" s="9" t="s">
@@ -4964,25 +4967,25 @@
       <c r="DJ15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="DK15" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="DL15" s="36"/>
-      <c r="DM15" s="37"/>
-      <c r="DN15" s="58"/>
-      <c r="DO15" s="37"/>
-      <c r="DP15" s="40" t="s">
+      <c r="DK15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="DL15" s="33"/>
+      <c r="DM15" s="34"/>
+      <c r="DN15" s="38"/>
+      <c r="DO15" s="34"/>
+      <c r="DP15" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:120" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
       <c r="F16" s="18">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -5068,8 +5071,8 @@
         <f>COUNTIF(nichtFreigegeben20,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="AB16" s="38"/>
-      <c r="AC16" s="38"/>
+      <c r="AB16" s="35"/>
+      <c r="AC16" s="35"/>
       <c r="AD16" s="15">
         <f>COUNTIF(nichtFreigegeben21,"&gt;0")</f>
         <v>0</v>
@@ -5150,8 +5153,8 @@
         <f>COUNTIF(nichtFreigegeben40,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="AX16" s="38"/>
-      <c r="AY16" s="38"/>
+      <c r="AX16" s="35"/>
+      <c r="AY16" s="35"/>
       <c r="AZ16" s="15">
         <f>COUNTIF(nichtFreigegeben41,"&gt;0")</f>
         <v>0</v>
@@ -5232,8 +5235,8 @@
         <f>COUNTIF(nichtFreigegeben60,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="BT16" s="38"/>
-      <c r="BU16" s="38"/>
+      <c r="BT16" s="35"/>
+      <c r="BU16" s="35"/>
       <c r="BV16" s="15">
         <f>COUNTIF(nichtFreigegeben61,"&gt;0")</f>
         <v>0</v>
@@ -5314,8 +5317,8 @@
         <f>COUNTIF(nichtFreigegeben80,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="CP16" s="38"/>
-      <c r="CQ16" s="38"/>
+      <c r="CP16" s="35"/>
+      <c r="CQ16" s="35"/>
       <c r="CR16" s="15">
         <f>COUNTIF(nichtFreigegeben81,"&gt;0")</f>
         <v>0</v>
@@ -5396,25 +5399,25 @@
         <f>COUNTIF(nichtFreigegeben100,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="DL16" s="38"/>
-      <c r="DM16" s="38"/>
-      <c r="DN16" s="35"/>
-      <c r="DO16" s="38"/>
-      <c r="DP16" s="40"/>
+      <c r="DL16" s="35"/>
+      <c r="DM16" s="35"/>
+      <c r="DN16" s="32"/>
+      <c r="DO16" s="35"/>
+      <c r="DP16" s="37"/>
     </row>
     <row r="17" spans="1:119" x14ac:dyDescent="0.25">
-      <c r="AB17" s="39"/>
-      <c r="AC17" s="39"/>
-      <c r="AX17" s="39"/>
-      <c r="AY17" s="39"/>
-      <c r="BT17" s="39"/>
-      <c r="BU17" s="39"/>
-      <c r="CP17" s="39"/>
-      <c r="CQ17" s="39"/>
-      <c r="DL17" s="39"/>
-      <c r="DM17" s="39"/>
-      <c r="DN17" s="39"/>
-      <c r="DO17" s="39"/>
+      <c r="AB17" s="36"/>
+      <c r="AC17" s="36"/>
+      <c r="AX17" s="36"/>
+      <c r="AY17" s="36"/>
+      <c r="BT17" s="36"/>
+      <c r="BU17" s="36"/>
+      <c r="CP17" s="36"/>
+      <c r="CQ17" s="36"/>
+      <c r="DL17" s="36"/>
+      <c r="DM17" s="36"/>
+      <c r="DN17" s="36"/>
+      <c r="DO17" s="36"/>
     </row>
     <row r="18" spans="1:119" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5557,57 +5560,41 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="31">
+      <c r="A37" s="29">
         <v>1</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="47"/>
+      <c r="C37" s="54"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="31">
+      <c r="A38" s="29">
         <v>2</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="47"/>
+      <c r="C38" s="54"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="31">
+      <c r="A39" s="29">
         <v>3</v>
       </c>
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="47"/>
+      <c r="C39" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="DN7:DO7"/>
-    <mergeCell ref="DN8:DN10"/>
-    <mergeCell ref="DO8:DO10"/>
-    <mergeCell ref="CP8:CP10"/>
-    <mergeCell ref="CQ8:CQ10"/>
-    <mergeCell ref="DL8:DL10"/>
-    <mergeCell ref="DM8:DM10"/>
-    <mergeCell ref="CR7:DM7"/>
-    <mergeCell ref="BV7:CQ7"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AD7:AY7"/>
     <mergeCell ref="AZ7:BU7"/>
@@ -5624,6 +5611,22 @@
     <mergeCell ref="H7:AC7"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="DN7:DO7"/>
+    <mergeCell ref="DN8:DN10"/>
+    <mergeCell ref="DO8:DO10"/>
+    <mergeCell ref="CP8:CP10"/>
+    <mergeCell ref="CQ8:CQ10"/>
+    <mergeCell ref="DL8:DL10"/>
+    <mergeCell ref="DM8:DM10"/>
+    <mergeCell ref="CR7:DM7"/>
+    <mergeCell ref="BV7:CQ7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
direct-to-dev fix rounding problem in AnmeldungenTagesschule Excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E8317B-B590-45F5-A3CA-826EAB62D5F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC82F0-6ADF-4915-89E8-D3CA085BF538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -777,9 +777,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -835,23 +832,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -861,21 +858,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -895,6 +877,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1308,7 +1308,9 @@
   </sheetPr>
   <dimension ref="A1:DV39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1413,10 +1415,10 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:126" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="3"/>
@@ -1852,170 +1854,170 @@
       <c r="DT6" s="13"/>
     </row>
     <row r="7" spans="1:126" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="60" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="61"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="60" t="s">
+      <c r="E7" s="55"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="61"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="42" t="s">
+      <c r="H7" s="55"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="41" t="s">
         <v>0</v>
       </c>
       <c r="M7" s="16"/>
-      <c r="N7" s="52" t="s">
+      <c r="N7" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="53"/>
-      <c r="Y7" s="53"/>
-      <c r="Z7" s="53"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="53"/>
-      <c r="AC7" s="53"/>
-      <c r="AD7" s="53"/>
-      <c r="AE7" s="53"/>
-      <c r="AF7" s="53"/>
-      <c r="AG7" s="53"/>
-      <c r="AH7" s="53"/>
-      <c r="AI7" s="54"/>
-      <c r="AJ7" s="52" t="s">
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+      <c r="X7" s="47"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
+      <c r="AA7" s="47"/>
+      <c r="AB7" s="47"/>
+      <c r="AC7" s="47"/>
+      <c r="AD7" s="47"/>
+      <c r="AE7" s="47"/>
+      <c r="AF7" s="47"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="47"/>
+      <c r="AI7" s="48"/>
+      <c r="AJ7" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="AK7" s="53"/>
-      <c r="AL7" s="53"/>
-      <c r="AM7" s="53"/>
-      <c r="AN7" s="53"/>
-      <c r="AO7" s="53"/>
-      <c r="AP7" s="53"/>
-      <c r="AQ7" s="53"/>
-      <c r="AR7" s="53"/>
-      <c r="AS7" s="53"/>
-      <c r="AT7" s="53"/>
-      <c r="AU7" s="53"/>
-      <c r="AV7" s="53"/>
-      <c r="AW7" s="53"/>
-      <c r="AX7" s="53"/>
-      <c r="AY7" s="53"/>
-      <c r="AZ7" s="53"/>
-      <c r="BA7" s="53"/>
-      <c r="BB7" s="53"/>
-      <c r="BC7" s="53"/>
-      <c r="BD7" s="53"/>
-      <c r="BE7" s="54"/>
-      <c r="BF7" s="52" t="s">
+      <c r="AK7" s="47"/>
+      <c r="AL7" s="47"/>
+      <c r="AM7" s="47"/>
+      <c r="AN7" s="47"/>
+      <c r="AO7" s="47"/>
+      <c r="AP7" s="47"/>
+      <c r="AQ7" s="47"/>
+      <c r="AR7" s="47"/>
+      <c r="AS7" s="47"/>
+      <c r="AT7" s="47"/>
+      <c r="AU7" s="47"/>
+      <c r="AV7" s="47"/>
+      <c r="AW7" s="47"/>
+      <c r="AX7" s="47"/>
+      <c r="AY7" s="47"/>
+      <c r="AZ7" s="47"/>
+      <c r="BA7" s="47"/>
+      <c r="BB7" s="47"/>
+      <c r="BC7" s="47"/>
+      <c r="BD7" s="47"/>
+      <c r="BE7" s="48"/>
+      <c r="BF7" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="53"/>
-      <c r="BH7" s="53"/>
-      <c r="BI7" s="53"/>
-      <c r="BJ7" s="53"/>
-      <c r="BK7" s="53"/>
-      <c r="BL7" s="53"/>
-      <c r="BM7" s="53"/>
-      <c r="BN7" s="53"/>
-      <c r="BO7" s="53"/>
-      <c r="BP7" s="53"/>
-      <c r="BQ7" s="53"/>
-      <c r="BR7" s="53"/>
-      <c r="BS7" s="53"/>
-      <c r="BT7" s="53"/>
-      <c r="BU7" s="53"/>
-      <c r="BV7" s="53"/>
-      <c r="BW7" s="53"/>
-      <c r="BX7" s="53"/>
-      <c r="BY7" s="53"/>
-      <c r="BZ7" s="53"/>
-      <c r="CA7" s="54"/>
-      <c r="CB7" s="52" t="s">
+      <c r="BG7" s="47"/>
+      <c r="BH7" s="47"/>
+      <c r="BI7" s="47"/>
+      <c r="BJ7" s="47"/>
+      <c r="BK7" s="47"/>
+      <c r="BL7" s="47"/>
+      <c r="BM7" s="47"/>
+      <c r="BN7" s="47"/>
+      <c r="BO7" s="47"/>
+      <c r="BP7" s="47"/>
+      <c r="BQ7" s="47"/>
+      <c r="BR7" s="47"/>
+      <c r="BS7" s="47"/>
+      <c r="BT7" s="47"/>
+      <c r="BU7" s="47"/>
+      <c r="BV7" s="47"/>
+      <c r="BW7" s="47"/>
+      <c r="BX7" s="47"/>
+      <c r="BY7" s="47"/>
+      <c r="BZ7" s="47"/>
+      <c r="CA7" s="48"/>
+      <c r="CB7" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="CC7" s="53"/>
-      <c r="CD7" s="53"/>
-      <c r="CE7" s="53"/>
-      <c r="CF7" s="53"/>
-      <c r="CG7" s="53"/>
-      <c r="CH7" s="53"/>
-      <c r="CI7" s="53"/>
-      <c r="CJ7" s="53"/>
-      <c r="CK7" s="53"/>
-      <c r="CL7" s="53"/>
-      <c r="CM7" s="53"/>
-      <c r="CN7" s="53"/>
-      <c r="CO7" s="53"/>
-      <c r="CP7" s="53"/>
-      <c r="CQ7" s="53"/>
-      <c r="CR7" s="53"/>
-      <c r="CS7" s="53"/>
-      <c r="CT7" s="53"/>
-      <c r="CU7" s="53"/>
-      <c r="CV7" s="53"/>
-      <c r="CW7" s="54"/>
-      <c r="CX7" s="52" t="s">
+      <c r="CC7" s="47"/>
+      <c r="CD7" s="47"/>
+      <c r="CE7" s="47"/>
+      <c r="CF7" s="47"/>
+      <c r="CG7" s="47"/>
+      <c r="CH7" s="47"/>
+      <c r="CI7" s="47"/>
+      <c r="CJ7" s="47"/>
+      <c r="CK7" s="47"/>
+      <c r="CL7" s="47"/>
+      <c r="CM7" s="47"/>
+      <c r="CN7" s="47"/>
+      <c r="CO7" s="47"/>
+      <c r="CP7" s="47"/>
+      <c r="CQ7" s="47"/>
+      <c r="CR7" s="47"/>
+      <c r="CS7" s="47"/>
+      <c r="CT7" s="47"/>
+      <c r="CU7" s="47"/>
+      <c r="CV7" s="47"/>
+      <c r="CW7" s="48"/>
+      <c r="CX7" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="CY7" s="53"/>
-      <c r="CZ7" s="53"/>
-      <c r="DA7" s="53"/>
-      <c r="DB7" s="53"/>
-      <c r="DC7" s="53"/>
-      <c r="DD7" s="53"/>
-      <c r="DE7" s="53"/>
-      <c r="DF7" s="53"/>
-      <c r="DG7" s="53"/>
-      <c r="DH7" s="53"/>
-      <c r="DI7" s="53"/>
-      <c r="DJ7" s="53"/>
-      <c r="DK7" s="53"/>
-      <c r="DL7" s="53"/>
-      <c r="DM7" s="53"/>
-      <c r="DN7" s="53"/>
-      <c r="DO7" s="53"/>
-      <c r="DP7" s="53"/>
-      <c r="DQ7" s="53"/>
-      <c r="DR7" s="53"/>
-      <c r="DS7" s="54"/>
-      <c r="DT7" s="45" t="s">
+      <c r="CY7" s="47"/>
+      <c r="CZ7" s="47"/>
+      <c r="DA7" s="47"/>
+      <c r="DB7" s="47"/>
+      <c r="DC7" s="47"/>
+      <c r="DD7" s="47"/>
+      <c r="DE7" s="47"/>
+      <c r="DF7" s="47"/>
+      <c r="DG7" s="47"/>
+      <c r="DH7" s="47"/>
+      <c r="DI7" s="47"/>
+      <c r="DJ7" s="47"/>
+      <c r="DK7" s="47"/>
+      <c r="DL7" s="47"/>
+      <c r="DM7" s="47"/>
+      <c r="DN7" s="47"/>
+      <c r="DO7" s="47"/>
+      <c r="DP7" s="47"/>
+      <c r="DQ7" s="47"/>
+      <c r="DR7" s="47"/>
+      <c r="DS7" s="48"/>
+      <c r="DT7" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="DU7" s="45"/>
+      <c r="DU7" s="60"/>
       <c r="DV7" s="11"/>
     </row>
     <row r="8" spans="1:126" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
       <c r="M8" s="17"/>
       <c r="N8" s="4" t="s">
         <v>6</v>
@@ -2077,10 +2079,10 @@
       <c r="AG8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AH8" s="49" t="s">
+      <c r="AH8" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="AI8" s="49" t="s">
+      <c r="AI8" s="50" t="s">
         <v>49</v>
       </c>
       <c r="AJ8" s="4" t="s">
@@ -2143,10 +2145,10 @@
       <c r="BC8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BD8" s="49" t="s">
+      <c r="BD8" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="BE8" s="49" t="s">
+      <c r="BE8" s="50" t="s">
         <v>49</v>
       </c>
       <c r="BF8" s="4" t="s">
@@ -2209,10 +2211,10 @@
       <c r="BY8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BZ8" s="49" t="s">
+      <c r="BZ8" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="CA8" s="49" t="s">
+      <c r="CA8" s="50" t="s">
         <v>49</v>
       </c>
       <c r="CB8" s="4" t="s">
@@ -2275,10 +2277,10 @@
       <c r="CU8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CV8" s="49" t="s">
+      <c r="CV8" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="CW8" s="49" t="s">
+      <c r="CW8" s="50" t="s">
         <v>49</v>
       </c>
       <c r="CX8" s="4" t="s">
@@ -2341,692 +2343,692 @@
       <c r="DQ8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DR8" s="49" t="s">
+      <c r="DR8" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="DS8" s="49" t="s">
+      <c r="DS8" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="DT8" s="46" t="s">
+      <c r="DT8" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="DU8" s="46" t="s">
+      <c r="DU8" s="61" t="s">
         <v>56</v>
       </c>
       <c r="DV8" s="11"/>
     </row>
     <row r="9" spans="1:126" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
       <c r="M9" s="17"/>
-      <c r="N9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="P9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="R9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="S9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="T9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="U9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="V9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="W9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="X9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH9" s="50"/>
-      <c r="AI9" s="50"/>
-      <c r="AJ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AO9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AT9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AU9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AW9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AX9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BB9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BC9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD9" s="50"/>
-      <c r="BE9" s="50"/>
-      <c r="BF9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BG9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BH9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BJ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BL9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BO9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BP9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BQ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BR9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BS9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BT9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BU9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BV9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BW9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BX9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BY9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="BZ9" s="50"/>
-      <c r="CA9" s="50"/>
-      <c r="CB9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CC9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CD9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CE9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CF9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CG9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CH9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CI9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CJ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CK9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CL9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CM9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CN9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CO9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CP9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CQ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CR9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CS9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CT9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CU9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CV9" s="50"/>
-      <c r="CW9" s="50"/>
-      <c r="CX9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CY9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CZ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DA9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DB9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DC9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DD9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DE9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DF9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DG9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DH9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DI9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DJ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DK9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DL9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DM9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DN9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DO9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DP9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DQ9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="DR9" s="50"/>
-      <c r="DS9" s="50"/>
-      <c r="DT9" s="47"/>
-      <c r="DU9" s="47"/>
+      <c r="N9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="R9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="V9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="W9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH9" s="51"/>
+      <c r="AI9" s="51"/>
+      <c r="AJ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AV9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BC9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD9" s="51"/>
+      <c r="BE9" s="51"/>
+      <c r="BF9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BG9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BH9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BM9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BN9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BO9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BP9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BQ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BR9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BS9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BT9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BW9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BX9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BY9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="BZ9" s="51"/>
+      <c r="CA9" s="51"/>
+      <c r="CB9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CC9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CD9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CE9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CF9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CG9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CH9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CI9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CJ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CK9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CL9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CM9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CN9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CO9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CP9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CQ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CR9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CS9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CT9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CU9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CV9" s="51"/>
+      <c r="CW9" s="51"/>
+      <c r="CX9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CY9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="CZ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DA9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DB9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DC9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DD9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DE9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DF9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DG9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DH9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DI9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DJ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DK9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DL9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DM9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DN9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DO9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DP9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DQ9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="DR9" s="51"/>
+      <c r="DS9" s="51"/>
+      <c r="DT9" s="62"/>
+      <c r="DU9" s="62"/>
       <c r="DV9" s="11"/>
     </row>
     <row r="10" spans="1:126" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="17"/>
-      <c r="N10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="O10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="T10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="U10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="V10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="W10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="X10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH10" s="51"/>
-      <c r="AI10" s="51"/>
-      <c r="AJ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AS10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AT10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AW10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AX10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AY10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AZ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BA10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BD10" s="51"/>
-      <c r="BE10" s="51"/>
-      <c r="BF10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BH10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BJ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BM10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BN10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BO10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BP10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BQ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BR10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BS10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BT10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BU10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BV10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BW10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BX10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BY10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="BZ10" s="51"/>
-      <c r="CA10" s="51"/>
-      <c r="CB10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CC10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CD10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CE10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CF10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CG10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CH10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CI10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CJ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CK10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CL10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CM10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CN10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CO10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CP10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CQ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CR10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CS10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CT10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CU10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CV10" s="51"/>
-      <c r="CW10" s="51"/>
-      <c r="CX10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CY10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="CZ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DA10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DB10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DC10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DD10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DE10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DF10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DG10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DH10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DI10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DJ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DK10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DL10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DM10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DN10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DO10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DP10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DQ10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="DR10" s="51"/>
-      <c r="DS10" s="51"/>
-      <c r="DT10" s="48"/>
-      <c r="DU10" s="48"/>
+      <c r="N10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="V10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="W10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="X10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH10" s="52"/>
+      <c r="AI10" s="52"/>
+      <c r="AJ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD10" s="52"/>
+      <c r="BE10" s="52"/>
+      <c r="BF10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BH10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BI10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BJ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BK10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BL10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BM10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BN10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BO10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BP10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BR10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BS10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BT10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BU10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BV10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BW10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BX10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BY10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BZ10" s="52"/>
+      <c r="CA10" s="52"/>
+      <c r="CB10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CC10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CD10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CE10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CF10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CG10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CH10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CI10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CJ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CK10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CL10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CM10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CN10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CO10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CP10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CQ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CR10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CS10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CT10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CU10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CV10" s="52"/>
+      <c r="CW10" s="52"/>
+      <c r="CX10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CY10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CZ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DA10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DB10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DC10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DD10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DE10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DF10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DG10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DH10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DI10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DJ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DK10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DL10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DM10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DN10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DO10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DP10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DQ10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="DR10" s="52"/>
+      <c r="DS10" s="52"/>
+      <c r="DT10" s="63"/>
+      <c r="DU10" s="63"/>
       <c r="DV10" s="11"/>
     </row>
     <row r="11" spans="1:126" x14ac:dyDescent="0.25">
@@ -3070,366 +3072,366 @@
         <f>VLOOKUP(L11,$A$18:$B$29,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="N11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="O11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="P11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="R11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="S11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="T11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="U11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="V11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="W11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="X11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH11" s="38">
+      <c r="N11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="U11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="V11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="W11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="X11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH11" s="37">
         <f>SUMIF(N11:AG11,1,N$9:AG$9)
 +SUMIF(N11:AG11,2,N$9:AG$9)*0.5
 +SUMIF(N11:AG11,3,N$9:AG$9)</f>
         <v>0</v>
       </c>
-      <c r="AI11" s="26">
+      <c r="AI11" s="25">
         <f>SUMIF(N11:AG11,1,N$10:AG$10)
 +SUMIF(N11:AG11,2,N$10:AG$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="AJ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AM11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AN11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AP11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AQ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AW11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AZ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BA11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BB11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BC11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BD11" s="38">
+      <c r="AJ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AQ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BC11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BD11" s="37">
         <f>SUMIF(AJ11:BC11,1,AJ$9:BC$9)
 +SUMIF(AJ11:BC11,2,AJ$9:BC$9)*0.5
 +SUMIF(AJ11:BC11,3,AJ$9:BC$9)</f>
         <v>0</v>
       </c>
-      <c r="BE11" s="26">
+      <c r="BE11" s="25">
         <f>SUMIF(AJ11:BC11,1,AJ$10:BC$10)
 +SUMIF(AJ11:BC11,2,AJ$10:BC$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="BF11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BG11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BH11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BI11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BJ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BK11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BL11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BM11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BN11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BO11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BP11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BQ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BR11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BS11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BT11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BU11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BV11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BW11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BX11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BY11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="BZ11" s="38">
+      <c r="BF11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BG11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BI11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BK11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BL11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BN11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BP11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BQ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BS11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BT11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BU11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BV11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BX11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BY11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="BZ11" s="37">
         <f>SUMIF(BF11:BY11,1,BF$9:BY$9)
 +SUMIF(BF11:BY11,2,BF$9:BY$9)*0.5
 +SUMIF(BF11:BY11,3,BF$9:BY$9)</f>
         <v>0</v>
       </c>
-      <c r="CA11" s="26">
+      <c r="CA11" s="25">
         <f>SUMIF(BF11:BY11,1,BF$10:BY$10)
 +SUMIF(BF11:BY11,2,BF$10:BY$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="CB11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CC11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CD11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CE11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CF11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CG11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CH11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CI11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CJ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CK11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CL11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CM11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CN11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CO11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CP11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CQ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CR11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CS11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CT11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CU11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CV11" s="38">
+      <c r="CB11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CC11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CD11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CE11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CF11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CG11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CH11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CI11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CJ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CK11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CL11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CM11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CN11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CO11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CP11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CQ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CR11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CS11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CT11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CU11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CV11" s="37">
         <f>SUMIF(CB11:CU11,1,CB$9:CU$9)
 +SUMIF(CB11:CU11,2,CB$9:CU$9)*0.5
 +SUMIF(CB11:CU11,3,CB$9:CU$9)</f>
         <v>0</v>
       </c>
-      <c r="CW11" s="26">
+      <c r="CW11" s="25">
         <f>SUMIF(CB11:CU11,1,CB$10:CU$10)
 +SUMIF(CB11:CU11,2,CB$10:CU$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="CX11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CY11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="CZ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DA11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DB11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DC11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DD11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DE11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DF11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DG11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DH11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DI11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DJ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DK11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DL11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DM11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DN11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DO11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DP11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DQ11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="DR11" s="38">
+      <c r="CX11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CY11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CZ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DA11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DB11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DC11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DD11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DE11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DF11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DG11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DH11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DI11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DJ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DK11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DL11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DM11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DN11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DO11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DP11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DQ11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="DR11" s="37">
         <f>SUMIF(CX11:DQ11,1,CX$9:DQ$9)
 +SUMIF(CX11:DQ11,2,CX$9:DQ$9)*0.5
 +SUMIF(CX11:DQ11,3,CX$9:DQ$9)</f>
         <v>0</v>
       </c>
-      <c r="DS11" s="26">
+      <c r="DS11" s="25">
         <f>SUMIF(CX11:DQ11,1,CX$10:DQ$10)
 +SUMIF(CX11:DQ11,2,CX$10:DQ$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="DT11" s="38">
+      <c r="DT11" s="37">
         <f>SUM(DR11,AH11,BD11,BZ11,CV11)</f>
         <v>0</v>
       </c>
-      <c r="DU11" s="27">
+      <c r="DU11" s="26">
         <f>SUM(DS11,AI11,BE11,CA11,CW11)</f>
         <v>0</v>
       </c>
@@ -3438,19 +3440,19 @@
       </c>
     </row>
     <row r="12" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="57"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="15">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -3536,11 +3538,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AH12" s="39">
+      <c r="AH12" s="38">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AI12" s="24">
+      <c r="AI12" s="23">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3624,11 +3626,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="BD12" s="39">
+      <c r="BD12" s="38">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="BE12" s="24">
+      <c r="BE12" s="23">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3712,11 +3714,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="BZ12" s="39">
+      <c r="BZ12" s="38">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CA12" s="24">
+      <c r="CA12" s="23">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3800,11 +3802,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CV12" s="39">
+      <c r="CV12" s="38">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CW12" s="24">
+      <c r="CW12" s="23">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3888,37 +3890,37 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DR12" s="39">
+      <c r="DR12" s="38">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DS12" s="24">
+      <c r="DS12" s="23">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DT12" s="39">
+      <c r="DT12" s="38">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DU12" s="23">
+      <c r="DU12" s="22">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="57"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="45"/>
       <c r="L13" s="15">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4004,11 +4006,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AH13" s="39">
+      <c r="AH13" s="38">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AI13" s="24">
+      <c r="AI13" s="23">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4092,11 +4094,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="BD13" s="39">
+      <c r="BD13" s="38">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="BE13" s="24">
+      <c r="BE13" s="23">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4180,11 +4182,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="BZ13" s="39">
+      <c r="BZ13" s="38">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CA13" s="24">
+      <c r="CA13" s="23">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4268,11 +4270,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CV13" s="39">
+      <c r="CV13" s="38">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CW13" s="24">
+      <c r="CW13" s="23">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4356,37 +4358,37 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DR13" s="39">
+      <c r="DR13" s="38">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DS13" s="24">
+      <c r="DS13" s="23">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DT13" s="39">
+      <c r="DT13" s="38">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DU13" s="24">
+      <c r="DU13" s="23">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="57"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="45"/>
       <c r="L14" s="15">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -4472,11 +4474,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AH14" s="40">
+      <c r="AH14" s="39">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AI14" s="29">
+      <c r="AI14" s="28">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4560,11 +4562,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="BD14" s="40">
+      <c r="BD14" s="39">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="BE14" s="29">
+      <c r="BE14" s="28">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4648,11 +4650,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="BZ14" s="40">
+      <c r="BZ14" s="39">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CA14" s="29">
+      <c r="CA14" s="28">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4736,11 +4738,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CV14" s="40">
+      <c r="CV14" s="39">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CW14" s="29">
+      <c r="CW14" s="28">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4824,19 +4826,19 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DR14" s="40">
+      <c r="DR14" s="39">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DS14" s="29">
+      <c r="DS14" s="28">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DT14" s="40">
+      <c r="DT14" s="39">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DU14" s="29">
+      <c r="DU14" s="28">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4919,12 +4921,12 @@
       <c r="AF15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AG15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH15" s="32"/>
-      <c r="AI15" s="33"/>
-      <c r="AJ15" s="30" t="s">
+      <c r="AG15" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH15" s="31"/>
+      <c r="AI15" s="32"/>
+      <c r="AJ15" s="29" t="s">
         <v>8</v>
       </c>
       <c r="AK15" s="9" t="s">
@@ -4981,12 +4983,12 @@
       <c r="BB15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BC15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="BD15" s="32"/>
-      <c r="BE15" s="33"/>
-      <c r="BF15" s="30" t="s">
+      <c r="BC15" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="BD15" s="31"/>
+      <c r="BE15" s="32"/>
+      <c r="BF15" s="29" t="s">
         <v>8</v>
       </c>
       <c r="BG15" s="9" t="s">
@@ -5043,12 +5045,12 @@
       <c r="BX15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BY15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="BZ15" s="32"/>
-      <c r="CA15" s="33"/>
-      <c r="CB15" s="30" t="s">
+      <c r="BY15" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="BZ15" s="31"/>
+      <c r="CA15" s="32"/>
+      <c r="CB15" s="29" t="s">
         <v>8</v>
       </c>
       <c r="CC15" s="9" t="s">
@@ -5105,12 +5107,12 @@
       <c r="CT15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="CU15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="CV15" s="32"/>
-      <c r="CW15" s="33"/>
-      <c r="CX15" s="30" t="s">
+      <c r="CU15" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="CV15" s="31"/>
+      <c r="CW15" s="32"/>
+      <c r="CX15" s="29" t="s">
         <v>8</v>
       </c>
       <c r="CY15" s="9" t="s">
@@ -5167,31 +5169,31 @@
       <c r="DP15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="DQ15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="DR15" s="32"/>
-      <c r="DS15" s="33"/>
-      <c r="DT15" s="37"/>
-      <c r="DU15" s="33"/>
-      <c r="DV15" s="36" t="s">
+      <c r="DQ15" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="DR15" s="31"/>
+      <c r="DS15" s="32"/>
+      <c r="DT15" s="36"/>
+      <c r="DU15" s="32"/>
+      <c r="DV15" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
       <c r="L16" s="18">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -5277,8 +5279,8 @@
         <f>COUNTIF(nichtFreigegeben20,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="AH16" s="34"/>
-      <c r="AI16" s="34"/>
+      <c r="AH16" s="33"/>
+      <c r="AI16" s="33"/>
       <c r="AJ16" s="15">
         <f>COUNTIF(nichtFreigegeben21,"&gt;0")</f>
         <v>0</v>
@@ -5359,8 +5361,8 @@
         <f>COUNTIF(nichtFreigegeben40,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="BD16" s="34"/>
-      <c r="BE16" s="34"/>
+      <c r="BD16" s="33"/>
+      <c r="BE16" s="33"/>
       <c r="BF16" s="15">
         <f>COUNTIF(nichtFreigegeben41,"&gt;0")</f>
         <v>0</v>
@@ -5441,8 +5443,8 @@
         <f>COUNTIF(nichtFreigegeben60,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="BZ16" s="34"/>
-      <c r="CA16" s="34"/>
+      <c r="BZ16" s="33"/>
+      <c r="CA16" s="33"/>
       <c r="CB16" s="15">
         <f>COUNTIF(nichtFreigegeben61,"&gt;0")</f>
         <v>0</v>
@@ -5523,8 +5525,8 @@
         <f>COUNTIF(nichtFreigegeben80,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="CV16" s="34"/>
-      <c r="CW16" s="34"/>
+      <c r="CV16" s="33"/>
+      <c r="CW16" s="33"/>
       <c r="CX16" s="15">
         <f>COUNTIF(nichtFreigegeben81,"&gt;0")</f>
         <v>0</v>
@@ -5605,25 +5607,25 @@
         <f>COUNTIF(nichtFreigegeben100,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="DR16" s="34"/>
-      <c r="DS16" s="34"/>
-      <c r="DT16" s="31"/>
-      <c r="DU16" s="34"/>
-      <c r="DV16" s="36"/>
+      <c r="DR16" s="33"/>
+      <c r="DS16" s="33"/>
+      <c r="DT16" s="30"/>
+      <c r="DU16" s="33"/>
+      <c r="DV16" s="35"/>
     </row>
     <row r="17" spans="1:125" x14ac:dyDescent="0.25">
-      <c r="AH17" s="35"/>
-      <c r="AI17" s="35"/>
-      <c r="BD17" s="35"/>
-      <c r="BE17" s="35"/>
-      <c r="BZ17" s="35"/>
-      <c r="CA17" s="35"/>
-      <c r="CV17" s="35"/>
-      <c r="CW17" s="35"/>
-      <c r="DR17" s="35"/>
-      <c r="DS17" s="35"/>
-      <c r="DT17" s="35"/>
-      <c r="DU17" s="35"/>
+      <c r="AH17" s="34"/>
+      <c r="AI17" s="34"/>
+      <c r="BD17" s="34"/>
+      <c r="BE17" s="34"/>
+      <c r="BZ17" s="34"/>
+      <c r="CA17" s="34"/>
+      <c r="CV17" s="34"/>
+      <c r="CW17" s="34"/>
+      <c r="DR17" s="34"/>
+      <c r="DS17" s="34"/>
+      <c r="DT17" s="34"/>
+      <c r="DU17" s="34"/>
     </row>
     <row r="18" spans="1:125" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5766,64 +5768,79 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="57"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="28">
+      <c r="A37" s="27">
         <v>1</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="28">
+      <c r="A38" s="27">
         <v>2</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="28">
+      <c r="A39" s="27">
         <v>3</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="DT7:DU7"/>
+    <mergeCell ref="DT8:DT10"/>
+    <mergeCell ref="DU8:DU10"/>
+    <mergeCell ref="CV8:CV10"/>
+    <mergeCell ref="CW8:CW10"/>
+    <mergeCell ref="DR8:DR10"/>
+    <mergeCell ref="DS8:DS10"/>
+    <mergeCell ref="CX7:DS7"/>
+    <mergeCell ref="CB7:CW7"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="D7:F8"/>
+    <mergeCell ref="G7:I8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AJ7:BE7"/>
     <mergeCell ref="BF7:CA7"/>
@@ -5840,26 +5857,11 @@
     <mergeCell ref="A16:K16"/>
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="D7:F8"/>
-    <mergeCell ref="G7:I8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="DT7:DU7"/>
-    <mergeCell ref="DT8:DT10"/>
-    <mergeCell ref="DU8:DU10"/>
-    <mergeCell ref="CV8:CV10"/>
-    <mergeCell ref="CW8:CW10"/>
-    <mergeCell ref="DR8:DR10"/>
-    <mergeCell ref="DS8:DS10"/>
-    <mergeCell ref="CX7:DS7"/>
-    <mergeCell ref="CB7:CW7"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2376 Stammdaten von nicht freigegebenen Anträgen in AnmeldungTagesschule Statistik zeigen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E044C55-517A-4AC0-BBE3-98F9F305D263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063A746E-A105-4FCF-9753-4DF7E17BAF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="81">
   <si>
     <t>{statusTitle}</t>
   </si>
@@ -859,26 +859,20 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -889,18 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -919,10 +902,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -930,6 +915,21 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1344,29 +1344,27 @@
   </sheetPr>
   <dimension ref="A1:DZ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625"/>
-    <col min="3" max="13" width="17.5546875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375"/>
+    <col min="3" max="13" width="17.5703125" style="1" customWidth="1"/>
     <col min="14" max="15" width="17"/>
-    <col min="16" max="16" width="33.109375" customWidth="1"/>
-    <col min="17" max="17" width="33.109375" hidden="1" customWidth="1"/>
-    <col min="18" max="22" width="13.33203125" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" customWidth="1"/>
-    <col min="24" max="37" width="10.5546875"/>
-    <col min="40" max="59" width="10.5546875"/>
-    <col min="62" max="81" width="10.5546875"/>
-    <col min="84" max="103" width="10.5546875"/>
-    <col min="106" max="124" width="10.5546875"/>
-    <col min="125" max="125" width="8.88671875" customWidth="1"/>
-    <col min="128" max="986" width="10.5546875"/>
+    <col min="16" max="16" width="33.140625" customWidth="1"/>
+    <col min="17" max="17" width="33.140625" hidden="1" customWidth="1"/>
+    <col min="18" max="22" width="13.28515625" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" customWidth="1"/>
+    <col min="24" max="37" width="10.5703125"/>
+    <col min="40" max="59" width="10.5703125"/>
+    <col min="62" max="81" width="10.5703125"/>
+    <col min="84" max="103" width="10.5703125"/>
+    <col min="106" max="124" width="10.5703125"/>
+    <col min="125" max="125" width="8.85546875" customWidth="1"/>
+    <col min="128" max="986" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:130" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:130" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -1392,7 +1390,7 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:130" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:130" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1418,7 +1416,7 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:130" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:130" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1442,7 +1440,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1466,7 +1464,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:130" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:130" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>51</v>
       </c>
@@ -1599,7 +1597,7 @@
       <c r="DV5" s="2"/>
       <c r="DW5" s="2"/>
     </row>
-    <row r="6" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
@@ -1913,179 +1911,179 @@
       </c>
       <c r="DX6" s="13"/>
     </row>
-    <row r="7" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58" t="s">
+    <row r="7" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="58" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="58" t="s">
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="42" t="s">
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="42" t="s">
+      <c r="O7" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="42" t="s">
+      <c r="P7" s="59" t="s">
         <v>0</v>
       </c>
       <c r="Q7" s="16"/>
-      <c r="R7" s="52" t="s">
+      <c r="R7" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="53"/>
-      <c r="Y7" s="53"/>
-      <c r="Z7" s="53"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="53"/>
-      <c r="AC7" s="53"/>
-      <c r="AD7" s="53"/>
-      <c r="AE7" s="53"/>
-      <c r="AF7" s="53"/>
-      <c r="AG7" s="53"/>
-      <c r="AH7" s="53"/>
-      <c r="AI7" s="53"/>
-      <c r="AJ7" s="53"/>
-      <c r="AK7" s="53"/>
-      <c r="AL7" s="53"/>
-      <c r="AM7" s="54"/>
-      <c r="AN7" s="52" t="s">
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="46"/>
+      <c r="AE7" s="46"/>
+      <c r="AF7" s="46"/>
+      <c r="AG7" s="46"/>
+      <c r="AH7" s="46"/>
+      <c r="AI7" s="46"/>
+      <c r="AJ7" s="46"/>
+      <c r="AK7" s="46"/>
+      <c r="AL7" s="46"/>
+      <c r="AM7" s="47"/>
+      <c r="AN7" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="AO7" s="53"/>
-      <c r="AP7" s="53"/>
-      <c r="AQ7" s="53"/>
-      <c r="AR7" s="53"/>
-      <c r="AS7" s="53"/>
-      <c r="AT7" s="53"/>
-      <c r="AU7" s="53"/>
-      <c r="AV7" s="53"/>
-      <c r="AW7" s="53"/>
-      <c r="AX7" s="53"/>
-      <c r="AY7" s="53"/>
-      <c r="AZ7" s="53"/>
-      <c r="BA7" s="53"/>
-      <c r="BB7" s="53"/>
-      <c r="BC7" s="53"/>
-      <c r="BD7" s="53"/>
-      <c r="BE7" s="53"/>
-      <c r="BF7" s="53"/>
-      <c r="BG7" s="53"/>
-      <c r="BH7" s="53"/>
-      <c r="BI7" s="54"/>
-      <c r="BJ7" s="52" t="s">
+      <c r="AO7" s="46"/>
+      <c r="AP7" s="46"/>
+      <c r="AQ7" s="46"/>
+      <c r="AR7" s="46"/>
+      <c r="AS7" s="46"/>
+      <c r="AT7" s="46"/>
+      <c r="AU7" s="46"/>
+      <c r="AV7" s="46"/>
+      <c r="AW7" s="46"/>
+      <c r="AX7" s="46"/>
+      <c r="AY7" s="46"/>
+      <c r="AZ7" s="46"/>
+      <c r="BA7" s="46"/>
+      <c r="BB7" s="46"/>
+      <c r="BC7" s="46"/>
+      <c r="BD7" s="46"/>
+      <c r="BE7" s="46"/>
+      <c r="BF7" s="46"/>
+      <c r="BG7" s="46"/>
+      <c r="BH7" s="46"/>
+      <c r="BI7" s="47"/>
+      <c r="BJ7" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="BK7" s="53"/>
-      <c r="BL7" s="53"/>
-      <c r="BM7" s="53"/>
-      <c r="BN7" s="53"/>
-      <c r="BO7" s="53"/>
-      <c r="BP7" s="53"/>
-      <c r="BQ7" s="53"/>
-      <c r="BR7" s="53"/>
-      <c r="BS7" s="53"/>
-      <c r="BT7" s="53"/>
-      <c r="BU7" s="53"/>
-      <c r="BV7" s="53"/>
-      <c r="BW7" s="53"/>
-      <c r="BX7" s="53"/>
-      <c r="BY7" s="53"/>
-      <c r="BZ7" s="53"/>
-      <c r="CA7" s="53"/>
-      <c r="CB7" s="53"/>
-      <c r="CC7" s="53"/>
-      <c r="CD7" s="53"/>
-      <c r="CE7" s="54"/>
-      <c r="CF7" s="52" t="s">
+      <c r="BK7" s="46"/>
+      <c r="BL7" s="46"/>
+      <c r="BM7" s="46"/>
+      <c r="BN7" s="46"/>
+      <c r="BO7" s="46"/>
+      <c r="BP7" s="46"/>
+      <c r="BQ7" s="46"/>
+      <c r="BR7" s="46"/>
+      <c r="BS7" s="46"/>
+      <c r="BT7" s="46"/>
+      <c r="BU7" s="46"/>
+      <c r="BV7" s="46"/>
+      <c r="BW7" s="46"/>
+      <c r="BX7" s="46"/>
+      <c r="BY7" s="46"/>
+      <c r="BZ7" s="46"/>
+      <c r="CA7" s="46"/>
+      <c r="CB7" s="46"/>
+      <c r="CC7" s="46"/>
+      <c r="CD7" s="46"/>
+      <c r="CE7" s="47"/>
+      <c r="CF7" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="CG7" s="53"/>
-      <c r="CH7" s="53"/>
-      <c r="CI7" s="53"/>
-      <c r="CJ7" s="53"/>
-      <c r="CK7" s="53"/>
-      <c r="CL7" s="53"/>
-      <c r="CM7" s="53"/>
-      <c r="CN7" s="53"/>
-      <c r="CO7" s="53"/>
-      <c r="CP7" s="53"/>
-      <c r="CQ7" s="53"/>
-      <c r="CR7" s="53"/>
-      <c r="CS7" s="53"/>
-      <c r="CT7" s="53"/>
-      <c r="CU7" s="53"/>
-      <c r="CV7" s="53"/>
-      <c r="CW7" s="53"/>
-      <c r="CX7" s="53"/>
-      <c r="CY7" s="53"/>
-      <c r="CZ7" s="53"/>
-      <c r="DA7" s="54"/>
-      <c r="DB7" s="52" t="s">
+      <c r="CG7" s="46"/>
+      <c r="CH7" s="46"/>
+      <c r="CI7" s="46"/>
+      <c r="CJ7" s="46"/>
+      <c r="CK7" s="46"/>
+      <c r="CL7" s="46"/>
+      <c r="CM7" s="46"/>
+      <c r="CN7" s="46"/>
+      <c r="CO7" s="46"/>
+      <c r="CP7" s="46"/>
+      <c r="CQ7" s="46"/>
+      <c r="CR7" s="46"/>
+      <c r="CS7" s="46"/>
+      <c r="CT7" s="46"/>
+      <c r="CU7" s="46"/>
+      <c r="CV7" s="46"/>
+      <c r="CW7" s="46"/>
+      <c r="CX7" s="46"/>
+      <c r="CY7" s="46"/>
+      <c r="CZ7" s="46"/>
+      <c r="DA7" s="47"/>
+      <c r="DB7" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="DC7" s="53"/>
-      <c r="DD7" s="53"/>
-      <c r="DE7" s="53"/>
-      <c r="DF7" s="53"/>
-      <c r="DG7" s="53"/>
-      <c r="DH7" s="53"/>
-      <c r="DI7" s="53"/>
-      <c r="DJ7" s="53"/>
-      <c r="DK7" s="53"/>
-      <c r="DL7" s="53"/>
-      <c r="DM7" s="53"/>
-      <c r="DN7" s="53"/>
-      <c r="DO7" s="53"/>
-      <c r="DP7" s="53"/>
-      <c r="DQ7" s="53"/>
-      <c r="DR7" s="53"/>
-      <c r="DS7" s="53"/>
-      <c r="DT7" s="53"/>
-      <c r="DU7" s="53"/>
-      <c r="DV7" s="53"/>
-      <c r="DW7" s="54"/>
-      <c r="DX7" s="45" t="s">
+      <c r="DC7" s="46"/>
+      <c r="DD7" s="46"/>
+      <c r="DE7" s="46"/>
+      <c r="DF7" s="46"/>
+      <c r="DG7" s="46"/>
+      <c r="DH7" s="46"/>
+      <c r="DI7" s="46"/>
+      <c r="DJ7" s="46"/>
+      <c r="DK7" s="46"/>
+      <c r="DL7" s="46"/>
+      <c r="DM7" s="46"/>
+      <c r="DN7" s="46"/>
+      <c r="DO7" s="46"/>
+      <c r="DP7" s="46"/>
+      <c r="DQ7" s="46"/>
+      <c r="DR7" s="46"/>
+      <c r="DS7" s="46"/>
+      <c r="DT7" s="46"/>
+      <c r="DU7" s="46"/>
+      <c r="DV7" s="46"/>
+      <c r="DW7" s="47"/>
+      <c r="DX7" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="DY7" s="45"/>
+      <c r="DY7" s="65"/>
       <c r="DZ7" s="11"/>
     </row>
-    <row r="8" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="61"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
+    <row r="8" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="56"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="64"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="4" t="s">
         <v>6</v>
@@ -2417,57 +2415,57 @@
       <c r="DW8" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="DX8" s="46" t="s">
+      <c r="DX8" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="DY8" s="46" t="s">
+      <c r="DY8" s="66" t="s">
         <v>56</v>
       </c>
       <c r="DZ8" s="11"/>
     </row>
-    <row r="9" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+    <row r="9" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="64"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="41" t="s">
         <v>50</v>
@@ -2779,27 +2777,27 @@
       </c>
       <c r="DV9" s="50"/>
       <c r="DW9" s="50"/>
-      <c r="DX9" s="47"/>
-      <c r="DY9" s="47"/>
+      <c r="DX9" s="67"/>
+      <c r="DY9" s="67"/>
       <c r="DZ9" s="11"/>
     </row>
-    <row r="10" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
+    <row r="10" spans="1:130" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="19" t="s">
         <v>53</v>
@@ -3111,11 +3109,11 @@
       </c>
       <c r="DV10" s="51"/>
       <c r="DW10" s="51"/>
-      <c r="DX10" s="48"/>
-      <c r="DY10" s="48"/>
+      <c r="DX10" s="68"/>
+      <c r="DY10" s="68"/>
       <c r="DZ10" s="11"/>
     </row>
-    <row r="11" spans="1:130" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
@@ -3535,24 +3533,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:130" x14ac:dyDescent="0.3">
-      <c r="A12" s="55" t="s">
+    <row r="12" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="57"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="44"/>
       <c r="P12" s="15">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -4007,24 +4005,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:130" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+    <row r="13" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="57"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="44"/>
       <c r="P13" s="15">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4479,24 +4477,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:130" x14ac:dyDescent="0.3">
-      <c r="A14" s="55" t="s">
+    <row r="14" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="57"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="44"/>
       <c r="P14" s="15">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -4951,24 +4949,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:130" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
+      <c r="B15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="P15" s="6" t="s">
         <v>5</v>
       </c>
@@ -5292,24 +5318,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:130" x14ac:dyDescent="0.3">
-      <c r="A16" s="65" t="s">
+    <row r="16" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="65"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
       <c r="P16" s="18">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -5729,7 +5755,7 @@
       <c r="DY16" s="33"/>
       <c r="DZ16" s="35"/>
     </row>
-    <row r="17" spans="1:129" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:129" x14ac:dyDescent="0.25">
       <c r="AL17" s="34"/>
       <c r="AM17" s="34"/>
       <c r="BH17" s="34"/>
@@ -5743,7 +5769,7 @@
       <c r="DX17" s="34"/>
       <c r="DY17" s="34"/>
     </row>
-    <row r="18" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -5751,7 +5777,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -5760,7 +5786,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="20" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -5769,7 +5795,7 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="21" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -5778,7 +5804,7 @@
         <v>ABGELEHNT</v>
       </c>
     </row>
-    <row r="22" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -5787,7 +5813,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="23" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -5796,7 +5822,7 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="24" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -5805,7 +5831,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="25" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -5814,7 +5840,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="26" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -5823,7 +5849,7 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="27" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -5832,7 +5858,7 @@
         <v>ABGELEHNT</v>
       </c>
     </row>
-    <row r="28" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -5841,7 +5867,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="29" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -5850,8 +5876,8 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="30" spans="1:129" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:129" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -5859,7 +5885,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -5867,7 +5893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -5875,7 +5901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -5883,21 +5909,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="55" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="57"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
         <v>1</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="64"/>
+      <c r="C37" s="48"/>
       <c r="D37" s="40"/>
       <c r="E37" s="40"/>
       <c r="F37" s="40"/>
@@ -5909,14 +5935,14 @@
       <c r="L37" s="40"/>
       <c r="M37" s="40"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>2</v>
       </c>
-      <c r="B38" s="64" t="s">
+      <c r="B38" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="64"/>
+      <c r="C38" s="48"/>
       <c r="D38" s="40"/>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
@@ -5928,14 +5954,14 @@
       <c r="L38" s="40"/>
       <c r="M38" s="40"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
         <v>3</v>
       </c>
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="64"/>
+      <c r="C39" s="48"/>
       <c r="D39" s="40"/>
       <c r="E39" s="40"/>
       <c r="F39" s="40"/>
@@ -5949,6 +5975,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="DX7:DY7"/>
+    <mergeCell ref="DX8:DX10"/>
+    <mergeCell ref="DY8:DY10"/>
+    <mergeCell ref="CZ8:CZ10"/>
+    <mergeCell ref="DA8:DA10"/>
+    <mergeCell ref="DV8:DV10"/>
+    <mergeCell ref="DW8:DW10"/>
+    <mergeCell ref="DB7:DW7"/>
+    <mergeCell ref="CF7:DA7"/>
+    <mergeCell ref="D7:H8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I7:M8"/>
+    <mergeCell ref="P7:P10"/>
+    <mergeCell ref="N7:N10"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AN7:BI7"/>
     <mergeCell ref="BJ7:CE7"/>
@@ -5965,35 +6020,6 @@
     <mergeCell ref="A16:O16"/>
     <mergeCell ref="A12:O12"/>
     <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D7:H8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I7:M8"/>
-    <mergeCell ref="P7:P10"/>
-    <mergeCell ref="N7:N10"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="DX7:DY7"/>
-    <mergeCell ref="DX8:DX10"/>
-    <mergeCell ref="DY8:DY10"/>
-    <mergeCell ref="CZ8:CZ10"/>
-    <mergeCell ref="DA8:DA10"/>
-    <mergeCell ref="DV8:DV10"/>
-    <mergeCell ref="DW8:DW10"/>
-    <mergeCell ref="DB7:DW7"/>
-    <mergeCell ref="CF7:DA7"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2298: Anzeige verbessert + FR Text von GUI
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\kibon-app\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45930771-2B1F-46FC-8C15-F42D2E3C9657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2763E8-A8D4-4D8B-96FA-06676B9490D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -780,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -826,7 +826,6 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -879,97 +878,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -979,19 +937,75 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1404,31 +1418,31 @@
   </sheetPr>
   <dimension ref="A1:EC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DZ11" sqref="DZ11"/>
+    <sheetView tabSelected="1" topLeftCell="DK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DZ39" sqref="DZ39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375"/>
-    <col min="3" max="13" width="17.5703125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625"/>
+    <col min="3" max="13" width="17.5546875" style="1" customWidth="1"/>
     <col min="14" max="15" width="17"/>
-    <col min="16" max="16" width="33.140625" customWidth="1"/>
-    <col min="17" max="17" width="33.140625" hidden="1" customWidth="1"/>
-    <col min="18" max="22" width="13.28515625" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" customWidth="1"/>
-    <col min="24" max="37" width="10.5703125"/>
-    <col min="40" max="59" width="10.5703125"/>
-    <col min="62" max="81" width="10.5703125"/>
-    <col min="84" max="103" width="10.5703125"/>
-    <col min="106" max="124" width="10.5703125"/>
-    <col min="125" max="125" width="8.85546875" customWidth="1"/>
-    <col min="128" max="129" width="10.5703125"/>
-    <col min="130" max="130" width="22.7109375" customWidth="1"/>
-    <col min="133" max="989" width="10.5703125"/>
+    <col min="16" max="16" width="33.109375" customWidth="1"/>
+    <col min="17" max="17" width="33.109375" hidden="1" customWidth="1"/>
+    <col min="18" max="22" width="13.33203125" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" customWidth="1"/>
+    <col min="24" max="37" width="10.5546875"/>
+    <col min="40" max="59" width="10.5546875"/>
+    <col min="62" max="81" width="10.5546875"/>
+    <col min="84" max="103" width="10.5546875"/>
+    <col min="106" max="124" width="10.5546875"/>
+    <col min="125" max="125" width="8.88671875" customWidth="1"/>
+    <col min="128" max="129" width="10.5546875"/>
+    <col min="130" max="130" width="22.6640625" customWidth="1"/>
+    <col min="133" max="989" width="10.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:133" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:133" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -1454,7 +1468,7 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:133" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:133" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1480,7 +1494,7 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:133" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:133" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1504,7 +1518,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1528,7 +1542,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:133" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:133" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
         <v>51</v>
       </c>
@@ -1661,7 +1675,7 @@
       <c r="DV5" s="2"/>
       <c r="DW5" s="2"/>
     </row>
-    <row r="6" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
@@ -1975,183 +1989,183 @@
       </c>
       <c r="DX6" s="12"/>
     </row>
-    <row r="7" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
+    <row r="7" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="66" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="66" t="s">
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="63" t="s">
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="63" t="s">
+      <c r="O7" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="63" t="s">
+      <c r="P7" s="59" t="s">
         <v>0</v>
       </c>
       <c r="Q7" s="15"/>
-      <c r="R7" s="57" t="s">
+      <c r="R7" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="58"/>
-      <c r="AB7" s="58"/>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="58"/>
-      <c r="AE7" s="58"/>
-      <c r="AF7" s="58"/>
-      <c r="AG7" s="58"/>
-      <c r="AH7" s="58"/>
-      <c r="AI7" s="58"/>
-      <c r="AJ7" s="58"/>
-      <c r="AK7" s="58"/>
-      <c r="AL7" s="58"/>
-      <c r="AM7" s="59"/>
-      <c r="AN7" s="57" t="s">
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="46"/>
+      <c r="AE7" s="46"/>
+      <c r="AF7" s="46"/>
+      <c r="AG7" s="46"/>
+      <c r="AH7" s="46"/>
+      <c r="AI7" s="46"/>
+      <c r="AJ7" s="46"/>
+      <c r="AK7" s="46"/>
+      <c r="AL7" s="46"/>
+      <c r="AM7" s="47"/>
+      <c r="AN7" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="AO7" s="58"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="58"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="58"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="58"/>
-      <c r="AW7" s="58"/>
-      <c r="AX7" s="58"/>
-      <c r="AY7" s="58"/>
-      <c r="AZ7" s="58"/>
-      <c r="BA7" s="58"/>
-      <c r="BB7" s="58"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="58"/>
-      <c r="BE7" s="58"/>
-      <c r="BF7" s="58"/>
-      <c r="BG7" s="58"/>
-      <c r="BH7" s="58"/>
-      <c r="BI7" s="59"/>
-      <c r="BJ7" s="57" t="s">
+      <c r="AO7" s="46"/>
+      <c r="AP7" s="46"/>
+      <c r="AQ7" s="46"/>
+      <c r="AR7" s="46"/>
+      <c r="AS7" s="46"/>
+      <c r="AT7" s="46"/>
+      <c r="AU7" s="46"/>
+      <c r="AV7" s="46"/>
+      <c r="AW7" s="46"/>
+      <c r="AX7" s="46"/>
+      <c r="AY7" s="46"/>
+      <c r="AZ7" s="46"/>
+      <c r="BA7" s="46"/>
+      <c r="BB7" s="46"/>
+      <c r="BC7" s="46"/>
+      <c r="BD7" s="46"/>
+      <c r="BE7" s="46"/>
+      <c r="BF7" s="46"/>
+      <c r="BG7" s="46"/>
+      <c r="BH7" s="46"/>
+      <c r="BI7" s="47"/>
+      <c r="BJ7" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="BK7" s="58"/>
-      <c r="BL7" s="58"/>
-      <c r="BM7" s="58"/>
-      <c r="BN7" s="58"/>
-      <c r="BO7" s="58"/>
-      <c r="BP7" s="58"/>
-      <c r="BQ7" s="58"/>
-      <c r="BR7" s="58"/>
-      <c r="BS7" s="58"/>
-      <c r="BT7" s="58"/>
-      <c r="BU7" s="58"/>
-      <c r="BV7" s="58"/>
-      <c r="BW7" s="58"/>
-      <c r="BX7" s="58"/>
-      <c r="BY7" s="58"/>
-      <c r="BZ7" s="58"/>
-      <c r="CA7" s="58"/>
-      <c r="CB7" s="58"/>
-      <c r="CC7" s="58"/>
-      <c r="CD7" s="58"/>
-      <c r="CE7" s="59"/>
-      <c r="CF7" s="57" t="s">
+      <c r="BK7" s="46"/>
+      <c r="BL7" s="46"/>
+      <c r="BM7" s="46"/>
+      <c r="BN7" s="46"/>
+      <c r="BO7" s="46"/>
+      <c r="BP7" s="46"/>
+      <c r="BQ7" s="46"/>
+      <c r="BR7" s="46"/>
+      <c r="BS7" s="46"/>
+      <c r="BT7" s="46"/>
+      <c r="BU7" s="46"/>
+      <c r="BV7" s="46"/>
+      <c r="BW7" s="46"/>
+      <c r="BX7" s="46"/>
+      <c r="BY7" s="46"/>
+      <c r="BZ7" s="46"/>
+      <c r="CA7" s="46"/>
+      <c r="CB7" s="46"/>
+      <c r="CC7" s="46"/>
+      <c r="CD7" s="46"/>
+      <c r="CE7" s="47"/>
+      <c r="CF7" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="CG7" s="58"/>
-      <c r="CH7" s="58"/>
-      <c r="CI7" s="58"/>
-      <c r="CJ7" s="58"/>
-      <c r="CK7" s="58"/>
-      <c r="CL7" s="58"/>
-      <c r="CM7" s="58"/>
-      <c r="CN7" s="58"/>
-      <c r="CO7" s="58"/>
-      <c r="CP7" s="58"/>
-      <c r="CQ7" s="58"/>
-      <c r="CR7" s="58"/>
-      <c r="CS7" s="58"/>
-      <c r="CT7" s="58"/>
-      <c r="CU7" s="58"/>
-      <c r="CV7" s="58"/>
-      <c r="CW7" s="58"/>
-      <c r="CX7" s="58"/>
-      <c r="CY7" s="58"/>
-      <c r="CZ7" s="58"/>
-      <c r="DA7" s="59"/>
-      <c r="DB7" s="57" t="s">
+      <c r="CG7" s="46"/>
+      <c r="CH7" s="46"/>
+      <c r="CI7" s="46"/>
+      <c r="CJ7" s="46"/>
+      <c r="CK7" s="46"/>
+      <c r="CL7" s="46"/>
+      <c r="CM7" s="46"/>
+      <c r="CN7" s="46"/>
+      <c r="CO7" s="46"/>
+      <c r="CP7" s="46"/>
+      <c r="CQ7" s="46"/>
+      <c r="CR7" s="46"/>
+      <c r="CS7" s="46"/>
+      <c r="CT7" s="46"/>
+      <c r="CU7" s="46"/>
+      <c r="CV7" s="46"/>
+      <c r="CW7" s="46"/>
+      <c r="CX7" s="46"/>
+      <c r="CY7" s="46"/>
+      <c r="CZ7" s="46"/>
+      <c r="DA7" s="47"/>
+      <c r="DB7" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="DC7" s="58"/>
-      <c r="DD7" s="58"/>
-      <c r="DE7" s="58"/>
-      <c r="DF7" s="58"/>
-      <c r="DG7" s="58"/>
-      <c r="DH7" s="58"/>
-      <c r="DI7" s="58"/>
-      <c r="DJ7" s="58"/>
-      <c r="DK7" s="58"/>
-      <c r="DL7" s="58"/>
-      <c r="DM7" s="58"/>
-      <c r="DN7" s="58"/>
-      <c r="DO7" s="58"/>
-      <c r="DP7" s="58"/>
-      <c r="DQ7" s="58"/>
-      <c r="DR7" s="58"/>
-      <c r="DS7" s="58"/>
-      <c r="DT7" s="58"/>
-      <c r="DU7" s="58"/>
-      <c r="DV7" s="58"/>
-      <c r="DW7" s="59"/>
-      <c r="DX7" s="50" t="s">
+      <c r="DC7" s="46"/>
+      <c r="DD7" s="46"/>
+      <c r="DE7" s="46"/>
+      <c r="DF7" s="46"/>
+      <c r="DG7" s="46"/>
+      <c r="DH7" s="46"/>
+      <c r="DI7" s="46"/>
+      <c r="DJ7" s="46"/>
+      <c r="DK7" s="46"/>
+      <c r="DL7" s="46"/>
+      <c r="DM7" s="46"/>
+      <c r="DN7" s="46"/>
+      <c r="DO7" s="46"/>
+      <c r="DP7" s="46"/>
+      <c r="DQ7" s="46"/>
+      <c r="DR7" s="46"/>
+      <c r="DS7" s="46"/>
+      <c r="DT7" s="46"/>
+      <c r="DU7" s="46"/>
+      <c r="DV7" s="46"/>
+      <c r="DW7" s="47"/>
+      <c r="DX7" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="DY7" s="50"/>
-      <c r="DZ7" s="60" t="s">
+      <c r="DY7" s="71"/>
+      <c r="DZ7" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="EA7" s="44" t="s">
+      <c r="EA7" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="EB7" s="45"/>
+      <c r="EB7" s="66"/>
       <c r="EC7" s="11"/>
     </row>
-    <row r="8" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="77"/>
+    <row r="8" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="56"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63"/>
       <c r="N8" s="64"/>
       <c r="O8" s="64"/>
       <c r="P8" s="64"/>
@@ -2216,10 +2230,10 @@
       <c r="AK8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AL8" s="54" t="s">
+      <c r="AL8" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="AM8" s="54" t="s">
+      <c r="AM8" s="49" t="s">
         <v>49</v>
       </c>
       <c r="AN8" s="4" t="s">
@@ -2282,10 +2296,10 @@
       <c r="BG8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BH8" s="54" t="s">
+      <c r="BH8" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="BI8" s="54" t="s">
+      <c r="BI8" s="49" t="s">
         <v>49</v>
       </c>
       <c r="BJ8" s="4" t="s">
@@ -2348,10 +2362,10 @@
       <c r="CC8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CD8" s="54" t="s">
+      <c r="CD8" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="CE8" s="54" t="s">
+      <c r="CE8" s="49" t="s">
         <v>49</v>
       </c>
       <c r="CF8" s="4" t="s">
@@ -2414,10 +2428,10 @@
       <c r="CY8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CZ8" s="54" t="s">
+      <c r="CZ8" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="DA8" s="54" t="s">
+      <c r="DA8" s="49" t="s">
         <v>49</v>
       </c>
       <c r="DB8" s="4" t="s">
@@ -2480,401 +2494,401 @@
       <c r="DU8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DV8" s="54" t="s">
+      <c r="DV8" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="DW8" s="54" t="s">
+      <c r="DW8" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="DX8" s="51" t="s">
+      <c r="DX8" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="DY8" s="51" t="s">
+      <c r="DY8" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="DZ8" s="61"/>
-      <c r="EA8" s="46"/>
-      <c r="EB8" s="47"/>
-      <c r="EC8" s="40"/>
+      <c r="DZ8" s="76"/>
+      <c r="EA8" s="67"/>
+      <c r="EB8" s="68"/>
+      <c r="EC8" s="39"/>
     </row>
-    <row r="9" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+    <row r="9" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="63" t="s">
+      <c r="F9" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="63" t="s">
+      <c r="I9" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="63" t="s">
+      <c r="J9" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="63" t="s">
+      <c r="K9" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="L9" s="63" t="s">
+      <c r="L9" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="63" t="s">
+      <c r="M9" s="59" t="s">
         <v>76</v>
       </c>
       <c r="N9" s="64"/>
       <c r="O9" s="64"/>
       <c r="P9" s="64"/>
       <c r="Q9" s="16"/>
-      <c r="R9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="S9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="T9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="U9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="V9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="W9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="X9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL9" s="55"/>
-      <c r="AM9" s="55"/>
-      <c r="AN9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AO9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AT9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AU9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AW9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AX9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BB9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BC9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BE9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BF9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BG9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BH9" s="55"/>
-      <c r="BI9" s="55"/>
-      <c r="BJ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BL9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BO9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BP9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BQ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BR9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BS9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BT9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BU9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BV9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BW9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BX9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BY9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="BZ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CA9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CB9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CC9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CD9" s="55"/>
-      <c r="CE9" s="55"/>
-      <c r="CF9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CG9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CH9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CI9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CJ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CK9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CL9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CM9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CN9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CO9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CP9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CQ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CR9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CS9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CT9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CU9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CV9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CW9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CX9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CY9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="CZ9" s="55"/>
-      <c r="DA9" s="55"/>
-      <c r="DB9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DC9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DD9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DE9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DF9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DG9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DH9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DI9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DJ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DK9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DL9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DM9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DN9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DO9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DP9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DQ9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DR9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DS9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DT9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DU9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="DV9" s="55"/>
-      <c r="DW9" s="55"/>
-      <c r="DX9" s="52"/>
-      <c r="DY9" s="52"/>
-      <c r="DZ9" s="61"/>
-      <c r="EA9" s="46"/>
-      <c r="EB9" s="47"/>
-      <c r="EC9" s="40"/>
+      <c r="R9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="V9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="W9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL9" s="50"/>
+      <c r="AM9" s="50"/>
+      <c r="AN9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AV9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BC9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BG9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BH9" s="50"/>
+      <c r="BI9" s="50"/>
+      <c r="BJ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BM9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BN9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BO9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BP9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BQ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BR9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BS9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BT9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BV9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BW9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BX9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BY9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BZ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CA9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CB9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CC9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CD9" s="50"/>
+      <c r="CE9" s="50"/>
+      <c r="CF9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CG9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CH9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CI9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CJ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CK9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CL9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CM9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CN9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CO9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CP9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CQ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CR9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CS9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CT9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CU9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CV9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CW9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CX9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CY9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="CZ9" s="50"/>
+      <c r="DA9" s="50"/>
+      <c r="DB9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DC9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DD9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DE9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DF9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DG9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DH9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DI9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DJ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DK9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DL9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DM9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DN9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DO9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DP9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DQ9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DR9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DS9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DT9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DU9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="DV9" s="50"/>
+      <c r="DW9" s="50"/>
+      <c r="DX9" s="73"/>
+      <c r="DY9" s="73"/>
+      <c r="DZ9" s="76"/>
+      <c r="EA9" s="67"/>
+      <c r="EB9" s="68"/>
+      <c r="EC9" s="39"/>
     </row>
-    <row r="10" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
+    <row r="10" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="18" t="s">
         <v>53</v>
@@ -2936,8 +2950,8 @@
       <c r="AK10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AL10" s="56"/>
-      <c r="AM10" s="56"/>
+      <c r="AL10" s="51"/>
+      <c r="AM10" s="51"/>
       <c r="AN10" s="18" t="s">
         <v>53</v>
       </c>
@@ -2998,8 +3012,8 @@
       <c r="BG10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BH10" s="56"/>
-      <c r="BI10" s="56"/>
+      <c r="BH10" s="51"/>
+      <c r="BI10" s="51"/>
       <c r="BJ10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3060,8 +3074,8 @@
       <c r="CC10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CD10" s="56"/>
-      <c r="CE10" s="56"/>
+      <c r="CD10" s="51"/>
+      <c r="CE10" s="51"/>
       <c r="CF10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3122,8 +3136,8 @@
       <c r="CY10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CZ10" s="56"/>
-      <c r="DA10" s="56"/>
+      <c r="CZ10" s="51"/>
+      <c r="DA10" s="51"/>
       <c r="DB10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3184,16 +3198,16 @@
       <c r="DU10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="DV10" s="56"/>
-      <c r="DW10" s="56"/>
-      <c r="DX10" s="53"/>
-      <c r="DY10" s="53"/>
-      <c r="DZ10" s="62"/>
-      <c r="EA10" s="48"/>
-      <c r="EB10" s="49"/>
-      <c r="EC10" s="40"/>
+      <c r="DV10" s="51"/>
+      <c r="DW10" s="51"/>
+      <c r="DX10" s="74"/>
+      <c r="DY10" s="74"/>
+      <c r="DZ10" s="77"/>
+      <c r="EA10" s="69"/>
+      <c r="EB10" s="70"/>
+      <c r="EC10" s="39"/>
     </row>
-    <row r="11" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
@@ -3246,398 +3260,398 @@
         <f>VLOOKUP(P11,$A$18:$B$29,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="R11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="S11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="T11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="U11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="V11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="W11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="X11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL11" s="35">
+      <c r="R11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="U11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="V11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="W11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="X11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL11" s="34">
         <f>SUMIF(R11:AK11,1,R$9:AK$9)
 +SUMIF(R11:AK11,2,R$9:AK$9)*0.5
 +SUMIF(R11:AK11,3,R$9:AK$9)</f>
         <v>0</v>
       </c>
-      <c r="AM11" s="24">
+      <c r="AM11" s="23">
         <f>SUMIF(R11:AK11,1,R$10:AK$10)
 +SUMIF(R11:AK11,2,R$10:AK$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="AN11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AP11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AQ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AW11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="AZ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BA11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BB11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BC11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BD11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BE11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BF11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BG11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BH11" s="35">
+      <c r="AN11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AQ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BC11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BD11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BE11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BG11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH11" s="34">
         <f>SUMIF(AN11:BG11,1,AN$9:BG$9)
 +SUMIF(AN11:BG11,2,AN$9:BG$9)*0.5
 +SUMIF(AN11:BG11,3,AN$9:BG$9)</f>
         <v>0</v>
       </c>
-      <c r="BI11" s="24">
+      <c r="BI11" s="23">
         <f>SUMIF(AN11:BG11,1,AN$10:BG$10)
 +SUMIF(AN11:BG11,2,AN$10:BG$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="BJ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BK11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BL11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BM11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BN11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BO11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BP11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BQ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BR11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BS11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BT11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BU11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BV11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BW11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BX11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BY11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BZ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CA11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CB11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CC11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CD11" s="35">
+      <c r="BJ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BK11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BL11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BN11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BP11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BQ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BS11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BT11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BU11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BV11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BX11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BY11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="BZ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CA11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CB11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CC11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CD11" s="34">
         <f>SUMIF(BJ11:CC11,1,BJ$9:CC$9)
 +SUMIF(BJ11:CC11,2,BJ$9:CC$9)*0.5
 +SUMIF(BJ11:CC11,3,BJ$9:CC$9)</f>
         <v>0</v>
       </c>
-      <c r="CE11" s="24">
+      <c r="CE11" s="23">
         <f>SUMIF(BJ11:CC11,1,BJ$10:CC$10)
 +SUMIF(BJ11:CC11,2,BJ$10:CC$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="CF11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CG11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CH11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CI11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CJ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CK11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CL11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CM11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CN11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CO11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CP11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CQ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CR11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CS11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CT11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CU11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CV11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CW11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CX11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CY11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="CZ11" s="35">
+      <c r="CF11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CG11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CH11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CI11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CJ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CK11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CL11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CM11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CN11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CO11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CP11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CQ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CR11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CS11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CT11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CU11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CV11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CW11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CX11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CY11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="CZ11" s="34">
         <f>SUMIF(CF11:CY11,1,CF$9:CY$9)
 +SUMIF(CF11:CY11,2,CF$9:CY$9)*0.5
 +SUMIF(CF11:CY11,3,CF$9:CY$9)</f>
         <v>0</v>
       </c>
-      <c r="DA11" s="24">
+      <c r="DA11" s="23">
         <f>SUMIF(CF11:CY11,1,CF$10:CY$10)
 +SUMIF(CF11:CY11,2,CF$10:CY$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="DB11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DC11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DD11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DE11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DF11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DG11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DH11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DI11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DJ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DK11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DL11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DM11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DN11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DO11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DP11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DQ11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DR11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DS11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DT11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DU11" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="DV11" s="35">
+      <c r="DB11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DC11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DD11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DE11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DF11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DG11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DH11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DI11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DJ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DK11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DL11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DM11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DN11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DO11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DP11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DQ11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DR11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DS11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DT11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DU11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="DV11" s="34">
         <f>SUMIF(DB11:DU11,1,DB$9:DU$9)
 +SUMIF(DB11:DU11,2,DB$9:DU$9)*0.5
 +SUMIF(DB11:DU11,3,DB$9:DU$9)</f>
         <v>0</v>
       </c>
-      <c r="DW11" s="24">
+      <c r="DW11" s="23">
         <f>SUMIF(DB11:DU11,1,DB$10:DU$10)
 +SUMIF(DB11:DU11,2,DB$10:DU$10)*0.5</f>
         <v>0</v>
       </c>
-      <c r="DX11" s="35">
+      <c r="DX11" s="34">
         <f>SUM(DV11,AL11,BH11,CD11,CZ11)</f>
         <v>0</v>
       </c>
-      <c r="DY11" s="25">
+      <c r="DY11" s="24">
         <f>SUM(DW11,AM11,BI11,CE11,DA11)</f>
         <v>0</v>
       </c>
-      <c r="DZ11" s="82" t="s">
+      <c r="DZ11" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="EA11" s="78" t="s">
+      <c r="EA11" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="EB11" s="79"/>
-      <c r="EC11" s="41" t="s">
+      <c r="EB11" s="87"/>
+      <c r="EC11" s="40" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
+    <row r="12" spans="1:133" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="74"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="44"/>
       <c r="P12" s="14">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -3723,11 +3737,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AL12" s="36">
+      <c r="AL12" s="35">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="AM12" s="22">
+      <c r="AM12" s="21">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3811,11 +3825,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="BH12" s="36">
+      <c r="BH12" s="35">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="BI12" s="22">
+      <c r="BI12" s="21">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3899,11 +3913,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CD12" s="36">
+      <c r="CD12" s="35">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CE12" s="22">
+      <c r="CE12" s="21">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -3987,11 +4001,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="CZ12" s="36">
+      <c r="CZ12" s="35">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DA12" s="22">
+      <c r="DA12" s="21">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
@@ -4075,41 +4089,44 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DV12" s="36">
+      <c r="DV12" s="35">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DW12" s="22">
+      <c r="DW12" s="21">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DX12" s="36">
+      <c r="DX12" s="35">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DY12" s="21">
+      <c r="DY12" s="82">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
+      <c r="DZ12" s="90"/>
+      <c r="EA12" s="80"/>
+      <c r="EB12" s="81"/>
     </row>
-    <row r="13" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A13" s="72" t="s">
+    <row r="13" spans="1:133" x14ac:dyDescent="0.3">
+      <c r="A13" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="74"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="44"/>
       <c r="P13" s="14">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4195,11 +4212,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AL13" s="36">
+      <c r="AL13" s="35">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="AM13" s="22">
+      <c r="AM13" s="21">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4283,11 +4300,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="BH13" s="36">
+      <c r="BH13" s="35">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="BI13" s="22">
+      <c r="BI13" s="21">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4371,11 +4388,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CD13" s="36">
+      <c r="CD13" s="35">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CE13" s="22">
+      <c r="CE13" s="21">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4459,11 +4476,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="CZ13" s="36">
+      <c r="CZ13" s="35">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DA13" s="22">
+      <c r="DA13" s="21">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
@@ -4547,41 +4564,44 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DV13" s="36">
+      <c r="DV13" s="35">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DW13" s="22">
+      <c r="DW13" s="21">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DX13" s="36">
+      <c r="DX13" s="35">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DY13" s="22">
+      <c r="DY13" s="83">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
+      <c r="DZ13" s="91"/>
+      <c r="EA13" s="31"/>
+      <c r="EB13" s="89"/>
     </row>
-    <row r="14" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A14" s="72" t="s">
+    <row r="14" spans="1:133" x14ac:dyDescent="0.3">
+      <c r="A14" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
-      <c r="O14" s="74"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="44"/>
       <c r="P14" s="14">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -4667,11 +4687,11 @@
         <f>COUNTIFS(angemeldet20,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AL14" s="37">
+      <c r="AL14" s="36">
         <f>SUMIFS(summeStundenMo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="AM14" s="27">
+      <c r="AM14" s="26">
         <f>SUMIFS(summeVerpflegungMo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4755,11 +4775,11 @@
         <f>COUNTIFS(angemeldet40,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="BH14" s="37">
+      <c r="BH14" s="36">
         <f>SUMIFS(summeStundenDi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="BI14" s="27">
+      <c r="BI14" s="26">
         <f>SUMIFS(summeVerpflegungDi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4843,11 +4863,11 @@
         <f>COUNTIFS(angemeldet60,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CD14" s="37">
+      <c r="CD14" s="36">
         <f>SUMIFS(summeStundenMi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CE14" s="27">
+      <c r="CE14" s="26">
         <f>SUMIFS(summeVerpflegungMi,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -4931,11 +4951,11 @@
         <f>COUNTIFS(angemeldet80,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="CZ14" s="37">
+      <c r="CZ14" s="36">
         <f>SUMIFS(summeStundenDo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DA14" s="27">
+      <c r="DA14" s="26">
         <f>SUMIFS(summeVerpflegungDo,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
@@ -5019,24 +5039,27 @@
         <f>COUNTIFS(angemeldet100,"&gt;0",statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DV14" s="37">
+      <c r="DV14" s="36">
         <f>SUMIFS(summeStundenFr,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DW14" s="27">
+      <c r="DW14" s="26">
         <f>SUMIFS(summeVerpflegungFr,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DX14" s="37">
+      <c r="DX14" s="36">
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DY14" s="27">
+      <c r="DY14" s="84">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
+      <c r="DZ14" s="92"/>
+      <c r="EA14" s="79"/>
+      <c r="EB14" s="41"/>
     </row>
-    <row r="15" spans="1:133" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:133" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
@@ -5118,12 +5141,12 @@
       <c r="AJ15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AK15" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL15" s="30"/>
-      <c r="AM15" s="31"/>
-      <c r="AN15" s="28" t="s">
+      <c r="AK15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL15" s="29"/>
+      <c r="AM15" s="30"/>
+      <c r="AN15" s="27" t="s">
         <v>8</v>
       </c>
       <c r="AO15" s="9" t="s">
@@ -5180,12 +5203,12 @@
       <c r="BF15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="BG15" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="BH15" s="30"/>
-      <c r="BI15" s="31"/>
-      <c r="BJ15" s="28" t="s">
+      <c r="BG15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH15" s="29"/>
+      <c r="BI15" s="30"/>
+      <c r="BJ15" s="27" t="s">
         <v>8</v>
       </c>
       <c r="BK15" s="9" t="s">
@@ -5242,12 +5265,12 @@
       <c r="CB15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="CC15" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="CD15" s="30"/>
-      <c r="CE15" s="31"/>
-      <c r="CF15" s="28" t="s">
+      <c r="CC15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="CD15" s="29"/>
+      <c r="CE15" s="30"/>
+      <c r="CF15" s="27" t="s">
         <v>8</v>
       </c>
       <c r="CG15" s="9" t="s">
@@ -5304,12 +5327,12 @@
       <c r="CX15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="CY15" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="CZ15" s="30"/>
-      <c r="DA15" s="31"/>
-      <c r="DB15" s="28" t="s">
+      <c r="CY15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="CZ15" s="29"/>
+      <c r="DA15" s="30"/>
+      <c r="DB15" s="27" t="s">
         <v>8</v>
       </c>
       <c r="DC15" s="9" t="s">
@@ -5366,35 +5389,38 @@
       <c r="DT15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="DU15" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="DV15" s="30"/>
-      <c r="DW15" s="31"/>
-      <c r="DX15" s="34"/>
-      <c r="DY15" s="42"/>
+      <c r="DU15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="DV15" s="29"/>
+      <c r="DW15" s="30"/>
+      <c r="DX15" s="33"/>
+      <c r="DY15" s="78"/>
+      <c r="DZ15" s="88"/>
+      <c r="EA15" s="31"/>
+      <c r="EB15" s="89"/>
       <c r="EC15" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A16" s="81" t="s">
+    <row r="16" spans="1:133" x14ac:dyDescent="0.3">
+      <c r="A16" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
       <c r="P16" s="17">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -5480,8 +5506,8 @@
         <f>COUNTIF(nichtFreigegeben20,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="AL16" s="32"/>
-      <c r="AM16" s="32"/>
+      <c r="AL16" s="31"/>
+      <c r="AM16" s="31"/>
       <c r="AN16" s="14">
         <f>COUNTIF(nichtFreigegeben21,"&gt;0")</f>
         <v>0</v>
@@ -5562,8 +5588,8 @@
         <f>COUNTIF(nichtFreigegeben40,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="BH16" s="32"/>
-      <c r="BI16" s="32"/>
+      <c r="BH16" s="31"/>
+      <c r="BI16" s="31"/>
       <c r="BJ16" s="14">
         <f>COUNTIF(nichtFreigegeben41,"&gt;0")</f>
         <v>0</v>
@@ -5644,8 +5670,8 @@
         <f>COUNTIF(nichtFreigegeben60,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="CD16" s="32"/>
-      <c r="CE16" s="32"/>
+      <c r="CD16" s="31"/>
+      <c r="CE16" s="31"/>
       <c r="CF16" s="14">
         <f>COUNTIF(nichtFreigegeben61,"&gt;0")</f>
         <v>0</v>
@@ -5726,8 +5752,8 @@
         <f>COUNTIF(nichtFreigegeben80,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="CZ16" s="32"/>
-      <c r="DA16" s="32"/>
+      <c r="CZ16" s="31"/>
+      <c r="DA16" s="31"/>
       <c r="DB16" s="14">
         <f>COUNTIF(nichtFreigegeben81,"&gt;0")</f>
         <v>0</v>
@@ -5808,30 +5834,33 @@
         <f>COUNTIF(nichtFreigegeben100,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="DV16" s="32"/>
-      <c r="DW16" s="32"/>
-      <c r="DX16" s="29"/>
-      <c r="DY16" s="43"/>
+      <c r="DV16" s="31"/>
+      <c r="DW16" s="31"/>
+      <c r="DX16" s="28"/>
+      <c r="DY16" s="79"/>
+      <c r="DZ16" s="28"/>
+      <c r="EA16" s="79"/>
+      <c r="EB16" s="41"/>
       <c r="EC16" s="12"/>
     </row>
-    <row r="17" spans="1:132" x14ac:dyDescent="0.25">
-      <c r="AL17" s="33"/>
-      <c r="AM17" s="33"/>
-      <c r="BH17" s="33"/>
-      <c r="BI17" s="33"/>
-      <c r="CD17" s="33"/>
-      <c r="CE17" s="33"/>
-      <c r="CZ17" s="33"/>
-      <c r="DA17" s="33"/>
-      <c r="DV17" s="33"/>
-      <c r="DW17" s="33"/>
-      <c r="DX17" s="33"/>
-      <c r="DY17" s="33"/>
+    <row r="17" spans="1:132" x14ac:dyDescent="0.3">
+      <c r="AL17" s="32"/>
+      <c r="AM17" s="32"/>
+      <c r="BH17" s="32"/>
+      <c r="BI17" s="32"/>
+      <c r="CD17" s="32"/>
+      <c r="CE17" s="32"/>
+      <c r="CZ17" s="32"/>
+      <c r="DA17" s="32"/>
+      <c r="DV17" s="32"/>
+      <c r="DW17" s="32"/>
+      <c r="DX17" s="32"/>
+      <c r="DY17" s="32"/>
       <c r="DZ17" s="12"/>
       <c r="EA17" s="12"/>
       <c r="EB17" s="12"/>
     </row>
-    <row r="18" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -5839,7 +5868,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -5848,7 +5877,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="20" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -5857,7 +5886,7 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="21" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -5866,7 +5895,7 @@
         <v>ABGELEHNT</v>
       </c>
     </row>
-    <row r="22" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -5875,7 +5904,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="23" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -5884,7 +5913,7 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="24" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -5893,7 +5922,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="25" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:132" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -5902,7 +5931,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="26" spans="1:132" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -5911,7 +5940,7 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="27" spans="1:132" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -5920,7 +5949,7 @@
         <v>ABGELEHNT</v>
       </c>
     </row>
-    <row r="28" spans="1:132" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -5929,7 +5958,7 @@
         <v>OFFEN</v>
       </c>
     </row>
-    <row r="29" spans="1:132" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -5938,8 +5967,8 @@
         <v>BESTÄTIGT</v>
       </c>
     </row>
-    <row r="30" spans="1:132" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:132" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:132" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -5947,7 +5976,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:132" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -5955,7 +5984,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -5963,7 +5992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -5971,72 +6000,104 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="72" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="73"/>
-      <c r="C36" s="74"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="26">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="25">
         <v>1</v>
       </c>
-      <c r="B37" s="80" t="s">
+      <c r="B37" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="80"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="26">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="25">
         <v>2</v>
       </c>
-      <c r="B38" s="80" t="s">
+      <c r="B38" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="80"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="26">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="25">
         <v>3</v>
       </c>
-      <c r="B39" s="80" t="s">
+      <c r="B39" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="80"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="38"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="EA7:EB10"/>
+    <mergeCell ref="DX7:DY7"/>
+    <mergeCell ref="DX8:DX10"/>
+    <mergeCell ref="DY8:DY10"/>
+    <mergeCell ref="CZ8:CZ10"/>
+    <mergeCell ref="DA8:DA10"/>
+    <mergeCell ref="DV8:DV10"/>
+    <mergeCell ref="DW8:DW10"/>
+    <mergeCell ref="DB7:DW7"/>
+    <mergeCell ref="CF7:DA7"/>
+    <mergeCell ref="DZ7:DZ10"/>
+    <mergeCell ref="P7:P10"/>
+    <mergeCell ref="N7:N10"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="D7:H8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I7:M8"/>
     <mergeCell ref="EA11:EB11"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AN7:BI7"/>
@@ -6053,38 +6114,6 @@
     <mergeCell ref="R7:AM7"/>
     <mergeCell ref="A16:O16"/>
     <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D7:H8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I7:M8"/>
-    <mergeCell ref="P7:P10"/>
-    <mergeCell ref="N7:N10"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="EA7:EB10"/>
-    <mergeCell ref="DX7:DY7"/>
-    <mergeCell ref="DX8:DX10"/>
-    <mergeCell ref="DY8:DY10"/>
-    <mergeCell ref="CZ8:CZ10"/>
-    <mergeCell ref="DA8:DA10"/>
-    <mergeCell ref="DV8:DV10"/>
-    <mergeCell ref="DW8:DW10"/>
-    <mergeCell ref="DB7:DW7"/>
-    <mergeCell ref="CF7:DA7"/>
-    <mergeCell ref="DZ7:DZ10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2376 add missing placeholders to excel after merge
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2763E8-A8D4-4D8B-96FA-06676B9490D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD0CF41-C4A5-4467-9CCF-81496F66B1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="85">
   <si>
     <t>{statusTitle}</t>
   </si>
@@ -879,106 +879,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -995,17 +895,117 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1418,9 +1418,7 @@
   </sheetPr>
   <dimension ref="A1:EC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DZ39" sqref="DZ39"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1990,185 +1988,185 @@
       <c r="DX6" s="12"/>
     </row>
     <row r="7" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="53" t="s">
+      <c r="B7" s="78"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="53" t="s">
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="59" t="s">
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="59" t="s">
+      <c r="O7" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="59" t="s">
+      <c r="P7" s="74" t="s">
         <v>0</v>
       </c>
       <c r="Q7" s="15"/>
-      <c r="R7" s="45" t="s">
+      <c r="R7" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="46"/>
-      <c r="T7" s="46"/>
-      <c r="U7" s="46"/>
-      <c r="V7" s="46"/>
-      <c r="W7" s="46"/>
-      <c r="X7" s="46"/>
-      <c r="Y7" s="46"/>
-      <c r="Z7" s="46"/>
-      <c r="AA7" s="46"/>
-      <c r="AB7" s="46"/>
-      <c r="AC7" s="46"/>
-      <c r="AD7" s="46"/>
-      <c r="AE7" s="46"/>
-      <c r="AF7" s="46"/>
-      <c r="AG7" s="46"/>
-      <c r="AH7" s="46"/>
-      <c r="AI7" s="46"/>
-      <c r="AJ7" s="46"/>
-      <c r="AK7" s="46"/>
-      <c r="AL7" s="46"/>
-      <c r="AM7" s="47"/>
-      <c r="AN7" s="45" t="s">
+      <c r="S7" s="69"/>
+      <c r="T7" s="69"/>
+      <c r="U7" s="69"/>
+      <c r="V7" s="69"/>
+      <c r="W7" s="69"/>
+      <c r="X7" s="69"/>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
+      <c r="AH7" s="69"/>
+      <c r="AI7" s="69"/>
+      <c r="AJ7" s="69"/>
+      <c r="AK7" s="69"/>
+      <c r="AL7" s="69"/>
+      <c r="AM7" s="70"/>
+      <c r="AN7" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="AO7" s="46"/>
-      <c r="AP7" s="46"/>
-      <c r="AQ7" s="46"/>
-      <c r="AR7" s="46"/>
-      <c r="AS7" s="46"/>
-      <c r="AT7" s="46"/>
-      <c r="AU7" s="46"/>
-      <c r="AV7" s="46"/>
-      <c r="AW7" s="46"/>
-      <c r="AX7" s="46"/>
-      <c r="AY7" s="46"/>
-      <c r="AZ7" s="46"/>
-      <c r="BA7" s="46"/>
-      <c r="BB7" s="46"/>
-      <c r="BC7" s="46"/>
-      <c r="BD7" s="46"/>
-      <c r="BE7" s="46"/>
-      <c r="BF7" s="46"/>
-      <c r="BG7" s="46"/>
-      <c r="BH7" s="46"/>
-      <c r="BI7" s="47"/>
-      <c r="BJ7" s="45" t="s">
+      <c r="AO7" s="69"/>
+      <c r="AP7" s="69"/>
+      <c r="AQ7" s="69"/>
+      <c r="AR7" s="69"/>
+      <c r="AS7" s="69"/>
+      <c r="AT7" s="69"/>
+      <c r="AU7" s="69"/>
+      <c r="AV7" s="69"/>
+      <c r="AW7" s="69"/>
+      <c r="AX7" s="69"/>
+      <c r="AY7" s="69"/>
+      <c r="AZ7" s="69"/>
+      <c r="BA7" s="69"/>
+      <c r="BB7" s="69"/>
+      <c r="BC7" s="69"/>
+      <c r="BD7" s="69"/>
+      <c r="BE7" s="69"/>
+      <c r="BF7" s="69"/>
+      <c r="BG7" s="69"/>
+      <c r="BH7" s="69"/>
+      <c r="BI7" s="70"/>
+      <c r="BJ7" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="BK7" s="46"/>
-      <c r="BL7" s="46"/>
-      <c r="BM7" s="46"/>
-      <c r="BN7" s="46"/>
-      <c r="BO7" s="46"/>
-      <c r="BP7" s="46"/>
-      <c r="BQ7" s="46"/>
-      <c r="BR7" s="46"/>
-      <c r="BS7" s="46"/>
-      <c r="BT7" s="46"/>
-      <c r="BU7" s="46"/>
-      <c r="BV7" s="46"/>
-      <c r="BW7" s="46"/>
-      <c r="BX7" s="46"/>
-      <c r="BY7" s="46"/>
-      <c r="BZ7" s="46"/>
-      <c r="CA7" s="46"/>
-      <c r="CB7" s="46"/>
-      <c r="CC7" s="46"/>
-      <c r="CD7" s="46"/>
-      <c r="CE7" s="47"/>
-      <c r="CF7" s="45" t="s">
+      <c r="BK7" s="69"/>
+      <c r="BL7" s="69"/>
+      <c r="BM7" s="69"/>
+      <c r="BN7" s="69"/>
+      <c r="BO7" s="69"/>
+      <c r="BP7" s="69"/>
+      <c r="BQ7" s="69"/>
+      <c r="BR7" s="69"/>
+      <c r="BS7" s="69"/>
+      <c r="BT7" s="69"/>
+      <c r="BU7" s="69"/>
+      <c r="BV7" s="69"/>
+      <c r="BW7" s="69"/>
+      <c r="BX7" s="69"/>
+      <c r="BY7" s="69"/>
+      <c r="BZ7" s="69"/>
+      <c r="CA7" s="69"/>
+      <c r="CB7" s="69"/>
+      <c r="CC7" s="69"/>
+      <c r="CD7" s="69"/>
+      <c r="CE7" s="70"/>
+      <c r="CF7" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="CG7" s="46"/>
-      <c r="CH7" s="46"/>
-      <c r="CI7" s="46"/>
-      <c r="CJ7" s="46"/>
-      <c r="CK7" s="46"/>
-      <c r="CL7" s="46"/>
-      <c r="CM7" s="46"/>
-      <c r="CN7" s="46"/>
-      <c r="CO7" s="46"/>
-      <c r="CP7" s="46"/>
-      <c r="CQ7" s="46"/>
-      <c r="CR7" s="46"/>
-      <c r="CS7" s="46"/>
-      <c r="CT7" s="46"/>
-      <c r="CU7" s="46"/>
-      <c r="CV7" s="46"/>
-      <c r="CW7" s="46"/>
-      <c r="CX7" s="46"/>
-      <c r="CY7" s="46"/>
-      <c r="CZ7" s="46"/>
-      <c r="DA7" s="47"/>
-      <c r="DB7" s="45" t="s">
+      <c r="CG7" s="69"/>
+      <c r="CH7" s="69"/>
+      <c r="CI7" s="69"/>
+      <c r="CJ7" s="69"/>
+      <c r="CK7" s="69"/>
+      <c r="CL7" s="69"/>
+      <c r="CM7" s="69"/>
+      <c r="CN7" s="69"/>
+      <c r="CO7" s="69"/>
+      <c r="CP7" s="69"/>
+      <c r="CQ7" s="69"/>
+      <c r="CR7" s="69"/>
+      <c r="CS7" s="69"/>
+      <c r="CT7" s="69"/>
+      <c r="CU7" s="69"/>
+      <c r="CV7" s="69"/>
+      <c r="CW7" s="69"/>
+      <c r="CX7" s="69"/>
+      <c r="CY7" s="69"/>
+      <c r="CZ7" s="69"/>
+      <c r="DA7" s="70"/>
+      <c r="DB7" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="DC7" s="46"/>
-      <c r="DD7" s="46"/>
-      <c r="DE7" s="46"/>
-      <c r="DF7" s="46"/>
-      <c r="DG7" s="46"/>
-      <c r="DH7" s="46"/>
-      <c r="DI7" s="46"/>
-      <c r="DJ7" s="46"/>
-      <c r="DK7" s="46"/>
-      <c r="DL7" s="46"/>
-      <c r="DM7" s="46"/>
-      <c r="DN7" s="46"/>
-      <c r="DO7" s="46"/>
-      <c r="DP7" s="46"/>
-      <c r="DQ7" s="46"/>
-      <c r="DR7" s="46"/>
-      <c r="DS7" s="46"/>
-      <c r="DT7" s="46"/>
-      <c r="DU7" s="46"/>
-      <c r="DV7" s="46"/>
-      <c r="DW7" s="47"/>
-      <c r="DX7" s="71" t="s">
+      <c r="DC7" s="69"/>
+      <c r="DD7" s="69"/>
+      <c r="DE7" s="69"/>
+      <c r="DF7" s="69"/>
+      <c r="DG7" s="69"/>
+      <c r="DH7" s="69"/>
+      <c r="DI7" s="69"/>
+      <c r="DJ7" s="69"/>
+      <c r="DK7" s="69"/>
+      <c r="DL7" s="69"/>
+      <c r="DM7" s="69"/>
+      <c r="DN7" s="69"/>
+      <c r="DO7" s="69"/>
+      <c r="DP7" s="69"/>
+      <c r="DQ7" s="69"/>
+      <c r="DR7" s="69"/>
+      <c r="DS7" s="69"/>
+      <c r="DT7" s="69"/>
+      <c r="DU7" s="69"/>
+      <c r="DV7" s="69"/>
+      <c r="DW7" s="70"/>
+      <c r="DX7" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="DY7" s="71"/>
-      <c r="DZ7" s="75" t="s">
+      <c r="DY7" s="61"/>
+      <c r="DZ7" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="EA7" s="65" t="s">
+      <c r="EA7" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="EB7" s="66"/>
+      <c r="EB7" s="56"/>
       <c r="EC7" s="11"/>
     </row>
     <row r="8" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="4" t="s">
         <v>6</v>
@@ -2230,10 +2228,10 @@
       <c r="AK8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AL8" s="49" t="s">
+      <c r="AL8" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="AM8" s="49" t="s">
+      <c r="AM8" s="65" t="s">
         <v>49</v>
       </c>
       <c r="AN8" s="4" t="s">
@@ -2296,10 +2294,10 @@
       <c r="BG8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BH8" s="49" t="s">
+      <c r="BH8" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="BI8" s="49" t="s">
+      <c r="BI8" s="65" t="s">
         <v>49</v>
       </c>
       <c r="BJ8" s="4" t="s">
@@ -2362,10 +2360,10 @@
       <c r="CC8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CD8" s="49" t="s">
+      <c r="CD8" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="CE8" s="49" t="s">
+      <c r="CE8" s="65" t="s">
         <v>49</v>
       </c>
       <c r="CF8" s="4" t="s">
@@ -2428,10 +2426,10 @@
       <c r="CY8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CZ8" s="49" t="s">
+      <c r="CZ8" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="DA8" s="49" t="s">
+      <c r="DA8" s="65" t="s">
         <v>49</v>
       </c>
       <c r="DB8" s="4" t="s">
@@ -2494,66 +2492,66 @@
       <c r="DU8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DV8" s="49" t="s">
+      <c r="DV8" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="DW8" s="49" t="s">
+      <c r="DW8" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="DX8" s="72" t="s">
+      <c r="DX8" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="DY8" s="72" t="s">
+      <c r="DY8" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="DZ8" s="76"/>
-      <c r="EA8" s="67"/>
-      <c r="EB8" s="68"/>
+      <c r="DZ8" s="72"/>
+      <c r="EA8" s="57"/>
+      <c r="EB8" s="58"/>
       <c r="EC8" s="39"/>
     </row>
     <row r="9" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="59" t="s">
+      <c r="K9" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="L9" s="59" t="s">
+      <c r="L9" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="59" t="s">
+      <c r="M9" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="38" t="s">
         <v>50</v>
@@ -2615,8 +2613,8 @@
       <c r="AK9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AL9" s="50"/>
-      <c r="AM9" s="50"/>
+      <c r="AL9" s="66"/>
+      <c r="AM9" s="66"/>
       <c r="AN9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2677,8 +2675,8 @@
       <c r="BG9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="BH9" s="50"/>
-      <c r="BI9" s="50"/>
+      <c r="BH9" s="66"/>
+      <c r="BI9" s="66"/>
       <c r="BJ9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2739,8 +2737,8 @@
       <c r="CC9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="CD9" s="50"/>
-      <c r="CE9" s="50"/>
+      <c r="CD9" s="66"/>
+      <c r="CE9" s="66"/>
       <c r="CF9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2801,8 +2799,8 @@
       <c r="CY9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="CZ9" s="50"/>
-      <c r="DA9" s="50"/>
+      <c r="CZ9" s="66"/>
+      <c r="DA9" s="66"/>
       <c r="DB9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2863,32 +2861,32 @@
       <c r="DU9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="DV9" s="50"/>
-      <c r="DW9" s="50"/>
-      <c r="DX9" s="73"/>
-      <c r="DY9" s="73"/>
-      <c r="DZ9" s="76"/>
-      <c r="EA9" s="67"/>
-      <c r="EB9" s="68"/>
+      <c r="DV9" s="66"/>
+      <c r="DW9" s="66"/>
+      <c r="DX9" s="63"/>
+      <c r="DY9" s="63"/>
+      <c r="DZ9" s="72"/>
+      <c r="EA9" s="57"/>
+      <c r="EB9" s="58"/>
       <c r="EC9" s="39"/>
     </row>
     <row r="10" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="18" t="s">
         <v>53</v>
@@ -2950,8 +2948,8 @@
       <c r="AK10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AL10" s="51"/>
-      <c r="AM10" s="51"/>
+      <c r="AL10" s="67"/>
+      <c r="AM10" s="67"/>
       <c r="AN10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3012,8 +3010,8 @@
       <c r="BG10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BH10" s="51"/>
-      <c r="BI10" s="51"/>
+      <c r="BH10" s="67"/>
+      <c r="BI10" s="67"/>
       <c r="BJ10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3074,8 +3072,8 @@
       <c r="CC10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CD10" s="51"/>
-      <c r="CE10" s="51"/>
+      <c r="CD10" s="67"/>
+      <c r="CE10" s="67"/>
       <c r="CF10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3136,8 +3134,8 @@
       <c r="CY10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CZ10" s="51"/>
-      <c r="DA10" s="51"/>
+      <c r="CZ10" s="67"/>
+      <c r="DA10" s="67"/>
       <c r="DB10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3198,13 +3196,13 @@
       <c r="DU10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="DV10" s="51"/>
-      <c r="DW10" s="51"/>
-      <c r="DX10" s="74"/>
-      <c r="DY10" s="74"/>
-      <c r="DZ10" s="77"/>
-      <c r="EA10" s="69"/>
-      <c r="EB10" s="70"/>
+      <c r="DV10" s="67"/>
+      <c r="DW10" s="67"/>
+      <c r="DX10" s="64"/>
+      <c r="DY10" s="64"/>
+      <c r="DZ10" s="73"/>
+      <c r="EA10" s="59"/>
+      <c r="EB10" s="60"/>
       <c r="EC10" s="39"/>
     </row>
     <row r="11" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3623,35 +3621,35 @@
         <f>SUM(DW11,AM11,BI11,CE11,DA11)</f>
         <v>0</v>
       </c>
-      <c r="DZ11" s="85" t="s">
+      <c r="DZ11" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="EA11" s="86" t="s">
+      <c r="EA11" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="EB11" s="87"/>
+      <c r="EB11" s="90"/>
       <c r="EC11" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="44"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="84"/>
+      <c r="L12" s="84"/>
+      <c r="M12" s="84"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="85"/>
       <c r="P12" s="14">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -4101,32 +4099,32 @@
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DY12" s="82">
+      <c r="DY12" s="46">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DZ12" s="90"/>
-      <c r="EA12" s="80"/>
-      <c r="EB12" s="81"/>
+      <c r="DZ12" s="52"/>
+      <c r="EA12" s="44"/>
+      <c r="EB12" s="45"/>
     </row>
     <row r="13" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="44"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="84"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="84"/>
+      <c r="N13" s="84"/>
+      <c r="O13" s="85"/>
       <c r="P13" s="14">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4576,32 +4574,32 @@
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DY13" s="83">
+      <c r="DY13" s="47">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DZ13" s="91"/>
+      <c r="DZ13" s="53"/>
       <c r="EA13" s="31"/>
-      <c r="EB13" s="89"/>
+      <c r="EB13" s="51"/>
     </row>
     <row r="14" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="44"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="84"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="85"/>
       <c r="P14" s="14">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -5051,32 +5049,60 @@
         <f>SUMIFS(summeStundenWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DY14" s="84">
+      <c r="DY14" s="48">
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DZ14" s="92"/>
-      <c r="EA14" s="79"/>
+      <c r="DZ14" s="54"/>
+      <c r="EA14" s="43"/>
       <c r="EB14" s="41"/>
     </row>
     <row r="15" spans="1:133" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
+      <c r="B15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="P15" s="6" t="s">
         <v>5</v>
       </c>
@@ -5395,32 +5421,32 @@
       <c r="DV15" s="29"/>
       <c r="DW15" s="30"/>
       <c r="DX15" s="33"/>
-      <c r="DY15" s="78"/>
-      <c r="DZ15" s="88"/>
+      <c r="DY15" s="42"/>
+      <c r="DZ15" s="50"/>
       <c r="EA15" s="31"/>
-      <c r="EB15" s="89"/>
+      <c r="EB15" s="51"/>
       <c r="EC15" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="92"/>
       <c r="P16" s="17">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -5837,9 +5863,9 @@
       <c r="DV16" s="31"/>
       <c r="DW16" s="31"/>
       <c r="DX16" s="28"/>
-      <c r="DY16" s="79"/>
+      <c r="DY16" s="43"/>
       <c r="DZ16" s="28"/>
-      <c r="EA16" s="79"/>
+      <c r="EA16" s="43"/>
       <c r="EB16" s="41"/>
       <c r="EC16" s="12"/>
     </row>
@@ -6001,20 +6027,20 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="85"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="25">
         <v>1</v>
       </c>
-      <c r="B37" s="48" t="s">
+      <c r="B37" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="48"/>
+      <c r="C37" s="91"/>
       <c r="D37" s="37"/>
       <c r="E37" s="37"/>
       <c r="F37" s="37"/>
@@ -6030,10 +6056,10 @@
       <c r="A38" s="25">
         <v>2</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="48"/>
+      <c r="C38" s="91"/>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
@@ -6049,10 +6075,10 @@
       <c r="A39" s="25">
         <v>3</v>
       </c>
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="48"/>
+      <c r="C39" s="91"/>
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
       <c r="F39" s="37"/>
@@ -6066,38 +6092,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="EA7:EB10"/>
-    <mergeCell ref="DX7:DY7"/>
-    <mergeCell ref="DX8:DX10"/>
-    <mergeCell ref="DY8:DY10"/>
-    <mergeCell ref="CZ8:CZ10"/>
-    <mergeCell ref="DA8:DA10"/>
-    <mergeCell ref="DV8:DV10"/>
-    <mergeCell ref="DW8:DW10"/>
-    <mergeCell ref="DB7:DW7"/>
-    <mergeCell ref="CF7:DA7"/>
-    <mergeCell ref="DZ7:DZ10"/>
-    <mergeCell ref="P7:P10"/>
-    <mergeCell ref="N7:N10"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D7:H8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I7:M8"/>
     <mergeCell ref="EA11:EB11"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AN7:BI7"/>
@@ -6114,6 +6108,38 @@
     <mergeCell ref="R7:AM7"/>
     <mergeCell ref="A16:O16"/>
     <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="D7:H8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I7:M8"/>
+    <mergeCell ref="P7:P10"/>
+    <mergeCell ref="N7:N10"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="EA7:EB10"/>
+    <mergeCell ref="DX7:DY7"/>
+    <mergeCell ref="DX8:DX10"/>
+    <mergeCell ref="DY8:DY10"/>
+    <mergeCell ref="CZ8:CZ10"/>
+    <mergeCell ref="DA8:DA10"/>
+    <mergeCell ref="DV8:DV10"/>
+    <mergeCell ref="DW8:DW10"/>
+    <mergeCell ref="DB7:DW7"/>
+    <mergeCell ref="CF7:DA7"/>
+    <mergeCell ref="DZ7:DZ10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2376: Fix Anzeigen Problemen + add Bemerkung und Abweichung zu die noch nicht freigegebene Antraege
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD0CF41-C4A5-4467-9CCF-81496F66B1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20978E70-159E-49D5-BE05-634FEB8EBA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="85">
   <si>
     <t>{statusTitle}</t>
   </si>
@@ -780,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -892,101 +892,65 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -996,16 +960,57 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1418,7 +1423,9 @@
   </sheetPr>
   <dimension ref="A1:EC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="DK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DZ37" sqref="DZ37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1434,7 +1441,7 @@
     <col min="62" max="81" width="10.5546875"/>
     <col min="84" max="103" width="10.5546875"/>
     <col min="106" max="124" width="10.5546875"/>
-    <col min="125" max="125" width="8.88671875" customWidth="1"/>
+    <col min="125" max="125" width="10" customWidth="1"/>
     <col min="128" max="129" width="10.5546875"/>
     <col min="130" max="130" width="22.6640625" customWidth="1"/>
     <col min="133" max="989" width="10.5546875"/>
@@ -1988,185 +1995,185 @@
       <c r="DX6" s="12"/>
     </row>
     <row r="7" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="77" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="77" t="s">
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="74" t="s">
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="74" t="s">
+      <c r="O7" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="74" t="s">
+      <c r="P7" s="72" t="s">
         <v>0</v>
       </c>
       <c r="Q7" s="15"/>
-      <c r="R7" s="68" t="s">
+      <c r="R7" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
-      <c r="W7" s="69"/>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="69"/>
-      <c r="AG7" s="69"/>
-      <c r="AH7" s="69"/>
-      <c r="AI7" s="69"/>
-      <c r="AJ7" s="69"/>
-      <c r="AK7" s="69"/>
-      <c r="AL7" s="69"/>
-      <c r="AM7" s="70"/>
-      <c r="AN7" s="68" t="s">
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="59"/>
+      <c r="AC7" s="59"/>
+      <c r="AD7" s="59"/>
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="59"/>
+      <c r="AG7" s="59"/>
+      <c r="AH7" s="59"/>
+      <c r="AI7" s="59"/>
+      <c r="AJ7" s="59"/>
+      <c r="AK7" s="59"/>
+      <c r="AL7" s="59"/>
+      <c r="AM7" s="60"/>
+      <c r="AN7" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="AO7" s="69"/>
-      <c r="AP7" s="69"/>
-      <c r="AQ7" s="69"/>
-      <c r="AR7" s="69"/>
-      <c r="AS7" s="69"/>
-      <c r="AT7" s="69"/>
-      <c r="AU7" s="69"/>
-      <c r="AV7" s="69"/>
-      <c r="AW7" s="69"/>
-      <c r="AX7" s="69"/>
-      <c r="AY7" s="69"/>
-      <c r="AZ7" s="69"/>
-      <c r="BA7" s="69"/>
-      <c r="BB7" s="69"/>
-      <c r="BC7" s="69"/>
-      <c r="BD7" s="69"/>
-      <c r="BE7" s="69"/>
-      <c r="BF7" s="69"/>
-      <c r="BG7" s="69"/>
-      <c r="BH7" s="69"/>
-      <c r="BI7" s="70"/>
-      <c r="BJ7" s="68" t="s">
+      <c r="AO7" s="59"/>
+      <c r="AP7" s="59"/>
+      <c r="AQ7" s="59"/>
+      <c r="AR7" s="59"/>
+      <c r="AS7" s="59"/>
+      <c r="AT7" s="59"/>
+      <c r="AU7" s="59"/>
+      <c r="AV7" s="59"/>
+      <c r="AW7" s="59"/>
+      <c r="AX7" s="59"/>
+      <c r="AY7" s="59"/>
+      <c r="AZ7" s="59"/>
+      <c r="BA7" s="59"/>
+      <c r="BB7" s="59"/>
+      <c r="BC7" s="59"/>
+      <c r="BD7" s="59"/>
+      <c r="BE7" s="59"/>
+      <c r="BF7" s="59"/>
+      <c r="BG7" s="59"/>
+      <c r="BH7" s="59"/>
+      <c r="BI7" s="60"/>
+      <c r="BJ7" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="BK7" s="69"/>
-      <c r="BL7" s="69"/>
-      <c r="BM7" s="69"/>
-      <c r="BN7" s="69"/>
-      <c r="BO7" s="69"/>
-      <c r="BP7" s="69"/>
-      <c r="BQ7" s="69"/>
-      <c r="BR7" s="69"/>
-      <c r="BS7" s="69"/>
-      <c r="BT7" s="69"/>
-      <c r="BU7" s="69"/>
-      <c r="BV7" s="69"/>
-      <c r="BW7" s="69"/>
-      <c r="BX7" s="69"/>
-      <c r="BY7" s="69"/>
-      <c r="BZ7" s="69"/>
-      <c r="CA7" s="69"/>
-      <c r="CB7" s="69"/>
-      <c r="CC7" s="69"/>
-      <c r="CD7" s="69"/>
-      <c r="CE7" s="70"/>
-      <c r="CF7" s="68" t="s">
+      <c r="BK7" s="59"/>
+      <c r="BL7" s="59"/>
+      <c r="BM7" s="59"/>
+      <c r="BN7" s="59"/>
+      <c r="BO7" s="59"/>
+      <c r="BP7" s="59"/>
+      <c r="BQ7" s="59"/>
+      <c r="BR7" s="59"/>
+      <c r="BS7" s="59"/>
+      <c r="BT7" s="59"/>
+      <c r="BU7" s="59"/>
+      <c r="BV7" s="59"/>
+      <c r="BW7" s="59"/>
+      <c r="BX7" s="59"/>
+      <c r="BY7" s="59"/>
+      <c r="BZ7" s="59"/>
+      <c r="CA7" s="59"/>
+      <c r="CB7" s="59"/>
+      <c r="CC7" s="59"/>
+      <c r="CD7" s="59"/>
+      <c r="CE7" s="60"/>
+      <c r="CF7" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="CG7" s="69"/>
-      <c r="CH7" s="69"/>
-      <c r="CI7" s="69"/>
-      <c r="CJ7" s="69"/>
-      <c r="CK7" s="69"/>
-      <c r="CL7" s="69"/>
-      <c r="CM7" s="69"/>
-      <c r="CN7" s="69"/>
-      <c r="CO7" s="69"/>
-      <c r="CP7" s="69"/>
-      <c r="CQ7" s="69"/>
-      <c r="CR7" s="69"/>
-      <c r="CS7" s="69"/>
-      <c r="CT7" s="69"/>
-      <c r="CU7" s="69"/>
-      <c r="CV7" s="69"/>
-      <c r="CW7" s="69"/>
-      <c r="CX7" s="69"/>
-      <c r="CY7" s="69"/>
-      <c r="CZ7" s="69"/>
-      <c r="DA7" s="70"/>
-      <c r="DB7" s="68" t="s">
+      <c r="CG7" s="59"/>
+      <c r="CH7" s="59"/>
+      <c r="CI7" s="59"/>
+      <c r="CJ7" s="59"/>
+      <c r="CK7" s="59"/>
+      <c r="CL7" s="59"/>
+      <c r="CM7" s="59"/>
+      <c r="CN7" s="59"/>
+      <c r="CO7" s="59"/>
+      <c r="CP7" s="59"/>
+      <c r="CQ7" s="59"/>
+      <c r="CR7" s="59"/>
+      <c r="CS7" s="59"/>
+      <c r="CT7" s="59"/>
+      <c r="CU7" s="59"/>
+      <c r="CV7" s="59"/>
+      <c r="CW7" s="59"/>
+      <c r="CX7" s="59"/>
+      <c r="CY7" s="59"/>
+      <c r="CZ7" s="59"/>
+      <c r="DA7" s="60"/>
+      <c r="DB7" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="DC7" s="69"/>
-      <c r="DD7" s="69"/>
-      <c r="DE7" s="69"/>
-      <c r="DF7" s="69"/>
-      <c r="DG7" s="69"/>
-      <c r="DH7" s="69"/>
-      <c r="DI7" s="69"/>
-      <c r="DJ7" s="69"/>
-      <c r="DK7" s="69"/>
-      <c r="DL7" s="69"/>
-      <c r="DM7" s="69"/>
-      <c r="DN7" s="69"/>
-      <c r="DO7" s="69"/>
-      <c r="DP7" s="69"/>
-      <c r="DQ7" s="69"/>
-      <c r="DR7" s="69"/>
-      <c r="DS7" s="69"/>
-      <c r="DT7" s="69"/>
-      <c r="DU7" s="69"/>
-      <c r="DV7" s="69"/>
-      <c r="DW7" s="70"/>
-      <c r="DX7" s="61" t="s">
+      <c r="DC7" s="59"/>
+      <c r="DD7" s="59"/>
+      <c r="DE7" s="59"/>
+      <c r="DF7" s="59"/>
+      <c r="DG7" s="59"/>
+      <c r="DH7" s="59"/>
+      <c r="DI7" s="59"/>
+      <c r="DJ7" s="59"/>
+      <c r="DK7" s="59"/>
+      <c r="DL7" s="59"/>
+      <c r="DM7" s="59"/>
+      <c r="DN7" s="59"/>
+      <c r="DO7" s="59"/>
+      <c r="DP7" s="59"/>
+      <c r="DQ7" s="59"/>
+      <c r="DR7" s="59"/>
+      <c r="DS7" s="59"/>
+      <c r="DT7" s="59"/>
+      <c r="DU7" s="59"/>
+      <c r="DV7" s="59"/>
+      <c r="DW7" s="60"/>
+      <c r="DX7" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="DY7" s="61"/>
-      <c r="DZ7" s="71" t="s">
+      <c r="DY7" s="84"/>
+      <c r="DZ7" s="88" t="s">
         <v>83</v>
       </c>
-      <c r="EA7" s="55" t="s">
+      <c r="EA7" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="EB7" s="56"/>
+      <c r="EB7" s="79"/>
       <c r="EC7" s="11"/>
     </row>
     <row r="8" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="4" t="s">
         <v>6</v>
@@ -2228,10 +2235,10 @@
       <c r="AK8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AL8" s="65" t="s">
+      <c r="AL8" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="AM8" s="65" t="s">
+      <c r="AM8" s="62" t="s">
         <v>49</v>
       </c>
       <c r="AN8" s="4" t="s">
@@ -2294,10 +2301,10 @@
       <c r="BG8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BH8" s="65" t="s">
+      <c r="BH8" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="BI8" s="65" t="s">
+      <c r="BI8" s="62" t="s">
         <v>49</v>
       </c>
       <c r="BJ8" s="4" t="s">
@@ -2360,10 +2367,10 @@
       <c r="CC8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CD8" s="65" t="s">
+      <c r="CD8" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="CE8" s="65" t="s">
+      <c r="CE8" s="62" t="s">
         <v>49</v>
       </c>
       <c r="CF8" s="4" t="s">
@@ -2426,10 +2433,10 @@
       <c r="CY8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CZ8" s="65" t="s">
+      <c r="CZ8" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="DA8" s="65" t="s">
+      <c r="DA8" s="62" t="s">
         <v>49</v>
       </c>
       <c r="DB8" s="4" t="s">
@@ -2492,66 +2499,66 @@
       <c r="DU8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DV8" s="65" t="s">
+      <c r="DV8" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="DW8" s="65" t="s">
+      <c r="DW8" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="DX8" s="62" t="s">
+      <c r="DX8" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="DY8" s="62" t="s">
+      <c r="DY8" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="DZ8" s="72"/>
-      <c r="EA8" s="57"/>
-      <c r="EB8" s="58"/>
+      <c r="DZ8" s="89"/>
+      <c r="EA8" s="80"/>
+      <c r="EB8" s="81"/>
       <c r="EC8" s="39"/>
     </row>
     <row r="9" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="74" t="s">
+      <c r="E9" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="74" t="s">
+      <c r="F9" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="74" t="s">
+      <c r="G9" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="74" t="s">
+      <c r="H9" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="74" t="s">
+      <c r="I9" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="74" t="s">
+      <c r="J9" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="74" t="s">
+      <c r="K9" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="L9" s="74" t="s">
+      <c r="L9" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="74" t="s">
+      <c r="M9" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="38" t="s">
         <v>50</v>
@@ -2613,8 +2620,8 @@
       <c r="AK9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AL9" s="66"/>
-      <c r="AM9" s="66"/>
+      <c r="AL9" s="63"/>
+      <c r="AM9" s="63"/>
       <c r="AN9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2675,8 +2682,8 @@
       <c r="BG9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="BH9" s="66"/>
-      <c r="BI9" s="66"/>
+      <c r="BH9" s="63"/>
+      <c r="BI9" s="63"/>
       <c r="BJ9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2737,8 +2744,8 @@
       <c r="CC9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="CD9" s="66"/>
-      <c r="CE9" s="66"/>
+      <c r="CD9" s="63"/>
+      <c r="CE9" s="63"/>
       <c r="CF9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2799,8 +2806,8 @@
       <c r="CY9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="CZ9" s="66"/>
-      <c r="DA9" s="66"/>
+      <c r="CZ9" s="63"/>
+      <c r="DA9" s="63"/>
       <c r="DB9" s="38" t="s">
         <v>50</v>
       </c>
@@ -2861,32 +2868,32 @@
       <c r="DU9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="DV9" s="66"/>
-      <c r="DW9" s="66"/>
-      <c r="DX9" s="63"/>
-      <c r="DY9" s="63"/>
-      <c r="DZ9" s="72"/>
-      <c r="EA9" s="57"/>
-      <c r="EB9" s="58"/>
+      <c r="DV9" s="63"/>
+      <c r="DW9" s="63"/>
+      <c r="DX9" s="86"/>
+      <c r="DY9" s="86"/>
+      <c r="DZ9" s="89"/>
+      <c r="EA9" s="80"/>
+      <c r="EB9" s="81"/>
       <c r="EC9" s="39"/>
     </row>
     <row r="10" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="18" t="s">
         <v>53</v>
@@ -2948,8 +2955,8 @@
       <c r="AK10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AL10" s="67"/>
-      <c r="AM10" s="67"/>
+      <c r="AL10" s="64"/>
+      <c r="AM10" s="64"/>
       <c r="AN10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3010,8 +3017,8 @@
       <c r="BG10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BH10" s="67"/>
-      <c r="BI10" s="67"/>
+      <c r="BH10" s="64"/>
+      <c r="BI10" s="64"/>
       <c r="BJ10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3072,8 +3079,8 @@
       <c r="CC10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CD10" s="67"/>
-      <c r="CE10" s="67"/>
+      <c r="CD10" s="64"/>
+      <c r="CE10" s="64"/>
       <c r="CF10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3134,8 +3141,8 @@
       <c r="CY10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CZ10" s="67"/>
-      <c r="DA10" s="67"/>
+      <c r="CZ10" s="64"/>
+      <c r="DA10" s="64"/>
       <c r="DB10" s="18" t="s">
         <v>53</v>
       </c>
@@ -3196,13 +3203,13 @@
       <c r="DU10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="DV10" s="67"/>
-      <c r="DW10" s="67"/>
-      <c r="DX10" s="64"/>
-      <c r="DY10" s="64"/>
-      <c r="DZ10" s="73"/>
-      <c r="EA10" s="59"/>
-      <c r="EB10" s="60"/>
+      <c r="DV10" s="64"/>
+      <c r="DW10" s="64"/>
+      <c r="DX10" s="87"/>
+      <c r="DY10" s="87"/>
+      <c r="DZ10" s="90"/>
+      <c r="EA10" s="82"/>
+      <c r="EB10" s="83"/>
       <c r="EC10" s="39"/>
     </row>
     <row r="11" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3621,35 +3628,35 @@
         <f>SUM(DW11,AM11,BI11,CE11,DA11)</f>
         <v>0</v>
       </c>
-      <c r="DZ11" s="49" t="s">
+      <c r="DZ11" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="EA11" s="89" t="s">
+      <c r="EA11" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="EB11" s="90"/>
+      <c r="EB11" s="54"/>
       <c r="EC11" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="84"/>
-      <c r="M12" s="84"/>
-      <c r="N12" s="84"/>
-      <c r="O12" s="85"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="57"/>
       <c r="P12" s="14">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -4103,28 +4110,28 @@
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="DZ12" s="52"/>
+      <c r="DZ12" s="50"/>
       <c r="EA12" s="44"/>
       <c r="EB12" s="45"/>
     </row>
     <row r="13" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="84"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="84"/>
-      <c r="O13" s="85"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="57"/>
       <c r="P13" s="14">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4578,28 +4585,28 @@
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="DZ13" s="53"/>
+      <c r="DZ13" s="51"/>
       <c r="EA13" s="31"/>
-      <c r="EB13" s="51"/>
+      <c r="EB13" s="49"/>
     </row>
     <row r="14" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A14" s="83" t="s">
+      <c r="A14" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="84"/>
-      <c r="O14" s="85"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="57"/>
       <c r="P14" s="14">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -5053,7 +5060,7 @@
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="DZ14" s="54"/>
+      <c r="DZ14" s="52"/>
       <c r="EA14" s="43"/>
       <c r="EB14" s="41"/>
     </row>
@@ -5422,31 +5429,35 @@
       <c r="DW15" s="30"/>
       <c r="DX15" s="33"/>
       <c r="DY15" s="42"/>
-      <c r="DZ15" s="50"/>
-      <c r="EA15" s="31"/>
-      <c r="EB15" s="51"/>
+      <c r="DZ15" s="91" t="s">
+        <v>84</v>
+      </c>
+      <c r="EA15" s="92" t="s">
+        <v>81</v>
+      </c>
+      <c r="EB15" s="93"/>
       <c r="EC15" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="92"/>
-      <c r="O16" s="92"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="65"/>
+      <c r="O16" s="65"/>
       <c r="P16" s="17">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -6027,20 +6038,20 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="83" t="s">
+      <c r="A36" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="84"/>
-      <c r="C36" s="85"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="57"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="25">
         <v>1</v>
       </c>
-      <c r="B37" s="91" t="s">
+      <c r="B37" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="91"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="37"/>
       <c r="E37" s="37"/>
       <c r="F37" s="37"/>
@@ -6056,10 +6067,10 @@
       <c r="A38" s="25">
         <v>2</v>
       </c>
-      <c r="B38" s="91" t="s">
+      <c r="B38" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="91"/>
+      <c r="C38" s="61"/>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
@@ -6075,10 +6086,10 @@
       <c r="A39" s="25">
         <v>3</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="91"/>
+      <c r="C39" s="61"/>
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
       <c r="F39" s="37"/>
@@ -6091,7 +6102,40 @@
       <c r="M39" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="49">
+    <mergeCell ref="EA15:EB15"/>
+    <mergeCell ref="EA7:EB10"/>
+    <mergeCell ref="DX7:DY7"/>
+    <mergeCell ref="DX8:DX10"/>
+    <mergeCell ref="DY8:DY10"/>
+    <mergeCell ref="CZ8:CZ10"/>
+    <mergeCell ref="DA8:DA10"/>
+    <mergeCell ref="DV8:DV10"/>
+    <mergeCell ref="DW8:DW10"/>
+    <mergeCell ref="DB7:DW7"/>
+    <mergeCell ref="CF7:DA7"/>
+    <mergeCell ref="DZ7:DZ10"/>
+    <mergeCell ref="P7:P10"/>
+    <mergeCell ref="N7:N10"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="D7:H8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I7:M8"/>
     <mergeCell ref="EA11:EB11"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AN7:BI7"/>
@@ -6108,38 +6152,6 @@
     <mergeCell ref="R7:AM7"/>
     <mergeCell ref="A16:O16"/>
     <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D7:H8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I7:M8"/>
-    <mergeCell ref="P7:P10"/>
-    <mergeCell ref="N7:N10"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="EA7:EB10"/>
-    <mergeCell ref="DX7:DY7"/>
-    <mergeCell ref="DX8:DX10"/>
-    <mergeCell ref="DY8:DY10"/>
-    <mergeCell ref="CZ8:CZ10"/>
-    <mergeCell ref="DA8:DA10"/>
-    <mergeCell ref="DV8:DV10"/>
-    <mergeCell ref="DW8:DW10"/>
-    <mergeCell ref="DB7:DW7"/>
-    <mergeCell ref="CF7:DA7"/>
-    <mergeCell ref="DZ7:DZ10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2658: Vergessene Platzholder und Uebersetzungen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BCCECC-3605-4B49-BE33-B8400F60B2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DB0543-E4FB-4DE3-82C9-F7D17D90E4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,15 +313,6 @@
     <t>{repeatCol5}</t>
   </si>
   <si>
-    <t>Anzahl bestätigte Anmeldungen</t>
-  </si>
-  <si>
-    <t>Anzahl abgelehnte Anmeldungen</t>
-  </si>
-  <si>
-    <t>Anzahl offene Anmeldungen</t>
-  </si>
-  <si>
     <t>In Bearbeitung</t>
   </si>
   <si>
@@ -374,9 +365,6 @@
   </si>
   <si>
     <t>BESTÄTIGT</t>
-  </si>
-  <si>
-    <t>Anzahl nicht freigegebene Anmeldungen</t>
   </si>
   <si>
     <t>{wochentagDi}</t>
@@ -517,6 +505,18 @@
   </si>
   <si>
     <t>{isAbweichung}</t>
+  </si>
+  <si>
+    <t>{anzahlBestaetigteAnmeldungen}</t>
+  </si>
+  <si>
+    <t>{anzahlAbgelehnteAnmeldungen}</t>
+  </si>
+  <si>
+    <t>{anzahlOffeneAnmeldungen}</t>
+  </si>
+  <si>
+    <t>{anzahlNichtFreigegebeneAnmeldungen}</t>
   </si>
 </sst>
 </file>
@@ -780,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -888,6 +888,66 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -916,30 +976,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -948,49 +984,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1404,7 +1403,7 @@
   <dimension ref="A1:EC39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A16" sqref="A16:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1429,7 +1428,7 @@
   <sheetData>
     <row r="1" spans="1:133" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1529,10 +1528,10 @@
     </row>
     <row r="5" spans="1:133" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1974,185 +1973,185 @@
       </c>
     </row>
     <row r="7" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="69" t="s">
+      <c r="A7" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="P7" s="69" t="s">
+      <c r="O7" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7" s="65" t="s">
         <v>0</v>
       </c>
       <c r="Q7" s="14"/>
-      <c r="R7" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="64"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-      <c r="AC7" s="64"/>
-      <c r="AD7" s="64"/>
-      <c r="AE7" s="64"/>
-      <c r="AF7" s="64"/>
-      <c r="AG7" s="64"/>
-      <c r="AH7" s="64"/>
-      <c r="AI7" s="64"/>
-      <c r="AJ7" s="64"/>
-      <c r="AK7" s="64"/>
-      <c r="AL7" s="64"/>
-      <c r="AM7" s="65"/>
-      <c r="AN7" s="63" t="s">
+      <c r="R7" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="53"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
+      <c r="X7" s="53"/>
+      <c r="Y7" s="53"/>
+      <c r="Z7" s="53"/>
+      <c r="AA7" s="53"/>
+      <c r="AB7" s="53"/>
+      <c r="AC7" s="53"/>
+      <c r="AD7" s="53"/>
+      <c r="AE7" s="53"/>
+      <c r="AF7" s="53"/>
+      <c r="AG7" s="53"/>
+      <c r="AH7" s="53"/>
+      <c r="AI7" s="53"/>
+      <c r="AJ7" s="53"/>
+      <c r="AK7" s="53"/>
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="54"/>
+      <c r="AN7" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO7" s="53"/>
+      <c r="AP7" s="53"/>
+      <c r="AQ7" s="53"/>
+      <c r="AR7" s="53"/>
+      <c r="AS7" s="53"/>
+      <c r="AT7" s="53"/>
+      <c r="AU7" s="53"/>
+      <c r="AV7" s="53"/>
+      <c r="AW7" s="53"/>
+      <c r="AX7" s="53"/>
+      <c r="AY7" s="53"/>
+      <c r="AZ7" s="53"/>
+      <c r="BA7" s="53"/>
+      <c r="BB7" s="53"/>
+      <c r="BC7" s="53"/>
+      <c r="BD7" s="53"/>
+      <c r="BE7" s="53"/>
+      <c r="BF7" s="53"/>
+      <c r="BG7" s="53"/>
+      <c r="BH7" s="53"/>
+      <c r="BI7" s="54"/>
+      <c r="BJ7" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="BK7" s="53"/>
+      <c r="BL7" s="53"/>
+      <c r="BM7" s="53"/>
+      <c r="BN7" s="53"/>
+      <c r="BO7" s="53"/>
+      <c r="BP7" s="53"/>
+      <c r="BQ7" s="53"/>
+      <c r="BR7" s="53"/>
+      <c r="BS7" s="53"/>
+      <c r="BT7" s="53"/>
+      <c r="BU7" s="53"/>
+      <c r="BV7" s="53"/>
+      <c r="BW7" s="53"/>
+      <c r="BX7" s="53"/>
+      <c r="BY7" s="53"/>
+      <c r="BZ7" s="53"/>
+      <c r="CA7" s="53"/>
+      <c r="CB7" s="53"/>
+      <c r="CC7" s="53"/>
+      <c r="CD7" s="53"/>
+      <c r="CE7" s="54"/>
+      <c r="CF7" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="CG7" s="53"/>
+      <c r="CH7" s="53"/>
+      <c r="CI7" s="53"/>
+      <c r="CJ7" s="53"/>
+      <c r="CK7" s="53"/>
+      <c r="CL7" s="53"/>
+      <c r="CM7" s="53"/>
+      <c r="CN7" s="53"/>
+      <c r="CO7" s="53"/>
+      <c r="CP7" s="53"/>
+      <c r="CQ7" s="53"/>
+      <c r="CR7" s="53"/>
+      <c r="CS7" s="53"/>
+      <c r="CT7" s="53"/>
+      <c r="CU7" s="53"/>
+      <c r="CV7" s="53"/>
+      <c r="CW7" s="53"/>
+      <c r="CX7" s="53"/>
+      <c r="CY7" s="53"/>
+      <c r="CZ7" s="53"/>
+      <c r="DA7" s="54"/>
+      <c r="DB7" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AO7" s="64"/>
-      <c r="AP7" s="64"/>
-      <c r="AQ7" s="64"/>
-      <c r="AR7" s="64"/>
-      <c r="AS7" s="64"/>
-      <c r="AT7" s="64"/>
-      <c r="AU7" s="64"/>
-      <c r="AV7" s="64"/>
-      <c r="AW7" s="64"/>
-      <c r="AX7" s="64"/>
-      <c r="AY7" s="64"/>
-      <c r="AZ7" s="64"/>
-      <c r="BA7" s="64"/>
-      <c r="BB7" s="64"/>
-      <c r="BC7" s="64"/>
-      <c r="BD7" s="64"/>
-      <c r="BE7" s="64"/>
-      <c r="BF7" s="64"/>
-      <c r="BG7" s="64"/>
-      <c r="BH7" s="64"/>
-      <c r="BI7" s="65"/>
-      <c r="BJ7" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="BK7" s="64"/>
-      <c r="BL7" s="64"/>
-      <c r="BM7" s="64"/>
-      <c r="BN7" s="64"/>
-      <c r="BO7" s="64"/>
-      <c r="BP7" s="64"/>
-      <c r="BQ7" s="64"/>
-      <c r="BR7" s="64"/>
-      <c r="BS7" s="64"/>
-      <c r="BT7" s="64"/>
-      <c r="BU7" s="64"/>
-      <c r="BV7" s="64"/>
-      <c r="BW7" s="64"/>
-      <c r="BX7" s="64"/>
-      <c r="BY7" s="64"/>
-      <c r="BZ7" s="64"/>
-      <c r="CA7" s="64"/>
-      <c r="CB7" s="64"/>
-      <c r="CC7" s="64"/>
-      <c r="CD7" s="64"/>
-      <c r="CE7" s="65"/>
-      <c r="CF7" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="CG7" s="64"/>
-      <c r="CH7" s="64"/>
-      <c r="CI7" s="64"/>
-      <c r="CJ7" s="64"/>
-      <c r="CK7" s="64"/>
-      <c r="CL7" s="64"/>
-      <c r="CM7" s="64"/>
-      <c r="CN7" s="64"/>
-      <c r="CO7" s="64"/>
-      <c r="CP7" s="64"/>
-      <c r="CQ7" s="64"/>
-      <c r="CR7" s="64"/>
-      <c r="CS7" s="64"/>
-      <c r="CT7" s="64"/>
-      <c r="CU7" s="64"/>
-      <c r="CV7" s="64"/>
-      <c r="CW7" s="64"/>
-      <c r="CX7" s="64"/>
-      <c r="CY7" s="64"/>
-      <c r="CZ7" s="64"/>
-      <c r="DA7" s="65"/>
-      <c r="DB7" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="DC7" s="64"/>
-      <c r="DD7" s="64"/>
-      <c r="DE7" s="64"/>
-      <c r="DF7" s="64"/>
-      <c r="DG7" s="64"/>
-      <c r="DH7" s="64"/>
-      <c r="DI7" s="64"/>
-      <c r="DJ7" s="64"/>
-      <c r="DK7" s="64"/>
-      <c r="DL7" s="64"/>
-      <c r="DM7" s="64"/>
-      <c r="DN7" s="64"/>
-      <c r="DO7" s="64"/>
-      <c r="DP7" s="64"/>
-      <c r="DQ7" s="64"/>
-      <c r="DR7" s="64"/>
-      <c r="DS7" s="64"/>
-      <c r="DT7" s="64"/>
-      <c r="DU7" s="64"/>
-      <c r="DV7" s="64"/>
-      <c r="DW7" s="65"/>
-      <c r="DX7" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="DY7" s="57"/>
-      <c r="DZ7" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="EA7" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="EB7" s="52"/>
+      <c r="DC7" s="53"/>
+      <c r="DD7" s="53"/>
+      <c r="DE7" s="53"/>
+      <c r="DF7" s="53"/>
+      <c r="DG7" s="53"/>
+      <c r="DH7" s="53"/>
+      <c r="DI7" s="53"/>
+      <c r="DJ7" s="53"/>
+      <c r="DK7" s="53"/>
+      <c r="DL7" s="53"/>
+      <c r="DM7" s="53"/>
+      <c r="DN7" s="53"/>
+      <c r="DO7" s="53"/>
+      <c r="DP7" s="53"/>
+      <c r="DQ7" s="53"/>
+      <c r="DR7" s="53"/>
+      <c r="DS7" s="53"/>
+      <c r="DT7" s="53"/>
+      <c r="DU7" s="53"/>
+      <c r="DV7" s="53"/>
+      <c r="DW7" s="54"/>
+      <c r="DX7" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="DY7" s="79"/>
+      <c r="DZ7" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="EA7" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="EB7" s="74"/>
       <c r="EC7" s="11"/>
     </row>
     <row r="8" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="73"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="59"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="70"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="4" t="s">
         <v>6</v>
@@ -2214,11 +2213,11 @@
       <c r="AK8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AL8" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM8" s="58" t="s">
-        <v>49</v>
+      <c r="AL8" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM8" s="56" t="s">
+        <v>45</v>
       </c>
       <c r="AN8" s="4" t="s">
         <v>6</v>
@@ -2280,11 +2279,11 @@
       <c r="BG8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BH8" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="BI8" s="58" t="s">
-        <v>49</v>
+      <c r="BH8" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="BI8" s="56" t="s">
+        <v>45</v>
       </c>
       <c r="BJ8" s="4" t="s">
         <v>6</v>
@@ -2346,11 +2345,11 @@
       <c r="CC8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CD8" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="CE8" s="58" t="s">
-        <v>49</v>
+      <c r="CD8" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="CE8" s="56" t="s">
+        <v>45</v>
       </c>
       <c r="CF8" s="4" t="s">
         <v>6</v>
@@ -2412,11 +2411,11 @@
       <c r="CY8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CZ8" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="DA8" s="58" t="s">
-        <v>49</v>
+      <c r="CZ8" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="DA8" s="56" t="s">
+        <v>45</v>
       </c>
       <c r="DB8" s="4" t="s">
         <v>6</v>
@@ -2478,715 +2477,715 @@
       <c r="DU8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DV8" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="DW8" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="DX8" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="DY8" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="DZ8" s="67"/>
-      <c r="EA8" s="53"/>
-      <c r="EB8" s="54"/>
+      <c r="DV8" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="DW8" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="DX8" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="DY8" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="DZ8" s="81"/>
+      <c r="EA8" s="75"/>
+      <c r="EB8" s="76"/>
     </row>
     <row r="9" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="69" t="s">
+      <c r="G9" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="69" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="M9" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
+      <c r="L9" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" s="70"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="70"/>
       <c r="Q9" s="15"/>
       <c r="R9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="S9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="T9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="U9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="V9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="W9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="X9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="Y9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="Z9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AA9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AB9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AC9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AD9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AE9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AF9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AG9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AH9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AI9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AJ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AK9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL9" s="61"/>
-      <c r="AM9" s="61"/>
+        <v>46</v>
+      </c>
+      <c r="AL9" s="57"/>
+      <c r="AM9" s="57"/>
       <c r="AN9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AO9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AP9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AQ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AR9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AS9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AT9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AU9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AV9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AW9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AX9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AY9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AZ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BA9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BB9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BC9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BD9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BE9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BF9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BG9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="BH9" s="61"/>
-      <c r="BI9" s="61"/>
+        <v>46</v>
+      </c>
+      <c r="BH9" s="57"/>
+      <c r="BI9" s="57"/>
       <c r="BJ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BK9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BL9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BM9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BN9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BO9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BP9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BQ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BR9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BS9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BT9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BU9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BV9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BW9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BX9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BY9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="BZ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CA9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CB9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CC9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="CD9" s="61"/>
-      <c r="CE9" s="61"/>
+        <v>46</v>
+      </c>
+      <c r="CD9" s="57"/>
+      <c r="CE9" s="57"/>
       <c r="CF9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CG9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CH9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CI9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CJ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CK9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CL9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CM9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CN9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CO9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CP9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CQ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CR9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CS9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CT9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CU9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CV9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CW9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CX9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="CY9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="CZ9" s="61"/>
-      <c r="DA9" s="61"/>
+        <v>46</v>
+      </c>
+      <c r="CZ9" s="57"/>
+      <c r="DA9" s="57"/>
       <c r="DB9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DC9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DD9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DE9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DF9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DG9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DH9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DI9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DJ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DK9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DL9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DM9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DN9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DO9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DP9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DQ9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DR9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DS9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DT9" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="DU9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="DV9" s="61"/>
-      <c r="DW9" s="61"/>
-      <c r="DX9" s="59"/>
-      <c r="DY9" s="59"/>
-      <c r="DZ9" s="67"/>
-      <c r="EA9" s="53"/>
-      <c r="EB9" s="54"/>
+        <v>46</v>
+      </c>
+      <c r="DV9" s="57"/>
+      <c r="DW9" s="57"/>
+      <c r="DX9" s="70"/>
+      <c r="DY9" s="70"/>
+      <c r="DZ9" s="81"/>
+      <c r="EA9" s="75"/>
+      <c r="EB9" s="76"/>
     </row>
     <row r="10" spans="1:133" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="S10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="V10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="W10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="X10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Y10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Z10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AA10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AB10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AC10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AD10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AE10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AF10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AG10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AH10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AI10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AJ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AK10" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL10" s="62"/>
-      <c r="AM10" s="62"/>
+        <v>49</v>
+      </c>
+      <c r="AL10" s="58"/>
+      <c r="AM10" s="58"/>
       <c r="AN10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AO10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AP10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AQ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AR10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AS10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AT10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AU10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AV10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AW10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AX10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AY10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AZ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BA10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BB10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BC10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BD10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BE10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BF10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BG10" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="BH10" s="62"/>
-      <c r="BI10" s="62"/>
+        <v>49</v>
+      </c>
+      <c r="BH10" s="58"/>
+      <c r="BI10" s="58"/>
       <c r="BJ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BK10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BL10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BM10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BN10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BO10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BP10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BQ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BR10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BS10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BT10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BU10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BV10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BW10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BX10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BY10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="BZ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CA10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CB10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CC10" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="CD10" s="62"/>
-      <c r="CE10" s="62"/>
+        <v>49</v>
+      </c>
+      <c r="CD10" s="58"/>
+      <c r="CE10" s="58"/>
       <c r="CF10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CG10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CH10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CI10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CJ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CK10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CL10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CM10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CN10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CO10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CP10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CQ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CR10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CS10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CT10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CU10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CV10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CW10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CX10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="CY10" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="CZ10" s="62"/>
-      <c r="DA10" s="62"/>
+        <v>49</v>
+      </c>
+      <c r="CZ10" s="58"/>
+      <c r="DA10" s="58"/>
       <c r="DB10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DC10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DD10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DE10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DF10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DG10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DH10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DI10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DJ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DK10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DL10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DM10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DN10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DO10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DP10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DQ10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DR10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DS10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DT10" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="DU10" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="DV10" s="62"/>
-      <c r="DW10" s="62"/>
-      <c r="DX10" s="60"/>
-      <c r="DY10" s="60"/>
-      <c r="DZ10" s="68"/>
-      <c r="EA10" s="55"/>
-      <c r="EB10" s="56"/>
+        <v>49</v>
+      </c>
+      <c r="DV10" s="58"/>
+      <c r="DW10" s="58"/>
+      <c r="DX10" s="66"/>
+      <c r="DY10" s="66"/>
+      <c r="DZ10" s="82"/>
+      <c r="EA10" s="77"/>
+      <c r="EB10" s="78"/>
     </row>
     <row r="11" spans="1:133" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -3199,40 +3198,40 @@
         <v>4</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="K11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="L11" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>5</v>
@@ -3605,34 +3604,34 @@
         <v>0</v>
       </c>
       <c r="DZ11" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="EA11" s="82" t="s">
-        <v>81</v>
-      </c>
-      <c r="EB11" s="83"/>
+        <v>80</v>
+      </c>
+      <c r="EA11" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="EB11" s="84"/>
       <c r="EC11" s="35" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A12" s="76" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="78"/>
+      <c r="A12" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="13">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -4091,23 +4090,23 @@
       <c r="EB12" s="40"/>
     </row>
     <row r="13" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A13" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="77"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="77"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="78"/>
+      <c r="A13" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="51"/>
       <c r="P13" s="13">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4566,23 +4565,23 @@
       <c r="EB13" s="44"/>
     </row>
     <row r="14" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="78"/>
+      <c r="A14" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="51"/>
       <c r="P14" s="13">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -5051,40 +5050,40 @@
         <v>4</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="K15" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="L15" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N15" s="7" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>5</v>
@@ -5406,34 +5405,34 @@
       <c r="DX15" s="30"/>
       <c r="DY15" s="37"/>
       <c r="DZ15" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="EA15" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="EB15" s="50"/>
+        <v>80</v>
+      </c>
+      <c r="EA15" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="EB15" s="72"/>
       <c r="EC15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:133" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="85"/>
-      <c r="K16" s="85"/>
-      <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
+      <c r="A16" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="51"/>
       <c r="P16" s="13">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -5871,15 +5870,15 @@
     </row>
     <row r="18" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" t="str">
         <f>B31</f>
@@ -5888,7 +5887,7 @@
     </row>
     <row r="20" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" t="str">
         <f>B33</f>
@@ -5897,7 +5896,7 @@
     </row>
     <row r="21" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" t="str">
         <f>B32</f>
@@ -5906,7 +5905,7 @@
     </row>
     <row r="22" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" t="str">
         <f>B31</f>
@@ -5915,7 +5914,7 @@
     </row>
     <row r="23" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" t="str">
         <f>B33</f>
@@ -5924,7 +5923,7 @@
     </row>
     <row r="24" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" t="str">
         <f>B31</f>
@@ -5933,7 +5932,7 @@
     </row>
     <row r="25" spans="1:129" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="str">
         <f>B31</f>
@@ -5942,7 +5941,7 @@
     </row>
     <row r="26" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" t="str">
         <f>B33</f>
@@ -5951,7 +5950,7 @@
     </row>
     <row r="27" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27" t="str">
         <f>B32</f>
@@ -5960,7 +5959,7 @@
     </row>
     <row r="28" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28" t="str">
         <f>B31</f>
@@ -5969,7 +5968,7 @@
     </row>
     <row r="29" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" t="str">
         <f>B33</f>
@@ -5979,51 +5978,51 @@
     <row r="30" spans="1:129" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:129" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="78"/>
+      <c r="A36" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="22">
         <v>1</v>
       </c>
-      <c r="B37" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="84"/>
+      <c r="B37" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="55"/>
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
@@ -6039,10 +6038,10 @@
       <c r="A38" s="22">
         <v>2</v>
       </c>
-      <c r="B38" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="84"/>
+      <c r="B38" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="55"/>
       <c r="D38" s="34"/>
       <c r="E38" s="34"/>
       <c r="F38" s="34"/>
@@ -6058,10 +6057,10 @@
       <c r="A39" s="22">
         <v>3</v>
       </c>
-      <c r="B39" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="84"/>
+      <c r="B39" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="55"/>
       <c r="D39" s="34"/>
       <c r="E39" s="34"/>
       <c r="F39" s="34"/>
@@ -6075,6 +6074,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="EA15:EB15"/>
+    <mergeCell ref="EA7:EB10"/>
+    <mergeCell ref="DX7:DY7"/>
+    <mergeCell ref="DX8:DX10"/>
+    <mergeCell ref="DY8:DY10"/>
+    <mergeCell ref="DZ7:DZ10"/>
+    <mergeCell ref="EA11:EB11"/>
+    <mergeCell ref="CZ8:CZ10"/>
+    <mergeCell ref="DA8:DA10"/>
+    <mergeCell ref="DV8:DV10"/>
+    <mergeCell ref="DW8:DW10"/>
+    <mergeCell ref="DB7:DW7"/>
+    <mergeCell ref="CF7:DA7"/>
+    <mergeCell ref="D7:H8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I7:M8"/>
+    <mergeCell ref="P7:P10"/>
+    <mergeCell ref="N7:N10"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AN7:BI7"/>
     <mergeCell ref="BJ7:CE7"/>
@@ -6091,39 +6123,6 @@
     <mergeCell ref="A16:O16"/>
     <mergeCell ref="A12:O12"/>
     <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D7:H8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I7:M8"/>
-    <mergeCell ref="P7:P10"/>
-    <mergeCell ref="N7:N10"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="CZ8:CZ10"/>
-    <mergeCell ref="DA8:DA10"/>
-    <mergeCell ref="DV8:DV10"/>
-    <mergeCell ref="DW8:DW10"/>
-    <mergeCell ref="DB7:DW7"/>
-    <mergeCell ref="CF7:DA7"/>
-    <mergeCell ref="EA15:EB15"/>
-    <mergeCell ref="EA7:EB10"/>
-    <mergeCell ref="DX7:DY7"/>
-    <mergeCell ref="DX8:DX10"/>
-    <mergeCell ref="DY8:DY10"/>
-    <mergeCell ref="DZ7:DZ10"/>
-    <mergeCell ref="EA11:EB11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-3026: Abholung aus der Tagesschule in Statistik zeigen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\kibon-app\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBDF030-304F-4961-8E79-F79CF9D54A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719803FC-FE78-4B92-8474-C82D281B7049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="94">
   <si>
     <t>{statusTitle}</t>
   </si>
@@ -538,6 +538,12 @@
   </si>
   <si>
     <t>{anzahlNichtFreigegebeneAnmeldungen}</t>
+  </si>
+  <si>
+    <t>{abholungTagesschuleTitle}</t>
+  </si>
+  <si>
+    <t>{abholungTagesschule}</t>
   </si>
 </sst>
 </file>
@@ -801,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -909,9 +915,22 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1103,9 +1122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1143,9 +1162,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1178,26 +1197,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1230,26 +1232,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1426,10 +1411,10 @@
   <sheetPr codeName="Tabelle1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EF39"/>
+  <dimension ref="A1:EG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="DK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="EC3" sqref="EC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,11 +1433,12 @@
     <col min="109" max="127" width="10.5703125"/>
     <col min="128" max="128" width="10" customWidth="1"/>
     <col min="131" max="132" width="10.5703125"/>
-    <col min="133" max="133" width="22.7109375" customWidth="1"/>
-    <col min="136" max="992" width="10.5703125"/>
+    <col min="133" max="133" width="34.5703125" customWidth="1"/>
+    <col min="134" max="134" width="22.7109375" customWidth="1"/>
+    <col min="137" max="993" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:136" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:137" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -1481,7 +1467,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:136" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:137" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1496,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:136" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:137" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1537,7 +1523,7 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:137" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1564,7 +1550,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:136" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:137" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
@@ -1700,7 +1686,7 @@
       <c r="DY5" s="2"/>
       <c r="DZ5" s="2"/>
     </row>
-    <row r="6" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:137" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
@@ -2016,194 +2002,197 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:136" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="51" t="s">
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="51" t="s">
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="51" t="s">
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="57" t="s">
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="57" t="s">
+      <c r="R7" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="S7" s="57" t="s">
+      <c r="S7" s="62" t="s">
         <v>0</v>
       </c>
       <c r="T7" s="14"/>
-      <c r="U7" s="77" t="s">
+      <c r="U7" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="V7" s="78"/>
-      <c r="W7" s="78"/>
-      <c r="X7" s="78"/>
-      <c r="Y7" s="78"/>
-      <c r="Z7" s="78"/>
-      <c r="AA7" s="78"/>
-      <c r="AB7" s="78"/>
-      <c r="AC7" s="78"/>
-      <c r="AD7" s="78"/>
-      <c r="AE7" s="78"/>
-      <c r="AF7" s="78"/>
-      <c r="AG7" s="78"/>
-      <c r="AH7" s="78"/>
-      <c r="AI7" s="78"/>
-      <c r="AJ7" s="78"/>
-      <c r="AK7" s="78"/>
-      <c r="AL7" s="78"/>
-      <c r="AM7" s="78"/>
-      <c r="AN7" s="78"/>
-      <c r="AO7" s="78"/>
-      <c r="AP7" s="79"/>
-      <c r="AQ7" s="77" t="s">
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
+      <c r="AH7" s="83"/>
+      <c r="AI7" s="83"/>
+      <c r="AJ7" s="83"/>
+      <c r="AK7" s="83"/>
+      <c r="AL7" s="83"/>
+      <c r="AM7" s="83"/>
+      <c r="AN7" s="83"/>
+      <c r="AO7" s="83"/>
+      <c r="AP7" s="84"/>
+      <c r="AQ7" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="AR7" s="78"/>
-      <c r="AS7" s="78"/>
-      <c r="AT7" s="78"/>
-      <c r="AU7" s="78"/>
-      <c r="AV7" s="78"/>
-      <c r="AW7" s="78"/>
-      <c r="AX7" s="78"/>
-      <c r="AY7" s="78"/>
-      <c r="AZ7" s="78"/>
-      <c r="BA7" s="78"/>
-      <c r="BB7" s="78"/>
-      <c r="BC7" s="78"/>
-      <c r="BD7" s="78"/>
-      <c r="BE7" s="78"/>
-      <c r="BF7" s="78"/>
-      <c r="BG7" s="78"/>
-      <c r="BH7" s="78"/>
-      <c r="BI7" s="78"/>
-      <c r="BJ7" s="78"/>
-      <c r="BK7" s="78"/>
-      <c r="BL7" s="79"/>
-      <c r="BM7" s="77" t="s">
+      <c r="AR7" s="83"/>
+      <c r="AS7" s="83"/>
+      <c r="AT7" s="83"/>
+      <c r="AU7" s="83"/>
+      <c r="AV7" s="83"/>
+      <c r="AW7" s="83"/>
+      <c r="AX7" s="83"/>
+      <c r="AY7" s="83"/>
+      <c r="AZ7" s="83"/>
+      <c r="BA7" s="83"/>
+      <c r="BB7" s="83"/>
+      <c r="BC7" s="83"/>
+      <c r="BD7" s="83"/>
+      <c r="BE7" s="83"/>
+      <c r="BF7" s="83"/>
+      <c r="BG7" s="83"/>
+      <c r="BH7" s="83"/>
+      <c r="BI7" s="83"/>
+      <c r="BJ7" s="83"/>
+      <c r="BK7" s="83"/>
+      <c r="BL7" s="84"/>
+      <c r="BM7" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="BN7" s="78"/>
-      <c r="BO7" s="78"/>
-      <c r="BP7" s="78"/>
-      <c r="BQ7" s="78"/>
-      <c r="BR7" s="78"/>
-      <c r="BS7" s="78"/>
-      <c r="BT7" s="78"/>
-      <c r="BU7" s="78"/>
-      <c r="BV7" s="78"/>
-      <c r="BW7" s="78"/>
-      <c r="BX7" s="78"/>
-      <c r="BY7" s="78"/>
-      <c r="BZ7" s="78"/>
-      <c r="CA7" s="78"/>
-      <c r="CB7" s="78"/>
-      <c r="CC7" s="78"/>
-      <c r="CD7" s="78"/>
-      <c r="CE7" s="78"/>
-      <c r="CF7" s="78"/>
-      <c r="CG7" s="78"/>
-      <c r="CH7" s="79"/>
-      <c r="CI7" s="77" t="s">
+      <c r="BN7" s="83"/>
+      <c r="BO7" s="83"/>
+      <c r="BP7" s="83"/>
+      <c r="BQ7" s="83"/>
+      <c r="BR7" s="83"/>
+      <c r="BS7" s="83"/>
+      <c r="BT7" s="83"/>
+      <c r="BU7" s="83"/>
+      <c r="BV7" s="83"/>
+      <c r="BW7" s="83"/>
+      <c r="BX7" s="83"/>
+      <c r="BY7" s="83"/>
+      <c r="BZ7" s="83"/>
+      <c r="CA7" s="83"/>
+      <c r="CB7" s="83"/>
+      <c r="CC7" s="83"/>
+      <c r="CD7" s="83"/>
+      <c r="CE7" s="83"/>
+      <c r="CF7" s="83"/>
+      <c r="CG7" s="83"/>
+      <c r="CH7" s="84"/>
+      <c r="CI7" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="CJ7" s="78"/>
-      <c r="CK7" s="78"/>
-      <c r="CL7" s="78"/>
-      <c r="CM7" s="78"/>
-      <c r="CN7" s="78"/>
-      <c r="CO7" s="78"/>
-      <c r="CP7" s="78"/>
-      <c r="CQ7" s="78"/>
-      <c r="CR7" s="78"/>
-      <c r="CS7" s="78"/>
-      <c r="CT7" s="78"/>
-      <c r="CU7" s="78"/>
-      <c r="CV7" s="78"/>
-      <c r="CW7" s="78"/>
-      <c r="CX7" s="78"/>
-      <c r="CY7" s="78"/>
-      <c r="CZ7" s="78"/>
-      <c r="DA7" s="78"/>
-      <c r="DB7" s="78"/>
-      <c r="DC7" s="78"/>
-      <c r="DD7" s="79"/>
-      <c r="DE7" s="77" t="s">
+      <c r="CJ7" s="83"/>
+      <c r="CK7" s="83"/>
+      <c r="CL7" s="83"/>
+      <c r="CM7" s="83"/>
+      <c r="CN7" s="83"/>
+      <c r="CO7" s="83"/>
+      <c r="CP7" s="83"/>
+      <c r="CQ7" s="83"/>
+      <c r="CR7" s="83"/>
+      <c r="CS7" s="83"/>
+      <c r="CT7" s="83"/>
+      <c r="CU7" s="83"/>
+      <c r="CV7" s="83"/>
+      <c r="CW7" s="83"/>
+      <c r="CX7" s="83"/>
+      <c r="CY7" s="83"/>
+      <c r="CZ7" s="83"/>
+      <c r="DA7" s="83"/>
+      <c r="DB7" s="83"/>
+      <c r="DC7" s="83"/>
+      <c r="DD7" s="84"/>
+      <c r="DE7" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="DF7" s="78"/>
-      <c r="DG7" s="78"/>
-      <c r="DH7" s="78"/>
-      <c r="DI7" s="78"/>
-      <c r="DJ7" s="78"/>
-      <c r="DK7" s="78"/>
-      <c r="DL7" s="78"/>
-      <c r="DM7" s="78"/>
-      <c r="DN7" s="78"/>
-      <c r="DO7" s="78"/>
-      <c r="DP7" s="78"/>
-      <c r="DQ7" s="78"/>
-      <c r="DR7" s="78"/>
-      <c r="DS7" s="78"/>
-      <c r="DT7" s="78"/>
-      <c r="DU7" s="78"/>
-      <c r="DV7" s="78"/>
-      <c r="DW7" s="78"/>
-      <c r="DX7" s="78"/>
-      <c r="DY7" s="78"/>
-      <c r="DZ7" s="79"/>
-      <c r="EA7" s="67" t="s">
+      <c r="DF7" s="83"/>
+      <c r="DG7" s="83"/>
+      <c r="DH7" s="83"/>
+      <c r="DI7" s="83"/>
+      <c r="DJ7" s="83"/>
+      <c r="DK7" s="83"/>
+      <c r="DL7" s="83"/>
+      <c r="DM7" s="83"/>
+      <c r="DN7" s="83"/>
+      <c r="DO7" s="83"/>
+      <c r="DP7" s="83"/>
+      <c r="DQ7" s="83"/>
+      <c r="DR7" s="83"/>
+      <c r="DS7" s="83"/>
+      <c r="DT7" s="83"/>
+      <c r="DU7" s="83"/>
+      <c r="DV7" s="83"/>
+      <c r="DW7" s="83"/>
+      <c r="DX7" s="83"/>
+      <c r="DY7" s="83"/>
+      <c r="DZ7" s="84"/>
+      <c r="EA7" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="EB7" s="67"/>
-      <c r="EC7" s="70" t="s">
+      <c r="EB7" s="72"/>
+      <c r="EC7" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="ED7" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="ED7" s="61" t="s">
+      <c r="EE7" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="EE7" s="62"/>
-      <c r="EF7" s="11"/>
+      <c r="EF7" s="67"/>
+      <c r="EG7" s="11"/>
     </row>
-    <row r="8" spans="1:136" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
+    <row r="8" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
       <c r="T8" s="15"/>
       <c r="U8" s="4" t="s">
         <v>6</v>
@@ -2265,10 +2254,10 @@
       <c r="AN8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AO8" s="68" t="s">
+      <c r="AO8" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="AP8" s="68" t="s">
+      <c r="AP8" s="73" t="s">
         <v>45</v>
       </c>
       <c r="AQ8" s="4" t="s">
@@ -2331,10 +2320,10 @@
       <c r="BJ8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BK8" s="68" t="s">
+      <c r="BK8" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="BL8" s="68" t="s">
+      <c r="BL8" s="73" t="s">
         <v>45</v>
       </c>
       <c r="BM8" s="4" t="s">
@@ -2397,10 +2386,10 @@
       <c r="CF8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CG8" s="68" t="s">
+      <c r="CG8" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="CH8" s="68" t="s">
+      <c r="CH8" s="73" t="s">
         <v>45</v>
       </c>
       <c r="CI8" s="4" t="s">
@@ -2463,10 +2452,10 @@
       <c r="DB8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="DC8" s="68" t="s">
+      <c r="DC8" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="DD8" s="68" t="s">
+      <c r="DD8" s="73" t="s">
         <v>45</v>
       </c>
       <c r="DE8" s="4" t="s">
@@ -2529,74 +2518,75 @@
       <c r="DX8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DY8" s="68" t="s">
+      <c r="DY8" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="DZ8" s="68" t="s">
+      <c r="DZ8" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="EA8" s="68" t="s">
+      <c r="EA8" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="EB8" s="68" t="s">
+      <c r="EB8" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="EC8" s="71"/>
-      <c r="ED8" s="63"/>
-      <c r="EE8" s="64"/>
+      <c r="EC8" s="53"/>
+      <c r="ED8" s="76"/>
+      <c r="EE8" s="68"/>
+      <c r="EF8" s="69"/>
     </row>
-    <row r="9" spans="1:136" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="57" t="s">
+      <c r="I9" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="57" t="s">
+      <c r="J9" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="57" t="s">
+      <c r="K9" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="57" t="s">
+      <c r="L9" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="57" t="s">
+      <c r="M9" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="57" t="s">
+      <c r="N9" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="57" t="s">
+      <c r="O9" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="P9" s="57" t="s">
+      <c r="P9" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="Q9" s="69"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
       <c r="T9" s="15"/>
       <c r="U9" s="32" t="s">
         <v>46</v>
@@ -2658,8 +2648,8 @@
       <c r="AN9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AO9" s="75"/>
-      <c r="AP9" s="75"/>
+      <c r="AO9" s="80"/>
+      <c r="AP9" s="80"/>
       <c r="AQ9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2720,8 +2710,8 @@
       <c r="BJ9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="BK9" s="75"/>
-      <c r="BL9" s="75"/>
+      <c r="BK9" s="80"/>
+      <c r="BL9" s="80"/>
       <c r="BM9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2782,8 +2772,8 @@
       <c r="CF9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="CG9" s="75"/>
-      <c r="CH9" s="75"/>
+      <c r="CG9" s="80"/>
+      <c r="CH9" s="80"/>
       <c r="CI9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2844,8 +2834,8 @@
       <c r="DB9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="DC9" s="75"/>
-      <c r="DD9" s="75"/>
+      <c r="DC9" s="80"/>
+      <c r="DD9" s="80"/>
       <c r="DE9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2906,34 +2896,35 @@
       <c r="DX9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="DY9" s="75"/>
-      <c r="DZ9" s="75"/>
-      <c r="EA9" s="69"/>
-      <c r="EB9" s="69"/>
-      <c r="EC9" s="71"/>
-      <c r="ED9" s="63"/>
-      <c r="EE9" s="64"/>
+      <c r="DY9" s="80"/>
+      <c r="DZ9" s="80"/>
+      <c r="EA9" s="74"/>
+      <c r="EB9" s="74"/>
+      <c r="EC9" s="51"/>
+      <c r="ED9" s="76"/>
+      <c r="EE9" s="68"/>
+      <c r="EF9" s="69"/>
     </row>
-    <row r="10" spans="1:136" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
+    <row r="10" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
       <c r="T10" s="15"/>
       <c r="U10" s="16" t="s">
         <v>49</v>
@@ -2995,8 +2986,8 @@
       <c r="AN10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AO10" s="76"/>
-      <c r="AP10" s="76"/>
+      <c r="AO10" s="81"/>
+      <c r="AP10" s="81"/>
       <c r="AQ10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3057,8 +3048,8 @@
       <c r="BJ10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="BK10" s="76"/>
-      <c r="BL10" s="76"/>
+      <c r="BK10" s="81"/>
+      <c r="BL10" s="81"/>
       <c r="BM10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3119,8 +3110,8 @@
       <c r="CF10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="CG10" s="76"/>
-      <c r="CH10" s="76"/>
+      <c r="CG10" s="81"/>
+      <c r="CH10" s="81"/>
       <c r="CI10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3181,8 +3172,8 @@
       <c r="DB10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="DC10" s="76"/>
-      <c r="DD10" s="76"/>
+      <c r="DC10" s="81"/>
+      <c r="DD10" s="81"/>
       <c r="DE10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3243,15 +3234,16 @@
       <c r="DX10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="DY10" s="76"/>
-      <c r="DZ10" s="76"/>
-      <c r="EA10" s="58"/>
-      <c r="EB10" s="58"/>
-      <c r="EC10" s="72"/>
-      <c r="ED10" s="65"/>
-      <c r="EE10" s="66"/>
+      <c r="DY10" s="81"/>
+      <c r="DZ10" s="81"/>
+      <c r="EA10" s="63"/>
+      <c r="EB10" s="63"/>
+      <c r="EC10" s="50"/>
+      <c r="ED10" s="77"/>
+      <c r="EE10" s="70"/>
+      <c r="EF10" s="71"/>
     </row>
-    <row r="11" spans="1:136" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:137" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -3676,38 +3668,41 @@
         <f>SUM(DZ11,AP11,BL11,CH11,DD11)</f>
         <v>0</v>
       </c>
-      <c r="EC11" s="48" t="s">
+      <c r="EC11" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="ED11" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="ED11" s="73" t="s">
+      <c r="EE11" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="EE11" s="74"/>
-      <c r="EF11" s="35" t="s">
+      <c r="EF11" s="79"/>
+      <c r="EG11" s="35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="A12" s="83" t="s">
+    <row r="12" spans="1:137" x14ac:dyDescent="0.25">
+      <c r="A12" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="84"/>
-      <c r="M12" s="84"/>
-      <c r="N12" s="84"/>
-      <c r="O12" s="84"/>
-      <c r="P12" s="84"/>
-      <c r="Q12" s="84"/>
-      <c r="R12" s="85"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="90"/>
       <c r="S12" s="13">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -4161,31 +4156,32 @@
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$33)</f>
         <v>0</v>
       </c>
-      <c r="EC12" s="45"/>
-      <c r="ED12" s="39"/>
-      <c r="EE12" s="40"/>
+      <c r="EC12" s="54"/>
+      <c r="ED12" s="45"/>
+      <c r="EE12" s="39"/>
+      <c r="EF12" s="40"/>
     </row>
-    <row r="13" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="A13" s="83" t="s">
+    <row r="13" spans="1:137" x14ac:dyDescent="0.25">
+      <c r="A13" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="84"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="84"/>
-      <c r="O13" s="84"/>
-      <c r="P13" s="84"/>
-      <c r="Q13" s="84"/>
-      <c r="R13" s="85"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="90"/>
       <c r="S13" s="13">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4639,31 +4635,32 @@
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$32)</f>
         <v>0</v>
       </c>
-      <c r="EC13" s="46"/>
-      <c r="ED13" s="28"/>
-      <c r="EE13" s="44"/>
+      <c r="EC13" s="55"/>
+      <c r="ED13" s="46"/>
+      <c r="EE13" s="28"/>
+      <c r="EF13" s="44"/>
     </row>
-    <row r="14" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="A14" s="83" t="s">
+    <row r="14" spans="1:137" x14ac:dyDescent="0.25">
+      <c r="A14" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="84"/>
-      <c r="O14" s="84"/>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="84"/>
-      <c r="R14" s="85"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="90"/>
       <c r="S14" s="13">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -5117,11 +5114,12 @@
         <f>SUMIFS(summeVerpflegungWoche,statusKategorie,$B$31)</f>
         <v>0</v>
       </c>
-      <c r="EC14" s="47"/>
-      <c r="ED14" s="38"/>
-      <c r="EE14" s="36"/>
+      <c r="EC14" s="42"/>
+      <c r="ED14" s="47"/>
+      <c r="EE14" s="38"/>
+      <c r="EF14" s="36"/>
     </row>
-    <row r="15" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
@@ -5495,38 +5493,39 @@
       <c r="DZ15" s="27"/>
       <c r="EA15" s="30"/>
       <c r="EB15" s="37"/>
-      <c r="EC15" s="48" t="s">
+      <c r="EC15" s="37"/>
+      <c r="ED15" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="ED15" s="59" t="s">
+      <c r="EE15" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="EE15" s="60"/>
-      <c r="EF15" t="s">
+      <c r="EF15" s="65"/>
+      <c r="EG15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="A16" s="87" t="s">
+    <row r="16" spans="1:137" x14ac:dyDescent="0.25">
+      <c r="A16" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="87"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="87"/>
-      <c r="R16" s="87"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="92"/>
+      <c r="P16" s="92"/>
+      <c r="Q16" s="92"/>
+      <c r="R16" s="92"/>
       <c r="S16" s="13">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -5944,9 +5943,10 @@
       <c r="DZ16" s="28"/>
       <c r="EA16" s="25"/>
       <c r="EB16" s="38"/>
-      <c r="EC16" s="25"/>
-      <c r="ED16" s="38"/>
-      <c r="EE16" s="36"/>
+      <c r="EC16" s="38"/>
+      <c r="ED16" s="25"/>
+      <c r="EE16" s="38"/>
+      <c r="EF16" s="36"/>
     </row>
     <row r="17" spans="1:132" x14ac:dyDescent="0.25">
       <c r="AO17" s="29"/>
@@ -6103,11 +6103,11 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="83" t="s">
+      <c r="A36" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="84"/>
-      <c r="C36" s="85"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="90"/>
       <c r="D36" s="49"/>
       <c r="E36" s="49"/>
       <c r="F36" s="49"/>
@@ -6116,13 +6116,13 @@
       <c r="A37" s="22">
         <v>1</v>
       </c>
-      <c r="B37" s="86" t="s">
+      <c r="B37" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="86"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -6138,13 +6138,13 @@
       <c r="A38" s="22">
         <v>2</v>
       </c>
-      <c r="B38" s="86" t="s">
+      <c r="B38" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="86"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -6160,13 +6160,13 @@
       <c r="A39" s="22">
         <v>3</v>
       </c>
-      <c r="B39" s="86" t="s">
+      <c r="B39" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="86"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
+      <c r="C39" s="91"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -6219,13 +6219,13 @@
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="D7:F8"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="ED15:EE15"/>
-    <mergeCell ref="ED7:EE10"/>
+    <mergeCell ref="EE15:EF15"/>
+    <mergeCell ref="EE7:EF10"/>
     <mergeCell ref="EA7:EB7"/>
     <mergeCell ref="EA8:EA10"/>
     <mergeCell ref="EB8:EB10"/>
-    <mergeCell ref="EC7:EC10"/>
-    <mergeCell ref="ED11:EE11"/>
+    <mergeCell ref="ED7:ED10"/>
+    <mergeCell ref="EE11:EF11"/>
     <mergeCell ref="DC8:DC10"/>
     <mergeCell ref="DD8:DD10"/>
     <mergeCell ref="DY8:DY10"/>

</xml_diff>

<commit_message>
KIBON-3026: Review anpassungen (Translation file, nicht freigegebene anmeldungen)
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleAnmeldungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\kibon-app\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719803FC-FE78-4B92-8474-C82D281B7049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9BF895-EE4C-4A85-839D-B9FB7E63CAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="94">
   <si>
     <t>{statusTitle}</t>
   </si>
@@ -807,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -932,109 +932,112 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1414,7 +1417,7 @@
   <dimension ref="A1:EG39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="DK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EC3" sqref="EC3"/>
+      <selection activeCell="EC38" sqref="EC38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,7 +1436,7 @@
     <col min="109" max="127" width="10.5703125"/>
     <col min="128" max="128" width="10" customWidth="1"/>
     <col min="131" max="132" width="10.5703125"/>
-    <col min="133" max="133" width="34.5703125" customWidth="1"/>
+    <col min="133" max="133" width="50" customWidth="1"/>
     <col min="134" max="134" width="22.7109375" customWidth="1"/>
     <col min="137" max="993" width="10.5703125"/>
   </cols>
@@ -2003,196 +2006,196 @@
       </c>
     </row>
     <row r="7" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="56" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="56" t="s">
+      <c r="E7" s="69"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="56" t="s">
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="62" t="s">
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="62" t="s">
+      <c r="R7" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="S7" s="62" t="s">
+      <c r="S7" s="74" t="s">
         <v>0</v>
       </c>
       <c r="T7" s="14"/>
-      <c r="U7" s="82" t="s">
+      <c r="U7" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
-      <c r="X7" s="83"/>
-      <c r="Y7" s="83"/>
-      <c r="Z7" s="83"/>
-      <c r="AA7" s="83"/>
-      <c r="AB7" s="83"/>
-      <c r="AC7" s="83"/>
-      <c r="AD7" s="83"/>
-      <c r="AE7" s="83"/>
-      <c r="AF7" s="83"/>
-      <c r="AG7" s="83"/>
-      <c r="AH7" s="83"/>
-      <c r="AI7" s="83"/>
-      <c r="AJ7" s="83"/>
-      <c r="AK7" s="83"/>
-      <c r="AL7" s="83"/>
-      <c r="AM7" s="83"/>
-      <c r="AN7" s="83"/>
-      <c r="AO7" s="83"/>
-      <c r="AP7" s="84"/>
-      <c r="AQ7" s="82" t="s">
+      <c r="V7" s="61"/>
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="61"/>
+      <c r="Z7" s="61"/>
+      <c r="AA7" s="61"/>
+      <c r="AB7" s="61"/>
+      <c r="AC7" s="61"/>
+      <c r="AD7" s="61"/>
+      <c r="AE7" s="61"/>
+      <c r="AF7" s="61"/>
+      <c r="AG7" s="61"/>
+      <c r="AH7" s="61"/>
+      <c r="AI7" s="61"/>
+      <c r="AJ7" s="61"/>
+      <c r="AK7" s="61"/>
+      <c r="AL7" s="61"/>
+      <c r="AM7" s="61"/>
+      <c r="AN7" s="61"/>
+      <c r="AO7" s="61"/>
+      <c r="AP7" s="62"/>
+      <c r="AQ7" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="AR7" s="83"/>
-      <c r="AS7" s="83"/>
-      <c r="AT7" s="83"/>
-      <c r="AU7" s="83"/>
-      <c r="AV7" s="83"/>
-      <c r="AW7" s="83"/>
-      <c r="AX7" s="83"/>
-      <c r="AY7" s="83"/>
-      <c r="AZ7" s="83"/>
-      <c r="BA7" s="83"/>
-      <c r="BB7" s="83"/>
-      <c r="BC7" s="83"/>
-      <c r="BD7" s="83"/>
-      <c r="BE7" s="83"/>
-      <c r="BF7" s="83"/>
-      <c r="BG7" s="83"/>
-      <c r="BH7" s="83"/>
-      <c r="BI7" s="83"/>
-      <c r="BJ7" s="83"/>
-      <c r="BK7" s="83"/>
-      <c r="BL7" s="84"/>
-      <c r="BM7" s="82" t="s">
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="61"/>
+      <c r="AT7" s="61"/>
+      <c r="AU7" s="61"/>
+      <c r="AV7" s="61"/>
+      <c r="AW7" s="61"/>
+      <c r="AX7" s="61"/>
+      <c r="AY7" s="61"/>
+      <c r="AZ7" s="61"/>
+      <c r="BA7" s="61"/>
+      <c r="BB7" s="61"/>
+      <c r="BC7" s="61"/>
+      <c r="BD7" s="61"/>
+      <c r="BE7" s="61"/>
+      <c r="BF7" s="61"/>
+      <c r="BG7" s="61"/>
+      <c r="BH7" s="61"/>
+      <c r="BI7" s="61"/>
+      <c r="BJ7" s="61"/>
+      <c r="BK7" s="61"/>
+      <c r="BL7" s="62"/>
+      <c r="BM7" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="BN7" s="83"/>
-      <c r="BO7" s="83"/>
-      <c r="BP7" s="83"/>
-      <c r="BQ7" s="83"/>
-      <c r="BR7" s="83"/>
-      <c r="BS7" s="83"/>
-      <c r="BT7" s="83"/>
-      <c r="BU7" s="83"/>
-      <c r="BV7" s="83"/>
-      <c r="BW7" s="83"/>
-      <c r="BX7" s="83"/>
-      <c r="BY7" s="83"/>
-      <c r="BZ7" s="83"/>
-      <c r="CA7" s="83"/>
-      <c r="CB7" s="83"/>
-      <c r="CC7" s="83"/>
-      <c r="CD7" s="83"/>
-      <c r="CE7" s="83"/>
-      <c r="CF7" s="83"/>
-      <c r="CG7" s="83"/>
-      <c r="CH7" s="84"/>
-      <c r="CI7" s="82" t="s">
+      <c r="BN7" s="61"/>
+      <c r="BO7" s="61"/>
+      <c r="BP7" s="61"/>
+      <c r="BQ7" s="61"/>
+      <c r="BR7" s="61"/>
+      <c r="BS7" s="61"/>
+      <c r="BT7" s="61"/>
+      <c r="BU7" s="61"/>
+      <c r="BV7" s="61"/>
+      <c r="BW7" s="61"/>
+      <c r="BX7" s="61"/>
+      <c r="BY7" s="61"/>
+      <c r="BZ7" s="61"/>
+      <c r="CA7" s="61"/>
+      <c r="CB7" s="61"/>
+      <c r="CC7" s="61"/>
+      <c r="CD7" s="61"/>
+      <c r="CE7" s="61"/>
+      <c r="CF7" s="61"/>
+      <c r="CG7" s="61"/>
+      <c r="CH7" s="62"/>
+      <c r="CI7" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="CJ7" s="83"/>
-      <c r="CK7" s="83"/>
-      <c r="CL7" s="83"/>
-      <c r="CM7" s="83"/>
-      <c r="CN7" s="83"/>
-      <c r="CO7" s="83"/>
-      <c r="CP7" s="83"/>
-      <c r="CQ7" s="83"/>
-      <c r="CR7" s="83"/>
-      <c r="CS7" s="83"/>
-      <c r="CT7" s="83"/>
-      <c r="CU7" s="83"/>
-      <c r="CV7" s="83"/>
-      <c r="CW7" s="83"/>
-      <c r="CX7" s="83"/>
-      <c r="CY7" s="83"/>
-      <c r="CZ7" s="83"/>
-      <c r="DA7" s="83"/>
-      <c r="DB7" s="83"/>
-      <c r="DC7" s="83"/>
-      <c r="DD7" s="84"/>
-      <c r="DE7" s="82" t="s">
+      <c r="CJ7" s="61"/>
+      <c r="CK7" s="61"/>
+      <c r="CL7" s="61"/>
+      <c r="CM7" s="61"/>
+      <c r="CN7" s="61"/>
+      <c r="CO7" s="61"/>
+      <c r="CP7" s="61"/>
+      <c r="CQ7" s="61"/>
+      <c r="CR7" s="61"/>
+      <c r="CS7" s="61"/>
+      <c r="CT7" s="61"/>
+      <c r="CU7" s="61"/>
+      <c r="CV7" s="61"/>
+      <c r="CW7" s="61"/>
+      <c r="CX7" s="61"/>
+      <c r="CY7" s="61"/>
+      <c r="CZ7" s="61"/>
+      <c r="DA7" s="61"/>
+      <c r="DB7" s="61"/>
+      <c r="DC7" s="61"/>
+      <c r="DD7" s="62"/>
+      <c r="DE7" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="DF7" s="83"/>
-      <c r="DG7" s="83"/>
-      <c r="DH7" s="83"/>
-      <c r="DI7" s="83"/>
-      <c r="DJ7" s="83"/>
-      <c r="DK7" s="83"/>
-      <c r="DL7" s="83"/>
-      <c r="DM7" s="83"/>
-      <c r="DN7" s="83"/>
-      <c r="DO7" s="83"/>
-      <c r="DP7" s="83"/>
-      <c r="DQ7" s="83"/>
-      <c r="DR7" s="83"/>
-      <c r="DS7" s="83"/>
-      <c r="DT7" s="83"/>
-      <c r="DU7" s="83"/>
-      <c r="DV7" s="83"/>
-      <c r="DW7" s="83"/>
-      <c r="DX7" s="83"/>
-      <c r="DY7" s="83"/>
-      <c r="DZ7" s="84"/>
-      <c r="EA7" s="72" t="s">
+      <c r="DF7" s="61"/>
+      <c r="DG7" s="61"/>
+      <c r="DH7" s="61"/>
+      <c r="DI7" s="61"/>
+      <c r="DJ7" s="61"/>
+      <c r="DK7" s="61"/>
+      <c r="DL7" s="61"/>
+      <c r="DM7" s="61"/>
+      <c r="DN7" s="61"/>
+      <c r="DO7" s="61"/>
+      <c r="DP7" s="61"/>
+      <c r="DQ7" s="61"/>
+      <c r="DR7" s="61"/>
+      <c r="DS7" s="61"/>
+      <c r="DT7" s="61"/>
+      <c r="DU7" s="61"/>
+      <c r="DV7" s="61"/>
+      <c r="DW7" s="61"/>
+      <c r="DX7" s="61"/>
+      <c r="DY7" s="61"/>
+      <c r="DZ7" s="62"/>
+      <c r="EA7" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="EB7" s="72"/>
+      <c r="EB7" s="88"/>
       <c r="EC7" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="ED7" s="75" t="s">
+      <c r="ED7" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="EE7" s="66" t="s">
+      <c r="EE7" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="EF7" s="67"/>
+      <c r="EF7" s="83"/>
       <c r="EG7" s="11"/>
     </row>
     <row r="8" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="86"/>
-      <c r="O8" s="86"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="74"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
       <c r="T8" s="15"/>
       <c r="U8" s="4" t="s">
         <v>6</v>
@@ -2254,10 +2257,10 @@
       <c r="AN8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AO8" s="73" t="s">
+      <c r="AO8" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="AP8" s="73" t="s">
+      <c r="AP8" s="64" t="s">
         <v>45</v>
       </c>
       <c r="AQ8" s="4" t="s">
@@ -2320,10 +2323,10 @@
       <c r="BJ8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BK8" s="73" t="s">
+      <c r="BK8" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="BL8" s="73" t="s">
+      <c r="BL8" s="64" t="s">
         <v>45</v>
       </c>
       <c r="BM8" s="4" t="s">
@@ -2386,10 +2389,10 @@
       <c r="CF8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CG8" s="73" t="s">
+      <c r="CG8" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="CH8" s="73" t="s">
+      <c r="CH8" s="64" t="s">
         <v>45</v>
       </c>
       <c r="CI8" s="4" t="s">
@@ -2452,10 +2455,10 @@
       <c r="DB8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="DC8" s="73" t="s">
+      <c r="DC8" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="DD8" s="73" t="s">
+      <c r="DD8" s="64" t="s">
         <v>45</v>
       </c>
       <c r="DE8" s="4" t="s">
@@ -2518,75 +2521,75 @@
       <c r="DX8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="DY8" s="73" t="s">
+      <c r="DY8" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="DZ8" s="73" t="s">
+      <c r="DZ8" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="EA8" s="73" t="s">
+      <c r="EA8" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="EB8" s="73" t="s">
+      <c r="EB8" s="64" t="s">
         <v>52</v>
       </c>
       <c r="EC8" s="53"/>
-      <c r="ED8" s="76"/>
-      <c r="EE8" s="68"/>
-      <c r="EF8" s="69"/>
+      <c r="ED8" s="90"/>
+      <c r="EE8" s="84"/>
+      <c r="EF8" s="85"/>
     </row>
     <row r="9" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="62" t="s">
+      <c r="G9" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="62" t="s">
+      <c r="H9" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="62" t="s">
+      <c r="I9" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="62" t="s">
+      <c r="J9" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="62" t="s">
+      <c r="K9" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="62" t="s">
+      <c r="L9" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="62" t="s">
+      <c r="M9" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="62" t="s">
+      <c r="N9" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="62" t="s">
+      <c r="O9" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="P9" s="62" t="s">
+      <c r="P9" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="74"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="79"/>
       <c r="T9" s="15"/>
       <c r="U9" s="32" t="s">
         <v>46</v>
@@ -2648,8 +2651,8 @@
       <c r="AN9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AO9" s="80"/>
-      <c r="AP9" s="80"/>
+      <c r="AO9" s="65"/>
+      <c r="AP9" s="65"/>
       <c r="AQ9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2710,8 +2713,8 @@
       <c r="BJ9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="BK9" s="80"/>
-      <c r="BL9" s="80"/>
+      <c r="BK9" s="65"/>
+      <c r="BL9" s="65"/>
       <c r="BM9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2772,8 +2775,8 @@
       <c r="CF9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="CG9" s="80"/>
-      <c r="CH9" s="80"/>
+      <c r="CG9" s="65"/>
+      <c r="CH9" s="65"/>
       <c r="CI9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2834,8 +2837,8 @@
       <c r="DB9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="DC9" s="80"/>
-      <c r="DD9" s="80"/>
+      <c r="DC9" s="65"/>
+      <c r="DD9" s="65"/>
       <c r="DE9" s="32" t="s">
         <v>46</v>
       </c>
@@ -2896,35 +2899,35 @@
       <c r="DX9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="DY9" s="80"/>
-      <c r="DZ9" s="80"/>
-      <c r="EA9" s="74"/>
-      <c r="EB9" s="74"/>
+      <c r="DY9" s="65"/>
+      <c r="DZ9" s="65"/>
+      <c r="EA9" s="79"/>
+      <c r="EB9" s="79"/>
       <c r="EC9" s="51"/>
-      <c r="ED9" s="76"/>
-      <c r="EE9" s="68"/>
-      <c r="EF9" s="69"/>
+      <c r="ED9" s="90"/>
+      <c r="EE9" s="84"/>
+      <c r="EF9" s="85"/>
     </row>
     <row r="10" spans="1:137" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="63"/>
-      <c r="S10" s="63"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
       <c r="T10" s="15"/>
       <c r="U10" s="16" t="s">
         <v>49</v>
@@ -2986,8 +2989,8 @@
       <c r="AN10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AO10" s="81"/>
-      <c r="AP10" s="81"/>
+      <c r="AO10" s="66"/>
+      <c r="AP10" s="66"/>
       <c r="AQ10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3048,8 +3051,8 @@
       <c r="BJ10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="BK10" s="81"/>
-      <c r="BL10" s="81"/>
+      <c r="BK10" s="66"/>
+      <c r="BL10" s="66"/>
       <c r="BM10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3110,8 +3113,8 @@
       <c r="CF10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="CG10" s="81"/>
-      <c r="CH10" s="81"/>
+      <c r="CG10" s="66"/>
+      <c r="CH10" s="66"/>
       <c r="CI10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3172,8 +3175,8 @@
       <c r="DB10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="DC10" s="81"/>
-      <c r="DD10" s="81"/>
+      <c r="DC10" s="66"/>
+      <c r="DD10" s="66"/>
       <c r="DE10" s="16" t="s">
         <v>49</v>
       </c>
@@ -3234,14 +3237,14 @@
       <c r="DX10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="DY10" s="81"/>
-      <c r="DZ10" s="81"/>
-      <c r="EA10" s="63"/>
-      <c r="EB10" s="63"/>
+      <c r="DY10" s="66"/>
+      <c r="DZ10" s="66"/>
+      <c r="EA10" s="75"/>
+      <c r="EB10" s="75"/>
       <c r="EC10" s="50"/>
-      <c r="ED10" s="77"/>
-      <c r="EE10" s="70"/>
-      <c r="EF10" s="71"/>
+      <c r="ED10" s="91"/>
+      <c r="EE10" s="86"/>
+      <c r="EF10" s="87"/>
     </row>
     <row r="11" spans="1:137" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -3674,35 +3677,35 @@
       <c r="ED11" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="EE11" s="78" t="s">
+      <c r="EE11" s="92" t="s">
         <v>77</v>
       </c>
-      <c r="EF11" s="79"/>
+      <c r="EF11" s="93"/>
       <c r="EG11" s="35" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:137" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="89"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="90"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="59"/>
       <c r="S12" s="13">
         <f>COUNTIF(statusKategorie,$B$33)</f>
         <v>0</v>
@@ -4162,26 +4165,26 @@
       <c r="EF12" s="40"/>
     </row>
     <row r="13" spans="1:137" x14ac:dyDescent="0.25">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="90"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="59"/>
       <c r="S13" s="13">
         <f>COUNTIF(statusKategorie,$B$32)</f>
         <v>0</v>
@@ -4641,26 +4644,26 @@
       <c r="EF13" s="44"/>
     </row>
     <row r="14" spans="1:137" x14ac:dyDescent="0.25">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="90"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="59"/>
       <c r="S14" s="13">
         <f>COUNTIF(statusKategorie,$B$31)</f>
         <v>0</v>
@@ -5121,10 +5124,10 @@
     </row>
     <row r="15" spans="1:137" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>2</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>4</v>
@@ -5493,39 +5496,41 @@
       <c r="DZ15" s="27"/>
       <c r="EA15" s="30"/>
       <c r="EB15" s="37"/>
-      <c r="EC15" s="37"/>
+      <c r="EC15" s="56" t="s">
+        <v>93</v>
+      </c>
       <c r="ED15" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="EE15" s="64" t="s">
+      <c r="EE15" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="EF15" s="65"/>
+      <c r="EF15" s="81"/>
       <c r="EG15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:137" x14ac:dyDescent="0.25">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="92"/>
-      <c r="O16" s="92"/>
-      <c r="P16" s="92"/>
-      <c r="Q16" s="92"/>
-      <c r="R16" s="92"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="67"/>
       <c r="S16" s="13">
         <f>COUNTIF(freigegebenKategorie,$B$34)</f>
         <v>0</v>
@@ -6103,11 +6108,11 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="89"/>
-      <c r="C36" s="90"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="59"/>
       <c r="D36" s="49"/>
       <c r="E36" s="49"/>
       <c r="F36" s="49"/>
@@ -6116,10 +6121,10 @@
       <c r="A37" s="22">
         <v>1</v>
       </c>
-      <c r="B37" s="91" t="s">
+      <c r="B37" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="91"/>
+      <c r="C37" s="63"/>
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
@@ -6138,10 +6143,10 @@
       <c r="A38" s="22">
         <v>2</v>
       </c>
-      <c r="B38" s="91" t="s">
+      <c r="B38" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="91"/>
+      <c r="C38" s="63"/>
       <c r="D38" s="34"/>
       <c r="E38" s="34"/>
       <c r="F38" s="34"/>
@@ -6160,10 +6165,10 @@
       <c r="A39" s="22">
         <v>3</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="91"/>
+      <c r="C39" s="63"/>
       <c r="D39" s="34"/>
       <c r="E39" s="34"/>
       <c r="F39" s="34"/>
@@ -6180,6 +6185,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="D7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="EE15:EF15"/>
+    <mergeCell ref="EE7:EF10"/>
+    <mergeCell ref="EA7:EB7"/>
+    <mergeCell ref="EA8:EA10"/>
+    <mergeCell ref="EB8:EB10"/>
+    <mergeCell ref="ED7:ED10"/>
+    <mergeCell ref="EE11:EF11"/>
+    <mergeCell ref="DC8:DC10"/>
+    <mergeCell ref="DD8:DD10"/>
+    <mergeCell ref="DY8:DY10"/>
+    <mergeCell ref="DZ8:DZ10"/>
+    <mergeCell ref="DE7:DZ7"/>
+    <mergeCell ref="CI7:DD7"/>
+    <mergeCell ref="G7:K8"/>
+    <mergeCell ref="L7:P8"/>
+    <mergeCell ref="S7:S10"/>
+    <mergeCell ref="Q7:Q10"/>
+    <mergeCell ref="R7:R10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="A13:R13"/>
+    <mergeCell ref="A14:R14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="AQ7:BL7"/>
     <mergeCell ref="BM7:CH7"/>
@@ -6196,43 +6238,6 @@
     <mergeCell ref="A16:R16"/>
     <mergeCell ref="A12:R12"/>
     <mergeCell ref="A7:C8"/>
-    <mergeCell ref="A13:R13"/>
-    <mergeCell ref="A14:R14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L7:P8"/>
-    <mergeCell ref="S7:S10"/>
-    <mergeCell ref="Q7:Q10"/>
-    <mergeCell ref="R7:R10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="D7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="EE15:EF15"/>
-    <mergeCell ref="EE7:EF10"/>
-    <mergeCell ref="EA7:EB7"/>
-    <mergeCell ref="EA8:EA10"/>
-    <mergeCell ref="EB8:EB10"/>
-    <mergeCell ref="ED7:ED10"/>
-    <mergeCell ref="EE11:EF11"/>
-    <mergeCell ref="DC8:DC10"/>
-    <mergeCell ref="DD8:DD10"/>
-    <mergeCell ref="DY8:DY10"/>
-    <mergeCell ref="DZ8:DZ10"/>
-    <mergeCell ref="DE7:DZ7"/>
-    <mergeCell ref="CI7:DD7"/>
-    <mergeCell ref="G7:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>